<commit_message>
Alright so we've actually got a program now that can parse Excel and populate a list with classes. Pretty cool.
</commit_message>
<xml_diff>
--- a/family-tree-data.xlsx
+++ b/family-tree-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASHil\PycharmProjects\Family-Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5273CEF8-B473-4B18-BAA6-6E1BF77BF39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68343D7-60F6-4A77-9D78-269AFE980E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -734,7 +734,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -839,10 +839,14 @@
       <c r="D4" s="2">
         <v>14</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2">
+        <v>10</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="H4" s="2">
+        <v>21</v>
+      </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -861,7 +865,9 @@
       <c r="D5" s="2">
         <v>27</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2">
+        <v>21</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -1273,10 +1279,14 @@
       <c r="D23" s="2">
         <v>21</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2">
+        <v>14</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="H23" s="2">
+        <v>27</v>
+      </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -1387,12 +1397,20 @@
       <c r="D28" s="2">
         <v>10</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="2">
+        <v>7</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
+      <c r="H28" s="2">
+        <v>14</v>
+      </c>
+      <c r="I28" s="2">
+        <v>15</v>
+      </c>
+      <c r="J28" s="2">
+        <v>16</v>
+      </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>

</xml_diff>

<commit_message>
I guess I modified something here.
</commit_message>
<xml_diff>
--- a/family-tree-data.xlsx
+++ b/family-tree-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASHil\PycharmProjects\Family-Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68343D7-60F6-4A77-9D78-269AFE980E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3183D1FE-25E4-465A-BF65-A9C5F5E09A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
   <si>
     <t>Class Year</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>Currin</t>
+  </si>
+  <si>
+    <t>Carpen</t>
   </si>
 </sst>
 </file>
@@ -327,15 +330,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -355,21 +355,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="00000"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -418,16 +403,31 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="medium">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color indexed="64"/>
-        </top>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -444,24 +444,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{11C3A996-264D-49A5-B58C-4848FCDD6F03}" name="Table2" displayName="Table2" ref="A1:L151" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="14" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{11C3A996-264D-49A5-B58C-4848FCDD6F03}" name="Table2" displayName="Table2" ref="A1:L151" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
   <autoFilter ref="A1:L151" xr:uid="{11C3A996-264D-49A5-B58C-4848FCDD6F03}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L151">
     <sortCondition ref="B1:B151"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{5EDD3C60-3C2C-40F1-97A9-01DC19C6B82F}" name="First Name" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{EF0889F4-AB8A-4E41-9EE4-5A2BF0BFD794}" name="Last Name" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{86E4CF69-FB69-4B21-9BFA-43FDA0099215}" name="Class Year" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{8F0F6FA8-92FF-40FE-A11F-6C2D1597C063}" name="Parse ID" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{61B9159E-610A-4A8F-9F0C-DEABBF5DB327}" name="Parent 1" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{199D1D06-A3D8-46C8-A02F-9AAF042D9958}" name="Parent 2" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{63E6E218-11FC-4D75-B8E3-C44083B6218B}" name="Parent 3" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{CA4B4E19-AB25-4B2D-9E06-CD50BB63F1BD}" name="Child 1" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{F4158ED3-1229-4E63-A0E7-5AD8267EBDC7}" name="Child 2" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{A731EFD4-7198-4860-8DC3-7C61CF8B688C}" name="Child 3" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{095C504D-C521-47E5-85CA-8FB45B7FF673}" name="Child 4" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{8A459A0C-705E-4C06-B161-AC9856E8D667}" name="Child 5" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{5EDD3C60-3C2C-40F1-97A9-01DC19C6B82F}" name="First Name" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{EF0889F4-AB8A-4E41-9EE4-5A2BF0BFD794}" name="Last Name" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{86E4CF69-FB69-4B21-9BFA-43FDA0099215}" name="Class Year" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{8F0F6FA8-92FF-40FE-A11F-6C2D1597C063}" name="Parse ID" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{61B9159E-610A-4A8F-9F0C-DEABBF5DB327}" name="Parent 1" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{199D1D06-A3D8-46C8-A02F-9AAF042D9958}" name="Parent 2" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{63E6E218-11FC-4D75-B8E3-C44083B6218B}" name="Parent 3" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{CA4B4E19-AB25-4B2D-9E06-CD50BB63F1BD}" name="Child 1" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{F4158ED3-1229-4E63-A0E7-5AD8267EBDC7}" name="Child 2" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{A731EFD4-7198-4860-8DC3-7C61CF8B688C}" name="Child 3" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{095C504D-C521-47E5-85CA-8FB45B7FF673}" name="Child 4" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{8A459A0C-705E-4C06-B161-AC9856E8D667}" name="Child 5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -733,52 +733,52 @@
   <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" style="5" customWidth="1"/>
     <col min="4" max="11" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -789,18 +789,26 @@
       <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>2017</v>
       </c>
       <c r="D2" s="2">
         <v>11</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2">
+        <v>8</v>
+      </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="H2" s="2">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2">
+        <v>19</v>
+      </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
@@ -811,13 +819,15 @@
       <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>9999</v>
       </c>
       <c r="D3" s="2">
         <v>25</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2">
+        <v>19</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -833,7 +843,7 @@
       <c r="B4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>2016</v>
       </c>
       <c r="D4" s="2">
@@ -859,7 +869,7 @@
       <c r="B5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>2020</v>
       </c>
       <c r="D5" s="2">
@@ -883,13 +893,15 @@
       <c r="B6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>2021</v>
       </c>
       <c r="D6" s="2">
         <v>23</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2">
+        <v>17</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -905,16 +917,20 @@
       <c r="B7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>2020</v>
       </c>
       <c r="D7" s="2">
         <v>18</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2">
+        <v>11</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>24</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -927,16 +943,20 @@
       <c r="B8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>2022</v>
       </c>
       <c r="D8" s="2">
         <v>24</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2">
+        <v>18</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2">
+        <v>28</v>
+      </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -944,18 +964,20 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="4">
-        <v>2025</v>
+        <v>64</v>
+      </c>
+      <c r="C9" s="3">
+        <v>9999</v>
       </c>
       <c r="D9" s="2">
-        <v>30</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="E9" s="2">
+        <v>20</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -966,79 +988,81 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="C10" s="3">
-        <v>2008</v>
+        <v>2025</v>
       </c>
       <c r="D10" s="2">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E10" s="2">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2">
-        <v>3</v>
-      </c>
-      <c r="I10" s="2">
-        <v>4</v>
-      </c>
-      <c r="J10" s="2">
-        <v>5</v>
-      </c>
-      <c r="K10" s="2">
-        <v>6</v>
-      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="3">
-        <v>9999</v>
+        <v>15</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2008</v>
       </c>
       <c r="D11" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2">
-        <v>7</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="I11" s="2">
+        <v>4</v>
+      </c>
+      <c r="J11" s="2">
+        <v>5</v>
+      </c>
+      <c r="K11" s="2">
+        <v>6</v>
+      </c>
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="4">
-        <v>2008</v>
+        <v>18</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9999</v>
       </c>
       <c r="D12" s="2">
-        <v>17</v>
-      </c>
-      <c r="E12" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2">
+        <v>7</v>
+      </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1046,40 +1070,48 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="4">
-        <v>2024</v>
+        <v>41</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2008</v>
       </c>
       <c r="D13" s="2">
-        <v>29</v>
-      </c>
-      <c r="E13" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="E13" s="2">
+        <v>11</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="H13" s="2">
+        <v>23</v>
+      </c>
+      <c r="I13" s="2">
+        <v>22</v>
+      </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="4">
-        <v>9999</v>
+        <v>62</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2024</v>
       </c>
       <c r="D14" s="2">
-        <v>13</v>
-      </c>
-      <c r="E14" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="E14" s="2">
+        <v>26</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1090,18 +1122,20 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="4">
-        <v>2023</v>
+        <v>35</v>
+      </c>
+      <c r="C15" s="3">
+        <v>9999</v>
       </c>
       <c r="D15" s="2">
-        <v>26</v>
-      </c>
-      <c r="E15" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="E15" s="2">
+        <v>9</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1112,21 +1146,25 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="4">
+        <v>56</v>
+      </c>
+      <c r="C16" s="3">
         <v>2023</v>
       </c>
       <c r="D16" s="2">
-        <v>28</v>
-      </c>
-      <c r="E16" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="E16" s="2">
+        <v>19</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2">
+        <v>29</v>
+      </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1134,21 +1172,25 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="4">
-        <v>2020</v>
+        <v>60</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2023</v>
       </c>
       <c r="D17" s="2">
-        <v>19</v>
-      </c>
-      <c r="E17" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="E17" s="2">
+        <v>24</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2">
+        <v>30</v>
+      </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1156,42 +1198,48 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="5">
-        <v>9999</v>
+        <v>44</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2020</v>
       </c>
       <c r="D18" s="2">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E18" s="2">
-        <v>99999</v>
+        <v>11</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="H18" s="2">
+        <v>25</v>
+      </c>
+      <c r="I18" s="2">
+        <v>26</v>
+      </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="3">
+        <v>13</v>
+      </c>
+      <c r="C19" s="4">
         <v>9999</v>
       </c>
       <c r="D19" s="2">
-        <v>4</v>
-      </c>
-      <c r="E19" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>99999</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1202,21 +1250,25 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="4">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1">
         <v>9999</v>
       </c>
       <c r="D20" s="2">
-        <v>12</v>
-      </c>
-      <c r="E20" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="E20" s="2">
+        <v>2</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="H20" s="2">
+        <v>8</v>
+      </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -1227,18 +1279,22 @@
         <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="4">
+        <v>34</v>
+      </c>
+      <c r="C21" s="3">
         <v>9999</v>
       </c>
       <c r="D21" s="2">
-        <v>20</v>
-      </c>
-      <c r="E21" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="E21" s="2">
+        <v>9</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="H21" s="2">
+        <v>20</v>
+      </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -1249,15 +1305,17 @@
         <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="4">
+        <v>45</v>
+      </c>
+      <c r="C22" s="3">
         <v>9999</v>
       </c>
       <c r="D22" s="2">
-        <v>9</v>
-      </c>
-      <c r="E22" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="E22" s="2">
+        <v>12</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1268,50 +1326,52 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="4">
-        <v>2017</v>
+        <v>29</v>
+      </c>
+      <c r="C23" s="3">
+        <v>9999</v>
       </c>
       <c r="D23" s="2">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E23" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2">
-        <v>27</v>
-      </c>
-      <c r="I23" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="I23" s="2">
+        <v>13</v>
+      </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C24" s="3">
-        <v>2013</v>
+        <v>2017</v>
       </c>
       <c r="D24" s="2">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E24" s="2">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1320,21 +1380,25 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="3">
-        <v>9999</v>
+        <v>26</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2013</v>
       </c>
       <c r="D25" s="2">
-        <v>6</v>
-      </c>
-      <c r="E25" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="E25" s="2">
+        <v>3</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="H25" s="2">
+        <v>10</v>
+      </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -1342,18 +1406,20 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="3">
+        <v>24</v>
+      </c>
+      <c r="C26" s="1">
         <v>9999</v>
       </c>
       <c r="D26" s="2">
-        <v>5</v>
-      </c>
-      <c r="E26" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -1364,18 +1430,20 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="4">
-        <v>2020</v>
+        <v>22</v>
+      </c>
+      <c r="C27" s="1">
+        <v>9999</v>
       </c>
       <c r="D27" s="2">
-        <v>22</v>
-      </c>
-      <c r="E27" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1386,70 +1454,74 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="4">
-        <v>2014</v>
+        <v>49</v>
+      </c>
+      <c r="C28" s="3">
+        <v>2020</v>
       </c>
       <c r="D28" s="2">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E28" s="2">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="2">
-        <v>14</v>
-      </c>
-      <c r="I28" s="2">
-        <v>15</v>
-      </c>
-      <c r="J28" s="2">
-        <v>16</v>
-      </c>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="4">
-        <v>9999</v>
+      <c r="C29" s="3">
+        <v>2014</v>
       </c>
       <c r="D29" s="2">
-        <v>15</v>
-      </c>
-      <c r="E29" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="E29" s="2">
+        <v>7</v>
+      </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
+      <c r="H29" s="2">
+        <v>14</v>
+      </c>
+      <c r="I29" s="2">
+        <v>15</v>
+      </c>
+      <c r="J29" s="2">
+        <v>16</v>
+      </c>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="3">
         <v>9999</v>
       </c>
       <c r="D30" s="2">
-        <v>16</v>
-      </c>
-      <c r="E30" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="E30" s="2">
+        <v>10</v>
+      </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -1460,18 +1532,20 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="4">
+        <v>31</v>
+      </c>
+      <c r="C31" s="3">
         <v>9999</v>
       </c>
       <c r="D31" s="2">
-        <v>8</v>
-      </c>
-      <c r="E31" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="E31" s="2">
+        <v>10</v>
+      </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -1481,16 +1555,26 @@
       <c r="L31" s="2"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="4"/>
+      <c r="A32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="3">
+        <v>9999</v>
+      </c>
       <c r="D32" s="2">
-        <v>31</v>
-      </c>
-      <c r="E32" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="E32" s="2">
+        <v>4</v>
+      </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="H32" s="2">
+        <v>11</v>
+      </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
@@ -1499,10 +1583,8 @@
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="2">
-        <v>32</v>
-      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -1515,10 +1597,8 @@
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="2">
-        <v>33</v>
-      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -1531,10 +1611,8 @@
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="2">
-        <v>34</v>
-      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -1547,10 +1625,8 @@
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="2">
-        <v>35</v>
-      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -1563,10 +1639,8 @@
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="2">
-        <v>36</v>
-      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -1579,10 +1653,8 @@
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="2">
-        <v>37</v>
-      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
@@ -1595,10 +1667,8 @@
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="2">
-        <v>38</v>
-      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -1611,10 +1681,8 @@
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="2">
-        <v>39</v>
-      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -1627,10 +1695,8 @@
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="2">
-        <v>40</v>
-      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -1643,10 +1709,8 @@
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="2">
-        <v>41</v>
-      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -1659,10 +1723,8 @@
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="2">
-        <v>42</v>
-      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -1675,10 +1737,8 @@
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="2">
-        <v>43</v>
-      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -1691,10 +1751,8 @@
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="2">
-        <v>44</v>
-      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -1707,10 +1765,8 @@
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="2">
-        <v>45</v>
-      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -1723,10 +1779,8 @@
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="2">
-        <v>46</v>
-      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -1739,10 +1793,8 @@
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="2">
-        <v>47</v>
-      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
@@ -1755,10 +1807,8 @@
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="2">
-        <v>48</v>
-      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
@@ -1771,10 +1821,8 @@
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="2">
-        <v>49</v>
-      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -1787,10 +1835,8 @@
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="2">
-        <v>50</v>
-      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
@@ -1803,10 +1849,8 @@
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="2">
-        <v>51</v>
-      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -1819,10 +1863,8 @@
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="2">
-        <v>52</v>
-      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
@@ -1835,10 +1877,8 @@
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="2">
-        <v>53</v>
-      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -1851,10 +1891,8 @@
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="2">
-        <v>54</v>
-      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
@@ -1867,10 +1905,8 @@
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="2">
-        <v>55</v>
-      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
@@ -1883,10 +1919,8 @@
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="2">
-        <v>56</v>
-      </c>
+      <c r="C57" s="3"/>
+      <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
@@ -1899,10 +1933,8 @@
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="2">
-        <v>57</v>
-      </c>
+      <c r="C58" s="3"/>
+      <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
@@ -1915,10 +1947,8 @@
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="2">
-        <v>58</v>
-      </c>
+      <c r="C59" s="3"/>
+      <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
@@ -1931,10 +1961,8 @@
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="2">
-        <v>59</v>
-      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
@@ -1947,10 +1975,8 @@
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="2">
-        <v>60</v>
-      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
@@ -1963,10 +1989,8 @@
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="2">
-        <v>61</v>
-      </c>
+      <c r="C62" s="3"/>
+      <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
@@ -1979,10 +2003,8 @@
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="2">
-        <v>62</v>
-      </c>
+      <c r="C63" s="3"/>
+      <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
@@ -1995,10 +2017,8 @@
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="2">
-        <v>63</v>
-      </c>
+      <c r="C64" s="3"/>
+      <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -2011,10 +2031,8 @@
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="2">
-        <v>64</v>
-      </c>
+      <c r="C65" s="3"/>
+      <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
@@ -2027,10 +2045,8 @@
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="2">
-        <v>65</v>
-      </c>
+      <c r="C66" s="3"/>
+      <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
@@ -2043,10 +2059,8 @@
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="2">
-        <v>66</v>
-      </c>
+      <c r="C67" s="3"/>
+      <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -2059,10 +2073,8 @@
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="2">
-        <v>67</v>
-      </c>
+      <c r="C68" s="3"/>
+      <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
@@ -2075,10 +2087,8 @@
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="2">
-        <v>68</v>
-      </c>
+      <c r="C69" s="3"/>
+      <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
@@ -2091,10 +2101,8 @@
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="2">
-        <v>69</v>
-      </c>
+      <c r="C70" s="3"/>
+      <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
@@ -2107,10 +2115,8 @@
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="2">
-        <v>70</v>
-      </c>
+      <c r="C71" s="3"/>
+      <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
@@ -2123,10 +2129,8 @@
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="2">
-        <v>71</v>
-      </c>
+      <c r="C72" s="3"/>
+      <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
@@ -2139,10 +2143,8 @@
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="2">
-        <v>72</v>
-      </c>
+      <c r="C73" s="3"/>
+      <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
@@ -2155,10 +2157,8 @@
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="2">
-        <v>73</v>
-      </c>
+      <c r="C74" s="3"/>
+      <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
@@ -2171,10 +2171,8 @@
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="2">
-        <v>74</v>
-      </c>
+      <c r="C75" s="3"/>
+      <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
@@ -2187,10 +2185,8 @@
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
-      <c r="C76" s="4"/>
-      <c r="D76" s="2">
-        <v>75</v>
-      </c>
+      <c r="C76" s="3"/>
+      <c r="D76" s="2"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
@@ -2203,10 +2199,8 @@
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
-      <c r="C77" s="4"/>
-      <c r="D77" s="2">
-        <v>76</v>
-      </c>
+      <c r="C77" s="3"/>
+      <c r="D77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
@@ -2219,10 +2213,8 @@
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
-      <c r="C78" s="4"/>
-      <c r="D78" s="2">
-        <v>77</v>
-      </c>
+      <c r="C78" s="3"/>
+      <c r="D78" s="2"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
@@ -2235,10 +2227,8 @@
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
-      <c r="C79" s="4"/>
-      <c r="D79" s="2">
-        <v>78</v>
-      </c>
+      <c r="C79" s="3"/>
+      <c r="D79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
@@ -2251,10 +2241,8 @@
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
-      <c r="C80" s="4"/>
-      <c r="D80" s="2">
-        <v>79</v>
-      </c>
+      <c r="C80" s="3"/>
+      <c r="D80" s="2"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
@@ -2267,10 +2255,8 @@
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="2">
-        <v>80</v>
-      </c>
+      <c r="C81" s="3"/>
+      <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
@@ -2283,10 +2269,8 @@
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
-      <c r="C82" s="4"/>
-      <c r="D82" s="2">
-        <v>81</v>
-      </c>
+      <c r="C82" s="3"/>
+      <c r="D82" s="2"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
@@ -2299,10 +2283,8 @@
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
-      <c r="C83" s="4"/>
-      <c r="D83" s="2">
-        <v>82</v>
-      </c>
+      <c r="C83" s="3"/>
+      <c r="D83" s="2"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
@@ -2315,10 +2297,8 @@
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
-      <c r="C84" s="4"/>
-      <c r="D84" s="2">
-        <v>83</v>
-      </c>
+      <c r="C84" s="3"/>
+      <c r="D84" s="2"/>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
@@ -2331,10 +2311,8 @@
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="2">
-        <v>84</v>
-      </c>
+      <c r="C85" s="3"/>
+      <c r="D85" s="2"/>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
@@ -2347,10 +2325,8 @@
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="2">
-        <v>85</v>
-      </c>
+      <c r="C86" s="3"/>
+      <c r="D86" s="2"/>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
@@ -2363,10 +2339,8 @@
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="2">
-        <v>86</v>
-      </c>
+      <c r="C87" s="3"/>
+      <c r="D87" s="2"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
@@ -2379,10 +2353,8 @@
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="2">
-        <v>87</v>
-      </c>
+      <c r="C88" s="3"/>
+      <c r="D88" s="2"/>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
@@ -2395,10 +2367,8 @@
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
-      <c r="C89" s="4"/>
-      <c r="D89" s="2">
-        <v>88</v>
-      </c>
+      <c r="C89" s="3"/>
+      <c r="D89" s="2"/>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
@@ -2411,10 +2381,8 @@
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
-      <c r="C90" s="4"/>
-      <c r="D90" s="2">
-        <v>89</v>
-      </c>
+      <c r="C90" s="3"/>
+      <c r="D90" s="2"/>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
@@ -2427,10 +2395,8 @@
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
-      <c r="C91" s="4"/>
-      <c r="D91" s="2">
-        <v>90</v>
-      </c>
+      <c r="C91" s="3"/>
+      <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
@@ -2443,10 +2409,8 @@
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
-      <c r="C92" s="4"/>
-      <c r="D92" s="2">
-        <v>91</v>
-      </c>
+      <c r="C92" s="3"/>
+      <c r="D92" s="2"/>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
@@ -2459,10 +2423,8 @@
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
-      <c r="C93" s="4"/>
-      <c r="D93" s="2">
-        <v>92</v>
-      </c>
+      <c r="C93" s="3"/>
+      <c r="D93" s="2"/>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
@@ -2475,10 +2437,8 @@
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
-      <c r="C94" s="4"/>
-      <c r="D94" s="2">
-        <v>93</v>
-      </c>
+      <c r="C94" s="3"/>
+      <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
@@ -2491,10 +2451,8 @@
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
-      <c r="C95" s="4"/>
-      <c r="D95" s="2">
-        <v>94</v>
-      </c>
+      <c r="C95" s="3"/>
+      <c r="D95" s="2"/>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
@@ -2507,10 +2465,8 @@
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
-      <c r="C96" s="4"/>
-      <c r="D96" s="2">
-        <v>95</v>
-      </c>
+      <c r="C96" s="3"/>
+      <c r="D96" s="2"/>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
@@ -2523,10 +2479,8 @@
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
-      <c r="C97" s="4"/>
-      <c r="D97" s="2">
-        <v>96</v>
-      </c>
+      <c r="C97" s="3"/>
+      <c r="D97" s="2"/>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
@@ -2539,10 +2493,8 @@
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
-      <c r="C98" s="4"/>
-      <c r="D98" s="2">
-        <v>97</v>
-      </c>
+      <c r="C98" s="3"/>
+      <c r="D98" s="2"/>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
@@ -2555,10 +2507,8 @@
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
-      <c r="C99" s="4"/>
-      <c r="D99" s="2">
-        <v>98</v>
-      </c>
+      <c r="C99" s="3"/>
+      <c r="D99" s="2"/>
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
@@ -2571,10 +2521,8 @@
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
-      <c r="C100" s="4"/>
-      <c r="D100" s="2">
-        <v>99</v>
-      </c>
+      <c r="C100" s="3"/>
+      <c r="D100" s="2"/>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
@@ -2587,10 +2535,8 @@
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
-      <c r="C101" s="4"/>
-      <c r="D101" s="2">
-        <v>100</v>
-      </c>
+      <c r="C101" s="3"/>
+      <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
@@ -2603,10 +2549,8 @@
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
-      <c r="C102" s="4"/>
-      <c r="D102" s="2">
-        <v>101</v>
-      </c>
+      <c r="C102" s="3"/>
+      <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
@@ -2619,10 +2563,8 @@
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
-      <c r="C103" s="4"/>
-      <c r="D103" s="2">
-        <v>102</v>
-      </c>
+      <c r="C103" s="3"/>
+      <c r="D103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
@@ -2635,10 +2577,8 @@
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
-      <c r="C104" s="4"/>
-      <c r="D104" s="2">
-        <v>103</v>
-      </c>
+      <c r="C104" s="3"/>
+      <c r="D104" s="2"/>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
@@ -2651,10 +2591,8 @@
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
-      <c r="C105" s="4"/>
-      <c r="D105" s="2">
-        <v>104</v>
-      </c>
+      <c r="C105" s="3"/>
+      <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
@@ -2667,10 +2605,8 @@
     <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
-      <c r="C106" s="4"/>
-      <c r="D106" s="2">
-        <v>105</v>
-      </c>
+      <c r="C106" s="3"/>
+      <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
@@ -2683,10 +2619,8 @@
     <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
-      <c r="C107" s="4"/>
-      <c r="D107" s="2">
-        <v>106</v>
-      </c>
+      <c r="C107" s="3"/>
+      <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
       <c r="G107" s="2"/>
@@ -2699,10 +2633,8 @@
     <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
-      <c r="C108" s="4"/>
-      <c r="D108" s="2">
-        <v>107</v>
-      </c>
+      <c r="C108" s="3"/>
+      <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
@@ -2715,10 +2647,8 @@
     <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
-      <c r="C109" s="4"/>
-      <c r="D109" s="2">
-        <v>108</v>
-      </c>
+      <c r="C109" s="3"/>
+      <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
@@ -2731,10 +2661,8 @@
     <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
-      <c r="C110" s="4"/>
-      <c r="D110" s="2">
-        <v>109</v>
-      </c>
+      <c r="C110" s="3"/>
+      <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
@@ -2747,10 +2675,8 @@
     <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
-      <c r="C111" s="4"/>
-      <c r="D111" s="2">
-        <v>110</v>
-      </c>
+      <c r="C111" s="3"/>
+      <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
       <c r="G111" s="2"/>
@@ -2763,10 +2689,8 @@
     <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
-      <c r="C112" s="4"/>
-      <c r="D112" s="2">
-        <v>111</v>
-      </c>
+      <c r="C112" s="3"/>
+      <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
       <c r="G112" s="2"/>
@@ -2779,10 +2703,8 @@
     <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
-      <c r="C113" s="4"/>
-      <c r="D113" s="2">
-        <v>112</v>
-      </c>
+      <c r="C113" s="3"/>
+      <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
@@ -2795,10 +2717,8 @@
     <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
-      <c r="C114" s="4"/>
-      <c r="D114" s="2">
-        <v>113</v>
-      </c>
+      <c r="C114" s="3"/>
+      <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
@@ -2811,10 +2731,8 @@
     <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
-      <c r="C115" s="4"/>
-      <c r="D115" s="2">
-        <v>114</v>
-      </c>
+      <c r="C115" s="3"/>
+      <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
       <c r="G115" s="2"/>
@@ -2827,10 +2745,8 @@
     <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
-      <c r="C116" s="4"/>
-      <c r="D116" s="2">
-        <v>115</v>
-      </c>
+      <c r="C116" s="3"/>
+      <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
@@ -2843,10 +2759,8 @@
     <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
-      <c r="C117" s="4"/>
-      <c r="D117" s="2">
-        <v>116</v>
-      </c>
+      <c r="C117" s="3"/>
+      <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
       <c r="G117" s="2"/>
@@ -2859,10 +2773,8 @@
     <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
-      <c r="C118" s="4"/>
-      <c r="D118" s="2">
-        <v>117</v>
-      </c>
+      <c r="C118" s="3"/>
+      <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
       <c r="G118" s="2"/>
@@ -2875,10 +2787,8 @@
     <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
-      <c r="C119" s="4"/>
-      <c r="D119" s="2">
-        <v>118</v>
-      </c>
+      <c r="C119" s="3"/>
+      <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
       <c r="G119" s="2"/>
@@ -2891,10 +2801,8 @@
     <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
-      <c r="C120" s="4"/>
-      <c r="D120" s="2">
-        <v>119</v>
-      </c>
+      <c r="C120" s="3"/>
+      <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="2"/>
@@ -2907,10 +2815,8 @@
     <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
-      <c r="C121" s="4"/>
-      <c r="D121" s="2">
-        <v>120</v>
-      </c>
+      <c r="C121" s="3"/>
+      <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
       <c r="G121" s="2"/>
@@ -2923,10 +2829,8 @@
     <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
-      <c r="C122" s="4"/>
-      <c r="D122" s="2">
-        <v>121</v>
-      </c>
+      <c r="C122" s="3"/>
+      <c r="D122" s="2"/>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
       <c r="G122" s="2"/>
@@ -2939,10 +2843,8 @@
     <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
-      <c r="C123" s="4"/>
-      <c r="D123" s="2">
-        <v>122</v>
-      </c>
+      <c r="C123" s="3"/>
+      <c r="D123" s="2"/>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
       <c r="G123" s="2"/>
@@ -2955,10 +2857,8 @@
     <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
-      <c r="C124" s="4"/>
-      <c r="D124" s="2">
-        <v>123</v>
-      </c>
+      <c r="C124" s="3"/>
+      <c r="D124" s="2"/>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
       <c r="G124" s="2"/>
@@ -2971,10 +2871,8 @@
     <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
-      <c r="C125" s="4"/>
-      <c r="D125" s="2">
-        <v>124</v>
-      </c>
+      <c r="C125" s="3"/>
+      <c r="D125" s="2"/>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
       <c r="G125" s="2"/>
@@ -2987,10 +2885,8 @@
     <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
-      <c r="C126" s="4"/>
-      <c r="D126" s="2">
-        <v>125</v>
-      </c>
+      <c r="C126" s="3"/>
+      <c r="D126" s="2"/>
       <c r="E126" s="2"/>
       <c r="F126" s="2"/>
       <c r="G126" s="2"/>
@@ -3003,10 +2899,8 @@
     <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
-      <c r="C127" s="4"/>
-      <c r="D127" s="2">
-        <v>126</v>
-      </c>
+      <c r="C127" s="3"/>
+      <c r="D127" s="2"/>
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
       <c r="G127" s="2"/>
@@ -3019,10 +2913,8 @@
     <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
-      <c r="C128" s="4"/>
-      <c r="D128" s="2">
-        <v>127</v>
-      </c>
+      <c r="C128" s="3"/>
+      <c r="D128" s="2"/>
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
       <c r="G128" s="2"/>
@@ -3035,10 +2927,8 @@
     <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
-      <c r="C129" s="4"/>
-      <c r="D129" s="2">
-        <v>128</v>
-      </c>
+      <c r="C129" s="3"/>
+      <c r="D129" s="2"/>
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
       <c r="G129" s="2"/>
@@ -3051,10 +2941,8 @@
     <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
-      <c r="C130" s="4"/>
-      <c r="D130" s="2">
-        <v>129</v>
-      </c>
+      <c r="C130" s="3"/>
+      <c r="D130" s="2"/>
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>
       <c r="G130" s="2"/>
@@ -3067,10 +2955,8 @@
     <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
-      <c r="C131" s="4"/>
-      <c r="D131" s="2">
-        <v>130</v>
-      </c>
+      <c r="C131" s="3"/>
+      <c r="D131" s="2"/>
       <c r="E131" s="2"/>
       <c r="F131" s="2"/>
       <c r="G131" s="2"/>
@@ -3083,10 +2969,8 @@
     <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
-      <c r="C132" s="4"/>
-      <c r="D132" s="2">
-        <v>131</v>
-      </c>
+      <c r="C132" s="3"/>
+      <c r="D132" s="2"/>
       <c r="E132" s="2"/>
       <c r="F132" s="2"/>
       <c r="G132" s="2"/>
@@ -3099,10 +2983,8 @@
     <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
-      <c r="C133" s="4"/>
-      <c r="D133" s="2">
-        <v>132</v>
-      </c>
+      <c r="C133" s="3"/>
+      <c r="D133" s="2"/>
       <c r="E133" s="2"/>
       <c r="F133" s="2"/>
       <c r="G133" s="2"/>
@@ -3115,10 +2997,8 @@
     <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
-      <c r="C134" s="4"/>
-      <c r="D134" s="2">
-        <v>133</v>
-      </c>
+      <c r="C134" s="3"/>
+      <c r="D134" s="2"/>
       <c r="E134" s="2"/>
       <c r="F134" s="2"/>
       <c r="G134" s="2"/>
@@ -3131,10 +3011,8 @@
     <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
-      <c r="C135" s="4"/>
-      <c r="D135" s="2">
-        <v>134</v>
-      </c>
+      <c r="C135" s="3"/>
+      <c r="D135" s="2"/>
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
@@ -3147,10 +3025,8 @@
     <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
-      <c r="C136" s="4"/>
-      <c r="D136" s="2">
-        <v>135</v>
-      </c>
+      <c r="C136" s="3"/>
+      <c r="D136" s="2"/>
       <c r="E136" s="2"/>
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
@@ -3163,10 +3039,8 @@
     <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
-      <c r="C137" s="4"/>
-      <c r="D137" s="2">
-        <v>136</v>
-      </c>
+      <c r="C137" s="3"/>
+      <c r="D137" s="2"/>
       <c r="E137" s="2"/>
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
@@ -3179,10 +3053,8 @@
     <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
-      <c r="C138" s="4"/>
-      <c r="D138" s="2">
-        <v>137</v>
-      </c>
+      <c r="C138" s="3"/>
+      <c r="D138" s="2"/>
       <c r="E138" s="2"/>
       <c r="F138" s="2"/>
       <c r="G138" s="2"/>
@@ -3195,10 +3067,8 @@
     <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
-      <c r="C139" s="4"/>
-      <c r="D139" s="2">
-        <v>138</v>
-      </c>
+      <c r="C139" s="3"/>
+      <c r="D139" s="2"/>
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
       <c r="G139" s="2"/>
@@ -3211,10 +3081,8 @@
     <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
-      <c r="C140" s="4"/>
-      <c r="D140" s="2">
-        <v>139</v>
-      </c>
+      <c r="C140" s="3"/>
+      <c r="D140" s="2"/>
       <c r="E140" s="2"/>
       <c r="F140" s="2"/>
       <c r="G140" s="2"/>
@@ -3227,10 +3095,8 @@
     <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
-      <c r="C141" s="4"/>
-      <c r="D141" s="2">
-        <v>140</v>
-      </c>
+      <c r="C141" s="3"/>
+      <c r="D141" s="2"/>
       <c r="E141" s="2"/>
       <c r="F141" s="2"/>
       <c r="G141" s="2"/>
@@ -3243,10 +3109,8 @@
     <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
-      <c r="C142" s="4"/>
-      <c r="D142" s="2">
-        <v>141</v>
-      </c>
+      <c r="C142" s="3"/>
+      <c r="D142" s="2"/>
       <c r="E142" s="2"/>
       <c r="F142" s="2"/>
       <c r="G142" s="2"/>
@@ -3259,10 +3123,8 @@
     <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
-      <c r="C143" s="4"/>
-      <c r="D143" s="2">
-        <v>142</v>
-      </c>
+      <c r="C143" s="3"/>
+      <c r="D143" s="2"/>
       <c r="E143" s="2"/>
       <c r="F143" s="2"/>
       <c r="G143" s="2"/>
@@ -3275,10 +3137,8 @@
     <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
-      <c r="C144" s="4"/>
-      <c r="D144" s="2">
-        <v>143</v>
-      </c>
+      <c r="C144" s="3"/>
+      <c r="D144" s="2"/>
       <c r="E144" s="2"/>
       <c r="F144" s="2"/>
       <c r="G144" s="2"/>
@@ -3291,10 +3151,8 @@
     <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
-      <c r="C145" s="4"/>
-      <c r="D145" s="2">
-        <v>144</v>
-      </c>
+      <c r="C145" s="3"/>
+      <c r="D145" s="2"/>
       <c r="E145" s="2"/>
       <c r="F145" s="2"/>
       <c r="G145" s="2"/>
@@ -3307,10 +3165,8 @@
     <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
-      <c r="C146" s="4"/>
-      <c r="D146" s="2">
-        <v>145</v>
-      </c>
+      <c r="C146" s="3"/>
+      <c r="D146" s="2"/>
       <c r="E146" s="2"/>
       <c r="F146" s="2"/>
       <c r="G146" s="2"/>
@@ -3323,10 +3179,8 @@
     <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
-      <c r="C147" s="4"/>
-      <c r="D147" s="2">
-        <v>146</v>
-      </c>
+      <c r="C147" s="3"/>
+      <c r="D147" s="2"/>
       <c r="E147" s="2"/>
       <c r="F147" s="2"/>
       <c r="G147" s="2"/>
@@ -3339,10 +3193,8 @@
     <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
-      <c r="C148" s="4"/>
-      <c r="D148" s="2">
-        <v>147</v>
-      </c>
+      <c r="C148" s="3"/>
+      <c r="D148" s="2"/>
       <c r="E148" s="2"/>
       <c r="F148" s="2"/>
       <c r="G148" s="2"/>
@@ -3355,10 +3207,8 @@
     <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
-      <c r="C149" s="4"/>
-      <c r="D149" s="2">
-        <v>148</v>
-      </c>
+      <c r="C149" s="3"/>
+      <c r="D149" s="2"/>
       <c r="E149" s="2"/>
       <c r="F149" s="2"/>
       <c r="G149" s="2"/>
@@ -3371,10 +3221,8 @@
     <row r="150" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
-      <c r="C150" s="4"/>
-      <c r="D150" s="2">
-        <v>149</v>
-      </c>
+      <c r="C150" s="3"/>
+      <c r="D150" s="2"/>
       <c r="E150" s="2"/>
       <c r="F150" s="2"/>
       <c r="G150" s="2"/>
@@ -3387,10 +3235,8 @@
     <row r="151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
-      <c r="C151" s="4"/>
-      <c r="D151" s="2">
-        <v>150</v>
-      </c>
+      <c r="C151" s="3"/>
+      <c r="D151" s="2"/>
       <c r="E151" s="2"/>
       <c r="F151" s="2"/>
       <c r="G151" s="2"/>

</xml_diff>

<commit_message>
Guess this got updated
</commit_message>
<xml_diff>
--- a/family-tree-data.xlsx
+++ b/family-tree-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASHil\PycharmProjects\Family-Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B7527F-0387-41BA-B6F1-B86BA18DB761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A911B073-EE98-40D0-B057-EB4F3CF6F07A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -356,7 +356,7 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="164" formatCode="00000"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -388,7 +388,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="00000"/>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -453,15 +453,15 @@
     <tableColumn id="1" xr3:uid="{5EDD3C60-3C2C-40F1-97A9-01DC19C6B82F}" name="First Name" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{EF0889F4-AB8A-4E41-9EE4-5A2BF0BFD794}" name="Last Name" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{86E4CF69-FB69-4B21-9BFA-43FDA0099215}" name="Class Year" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{8F0F6FA8-92FF-40FE-A11F-6C2D1597C063}" name="Parse ID" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{61B9159E-610A-4A8F-9F0C-DEABBF5DB327}" name="Parent 1" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{199D1D06-A3D8-46C8-A02F-9AAF042D9958}" name="Parent 2" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{63E6E218-11FC-4D75-B8E3-C44083B6218B}" name="Parent 3" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{CA4B4E19-AB25-4B2D-9E06-CD50BB63F1BD}" name="Child 1" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{F4158ED3-1229-4E63-A0E7-5AD8267EBDC7}" name="Child 2" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{A731EFD4-7198-4860-8DC3-7C61CF8B688C}" name="Child 3" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{095C504D-C521-47E5-85CA-8FB45B7FF673}" name="Child 4" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{8A459A0C-705E-4C06-B161-AC9856E8D667}" name="Child 5" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{8F0F6FA8-92FF-40FE-A11F-6C2D1597C063}" name="Parse ID" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{61B9159E-610A-4A8F-9F0C-DEABBF5DB327}" name="Parent 1" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{199D1D06-A3D8-46C8-A02F-9AAF042D9958}" name="Parent 2" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{63E6E218-11FC-4D75-B8E3-C44083B6218B}" name="Parent 3" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{CA4B4E19-AB25-4B2D-9E06-CD50BB63F1BD}" name="Child 1" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{F4158ED3-1229-4E63-A0E7-5AD8267EBDC7}" name="Child 2" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{A731EFD4-7198-4860-8DC3-7C61CF8B688C}" name="Child 3" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{095C504D-C521-47E5-85CA-8FB45B7FF673}" name="Child 4" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{8A459A0C-705E-4C06-B161-AC9856E8D667}" name="Child 5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -734,7 +734,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H45" sqref="H45"/>
+      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added 3 people from Mr Wood family
Rich Marquardt, Josh Wood, and Joseph Scroggins
</commit_message>
<xml_diff>
--- a/family-tree-data.xlsx
+++ b/family-tree-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASHil\PycharmProjects\Family-Tree\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Family-Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0545CD8-8B1F-4608-8108-F99863EFBD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E935C614-A728-4DC9-AE01-712E1C8E1E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
   <si>
     <t>Class Year</t>
   </si>
@@ -237,6 +237,24 @@
   </si>
   <si>
     <t>Coss</t>
+  </si>
+  <si>
+    <t>Rich</t>
+  </si>
+  <si>
+    <t>Marquardt</t>
+  </si>
+  <si>
+    <t>Josh</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Scroggins</t>
   </si>
 </sst>
 </file>
@@ -461,15 +479,15 @@
     <tableColumn id="1" xr3:uid="{5EDD3C60-3C2C-40F1-97A9-01DC19C6B82F}" name="First Name" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{EF0889F4-AB8A-4E41-9EE4-5A2BF0BFD794}" name="Last Name" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{86E4CF69-FB69-4B21-9BFA-43FDA0099215}" name="Class Year" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{8F0F6FA8-92FF-40FE-A11F-6C2D1597C063}" name="Parse ID" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{61B9159E-610A-4A8F-9F0C-DEABBF5DB327}" name="Parent 1" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{199D1D06-A3D8-46C8-A02F-9AAF042D9958}" name="Parent 2" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{63E6E218-11FC-4D75-B8E3-C44083B6218B}" name="Parent 3" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{CA4B4E19-AB25-4B2D-9E06-CD50BB63F1BD}" name="Child 1" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{F4158ED3-1229-4E63-A0E7-5AD8267EBDC7}" name="Child 2" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{A731EFD4-7198-4860-8DC3-7C61CF8B688C}" name="Child 3" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{095C504D-C521-47E5-85CA-8FB45B7FF673}" name="Child 4" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{8A459A0C-705E-4C06-B161-AC9856E8D667}" name="Child 5" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{8F0F6FA8-92FF-40FE-A11F-6C2D1597C063}" name="Parse ID" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{61B9159E-610A-4A8F-9F0C-DEABBF5DB327}" name="Parent 1" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{199D1D06-A3D8-46C8-A02F-9AAF042D9958}" name="Parent 2" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{63E6E218-11FC-4D75-B8E3-C44083B6218B}" name="Parent 3" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{CA4B4E19-AB25-4B2D-9E06-CD50BB63F1BD}" name="Child 1" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{F4158ED3-1229-4E63-A0E7-5AD8267EBDC7}" name="Child 2" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{A731EFD4-7198-4860-8DC3-7C61CF8B688C}" name="Child 3" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{095C504D-C521-47E5-85CA-8FB45B7FF673}" name="Child 4" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{8A459A0C-705E-4C06-B161-AC9856E8D667}" name="Child 5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -742,18 +760,18 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" style="12" customWidth="1"/>
-    <col min="5" max="11" width="17.77734375" customWidth="1"/>
+    <col min="1" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="12" customWidth="1"/>
+    <col min="5" max="11" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
@@ -791,7 +809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -821,7 +839,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -845,7 +863,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
@@ -871,7 +889,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>57</v>
       </c>
@@ -895,7 +913,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
@@ -919,7 +937,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -945,7 +963,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
@@ -971,7 +989,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -995,7 +1013,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1019,7 +1037,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1053,7 +1071,7 @@
       </c>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1079,7 +1097,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -1107,7 +1125,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>61</v>
       </c>
@@ -1131,7 +1149,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1155,7 +1173,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>55</v>
       </c>
@@ -1181,7 +1199,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
@@ -1207,7 +1225,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
@@ -1235,7 +1253,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -1259,7 +1277,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1285,7 +1303,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -1311,7 +1329,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -1335,7 +1353,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
@@ -1363,7 +1381,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -1389,7 +1407,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1415,7 +1433,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1439,7 +1457,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -1463,7 +1481,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>48</v>
       </c>
@@ -1487,7 +1505,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1517,7 +1535,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
@@ -1541,7 +1559,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -1565,7 +1583,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
@@ -1591,7 +1609,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>65</v>
       </c>
@@ -1613,46 +1631,72 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="3"/>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="3">
+        <v>2021</v>
+      </c>
       <c r="D34" s="2">
         <v>33</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
+      <c r="H34" s="2">
+        <v>34</v>
+      </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="3"/>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="3">
+        <v>2023</v>
+      </c>
       <c r="D35" s="2">
         <v>34</v>
       </c>
-      <c r="E35" s="2"/>
+      <c r="E35" s="2">
+        <v>33</v>
+      </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
+      <c r="H35" s="2">
+        <v>35</v>
+      </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="3"/>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="3">
+        <v>2025</v>
+      </c>
       <c r="D36" s="2">
         <v>35</v>
       </c>
-      <c r="E36" s="2"/>
+      <c r="E36" s="2">
+        <v>34</v>
+      </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -1661,7 +1705,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="3"/>
@@ -1677,7 +1721,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="3"/>
@@ -1693,7 +1737,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="3"/>
@@ -1709,7 +1753,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
@@ -1725,7 +1769,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
@@ -1741,7 +1785,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
@@ -1757,7 +1801,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
@@ -1773,7 +1817,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
@@ -1789,7 +1833,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="3"/>
@@ -1805,7 +1849,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="3"/>
@@ -1821,7 +1865,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="3"/>
@@ -1837,7 +1881,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="3"/>
@@ -1853,7 +1897,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="3"/>
@@ -1869,7 +1913,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="3"/>
@@ -1885,7 +1929,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="3"/>
@@ -1901,7 +1945,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="3"/>
@@ -1917,7 +1961,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="3"/>
@@ -1933,7 +1977,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="3"/>
@@ -1949,7 +1993,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="3"/>
@@ -1965,7 +2009,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="3"/>
@@ -1981,7 +2025,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="3"/>
@@ -1997,7 +2041,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="3"/>
@@ -2013,7 +2057,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="3"/>
@@ -2029,7 +2073,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="3"/>
@@ -2045,7 +2089,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="3"/>
@@ -2061,7 +2105,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="3"/>
@@ -2077,7 +2121,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="3"/>
@@ -2093,7 +2137,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="3"/>
@@ -2109,7 +2153,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="3"/>
@@ -2125,7 +2169,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="3"/>
@@ -2141,7 +2185,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="3"/>
@@ -2157,7 +2201,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="3"/>
@@ -2173,7 +2217,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="3"/>
@@ -2189,7 +2233,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="3"/>
@@ -2205,7 +2249,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="3"/>
@@ -2221,7 +2265,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="3"/>
@@ -2237,7 +2281,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="3"/>
@@ -2253,7 +2297,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="3"/>
@@ -2269,7 +2313,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="3"/>
@@ -2285,7 +2329,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="3"/>
@@ -2301,7 +2345,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="3"/>
@@ -2317,7 +2361,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="3"/>
@@ -2333,7 +2377,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="3"/>
@@ -2349,7 +2393,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="3"/>
@@ -2365,7 +2409,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="3"/>
@@ -2381,7 +2425,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="3"/>
@@ -2397,7 +2441,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="3"/>
@@ -2413,7 +2457,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="3"/>
@@ -2429,7 +2473,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="3"/>
@@ -2445,7 +2489,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="3"/>
@@ -2461,7 +2505,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="3"/>
@@ -2477,7 +2521,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="3"/>
@@ -2493,7 +2537,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="3"/>
@@ -2509,7 +2553,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="3"/>
@@ -2525,7 +2569,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="3"/>
@@ -2541,7 +2585,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="3"/>
@@ -2557,7 +2601,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="3"/>
@@ -2573,7 +2617,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="3"/>
@@ -2589,7 +2633,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="3"/>
@@ -2605,7 +2649,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="3"/>
@@ -2621,7 +2665,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="3"/>
@@ -2637,7 +2681,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="3"/>
@@ -2653,7 +2697,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="3"/>
@@ -2669,7 +2713,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="3"/>
@@ -2685,7 +2729,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="3"/>
@@ -2701,7 +2745,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="3"/>
@@ -2717,7 +2761,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="3"/>
@@ -2733,7 +2777,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="3"/>
@@ -2749,7 +2793,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="3"/>
@@ -2765,7 +2809,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="3"/>
@@ -2781,7 +2825,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="3"/>
@@ -2797,7 +2841,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="3"/>
@@ -2813,7 +2857,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="3"/>
@@ -2829,7 +2873,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="3"/>
@@ -2845,7 +2889,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="3"/>
@@ -2861,7 +2905,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="3"/>
@@ -2877,7 +2921,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="3"/>
@@ -2893,7 +2937,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="3"/>
@@ -2909,7 +2953,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="3"/>
@@ -2925,7 +2969,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="3"/>
@@ -2941,7 +2985,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="3"/>
@@ -2957,7 +3001,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="3"/>
@@ -2973,7 +3017,7 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="3"/>
@@ -2989,7 +3033,7 @@
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="3"/>
@@ -3005,7 +3049,7 @@
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="3"/>
@@ -3021,7 +3065,7 @@
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="3"/>
@@ -3037,7 +3081,7 @@
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="3"/>
@@ -3053,7 +3097,7 @@
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="3"/>
@@ -3069,7 +3113,7 @@
       <c r="K124" s="2"/>
       <c r="L124" s="2"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="3"/>
@@ -3085,7 +3129,7 @@
       <c r="K125" s="2"/>
       <c r="L125" s="2"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="3"/>
@@ -3101,7 +3145,7 @@
       <c r="K126" s="2"/>
       <c r="L126" s="2"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="3"/>
@@ -3117,7 +3161,7 @@
       <c r="K127" s="2"/>
       <c r="L127" s="2"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="3"/>
@@ -3133,7 +3177,7 @@
       <c r="K128" s="2"/>
       <c r="L128" s="2"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="3"/>
@@ -3149,7 +3193,7 @@
       <c r="K129" s="2"/>
       <c r="L129" s="2"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="3"/>
@@ -3165,7 +3209,7 @@
       <c r="K130" s="2"/>
       <c r="L130" s="2"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="3"/>
@@ -3181,7 +3225,7 @@
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="3"/>
@@ -3197,7 +3241,7 @@
       <c r="K132" s="2"/>
       <c r="L132" s="2"/>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="3"/>
@@ -3213,7 +3257,7 @@
       <c r="K133" s="2"/>
       <c r="L133" s="2"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="3"/>
@@ -3229,7 +3273,7 @@
       <c r="K134" s="2"/>
       <c r="L134" s="2"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="3"/>
@@ -3245,7 +3289,7 @@
       <c r="K135" s="2"/>
       <c r="L135" s="2"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="3"/>
@@ -3261,7 +3305,7 @@
       <c r="K136" s="2"/>
       <c r="L136" s="2"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="3"/>
@@ -3277,7 +3321,7 @@
       <c r="K137" s="2"/>
       <c r="L137" s="2"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="3"/>
@@ -3293,7 +3337,7 @@
       <c r="K138" s="2"/>
       <c r="L138" s="2"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="3"/>
@@ -3309,7 +3353,7 @@
       <c r="K139" s="2"/>
       <c r="L139" s="2"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="3"/>
@@ -3325,7 +3369,7 @@
       <c r="K140" s="2"/>
       <c r="L140" s="2"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="3"/>
@@ -3341,7 +3385,7 @@
       <c r="K141" s="2"/>
       <c r="L141" s="2"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="3"/>
@@ -3357,7 +3401,7 @@
       <c r="K142" s="2"/>
       <c r="L142" s="2"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="3"/>
@@ -3373,7 +3417,7 @@
       <c r="K143" s="2"/>
       <c r="L143" s="2"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="3"/>
@@ -3389,7 +3433,7 @@
       <c r="K144" s="2"/>
       <c r="L144" s="2"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="3"/>
@@ -3405,7 +3449,7 @@
       <c r="K145" s="2"/>
       <c r="L145" s="2"/>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="3"/>
@@ -3421,7 +3465,7 @@
       <c r="K146" s="2"/>
       <c r="L146" s="2"/>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="3"/>
@@ -3437,7 +3481,7 @@
       <c r="K147" s="2"/>
       <c r="L147" s="2"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="3"/>
@@ -3453,7 +3497,7 @@
       <c r="K148" s="2"/>
       <c r="L148" s="2"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="3"/>
@@ -3469,7 +3513,7 @@
       <c r="K149" s="2"/>
       <c r="L149" s="2"/>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="3"/>
@@ -3485,7 +3529,7 @@
       <c r="K150" s="2"/>
       <c r="L150" s="2"/>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="3"/>

</xml_diff>

<commit_message>
updated Ben King's child
</commit_message>
<xml_diff>
--- a/family-tree-data.xlsx
+++ b/family-tree-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASHil\PycharmProjects\Family-Tree\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Family-Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEF8B5E-F0BD-4C8E-8C9E-35A0AF2E83A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECB7941-E3D4-4C2E-BC7B-708263E8B01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5250" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -476,7 +476,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{11C3A996-264D-49A5-B58C-4848FCDD6F03}" name="Table2" displayName="Table2" ref="A1:L151" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
   <autoFilter ref="A1:L151" xr:uid="{11C3A996-264D-49A5-B58C-4848FCDD6F03}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L151">
-    <sortCondition ref="D1:D151"/>
+    <sortCondition ref="B1:B151"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{5EDD3C60-3C2C-40F1-97A9-01DC19C6B82F}" name="First Name" dataDxfId="11"/>
@@ -763,18 +763,18 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="12" customWidth="1"/>
-    <col min="5" max="11" width="17.6640625" customWidth="1"/>
+    <col min="1" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="12" customWidth="1"/>
+    <col min="5" max="11" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
@@ -812,131 +812,125 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4">
-        <v>9999</v>
+        <v>33</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2017</v>
       </c>
       <c r="D2" s="2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2">
-        <v>99999</v>
+        <v>8</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="H2" s="2">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2">
+        <v>19</v>
+      </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="3">
+        <v>9999</v>
+      </c>
+      <c r="D3" s="2">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2016</v>
+      </c>
+      <c r="D4" s="2">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2008</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>32</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2">
-        <v>3</v>
-      </c>
-      <c r="I3" s="2">
-        <v>4</v>
-      </c>
-      <c r="J3" s="2">
-        <v>5</v>
-      </c>
-      <c r="K3" s="2">
-        <v>6</v>
-      </c>
-      <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1">
-        <v>9999</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3</v>
-      </c>
       <c r="E4" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="1">
-        <v>9999</v>
+        <v>58</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2020</v>
       </c>
       <c r="D5" s="2">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2">
-        <v>8</v>
-      </c>
+      <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="1">
-        <v>9999</v>
+        <v>51</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2021</v>
       </c>
       <c r="D6" s="2">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -946,211 +940,209 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="1">
-        <v>9999</v>
+        <v>42</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2020</v>
       </c>
       <c r="D7" s="2">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>24</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2013</v>
+        <v>53</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2022</v>
       </c>
       <c r="D8" s="2">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E8" s="2">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="C9" s="3">
         <v>9999</v>
       </c>
       <c r="D9" s="2">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E9" s="2">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2">
-        <v>11</v>
-      </c>
+      <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="C10" s="3">
-        <v>9999</v>
+        <v>2025</v>
       </c>
       <c r="D10" s="2">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E10" s="2">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2">
-        <v>12</v>
-      </c>
-      <c r="I10" s="2">
-        <v>13</v>
-      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="3">
-        <v>2014</v>
+        <v>15</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2008</v>
       </c>
       <c r="D11" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E11" s="2">
-        <v>7</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>32</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="I11" s="2">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="J11" s="2">
-        <v>16</v>
-      </c>
-      <c r="K11" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="K11" s="2">
+        <v>6</v>
+      </c>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="3">
-        <v>2017</v>
+        <v>18</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9999</v>
       </c>
       <c r="D12" s="2">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E12" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2">
-        <v>17</v>
-      </c>
-      <c r="I12" s="2">
-        <v>18</v>
-      </c>
-      <c r="J12" s="2">
-        <v>19</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C13" s="3">
-        <v>9999</v>
+        <v>2008</v>
       </c>
       <c r="D13" s="2">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E13" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2">
-        <v>20</v>
-      </c>
-      <c r="I13" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="I13" s="2">
+        <v>22</v>
+      </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="C14" s="3">
-        <v>9999</v>
+        <v>2024</v>
       </c>
       <c r="D14" s="2">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="E14" s="2">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1160,92 +1152,94 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="3">
-        <v>2016</v>
+        <v>9999</v>
       </c>
       <c r="D15" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="2">
-        <v>21</v>
-      </c>
+      <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="C16" s="3">
-        <v>9999</v>
+        <v>2023</v>
       </c>
       <c r="D16" s="2">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E16" s="2">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2">
+        <v>29</v>
+      </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="C17" s="3">
-        <v>9999</v>
+        <v>2023</v>
       </c>
       <c r="D17" s="2">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E17" s="2">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2">
+        <v>30</v>
+      </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C18" s="3">
-        <v>2008</v>
+        <v>2020</v>
       </c>
       <c r="D18" s="2">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E18" s="2">
         <v>11</v>
@@ -1253,208 +1247,212 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I18" s="2">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="3">
-        <v>2020</v>
+        <v>13</v>
+      </c>
+      <c r="C19" s="4">
+        <v>9999</v>
       </c>
       <c r="D19" s="2">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2">
-        <v>11</v>
+        <v>99999</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="3">
-        <v>2020</v>
+        <v>20</v>
+      </c>
+      <c r="C20" s="1">
+        <v>9999</v>
       </c>
       <c r="D20" s="2">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E20" s="2">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2">
-        <v>25</v>
-      </c>
-      <c r="I20" s="2">
-        <v>26</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C21" s="3">
         <v>9999</v>
       </c>
       <c r="D21" s="2">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E21" s="2">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="H21" s="2">
+        <v>20</v>
+      </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" s="3">
-        <v>2017</v>
+        <v>9999</v>
       </c>
       <c r="D22" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E22" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="2">
-        <v>27</v>
-      </c>
+      <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C23" s="3">
-        <v>2020</v>
+        <v>9999</v>
       </c>
       <c r="D23" s="2">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E23" s="2">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+      <c r="H23" s="2">
+        <v>12</v>
+      </c>
+      <c r="I23" s="2">
+        <v>13</v>
+      </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C24" s="3">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="D24" s="2">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E24" s="2">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="H24" s="2">
+        <v>27</v>
+      </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="3">
-        <v>2022</v>
+        <v>26</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2013</v>
       </c>
       <c r="D25" s="2">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E25" s="2">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="3">
+        <v>24</v>
+      </c>
+      <c r="C26" s="1">
         <v>9999</v>
       </c>
       <c r="D26" s="2">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E26" s="2">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1464,47 +1462,45 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="3">
-        <v>2023</v>
+        <v>22</v>
+      </c>
+      <c r="C27" s="1">
+        <v>9999</v>
       </c>
       <c r="D27" s="2">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="E27" s="2">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="2">
-        <v>29</v>
-      </c>
+      <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C28" s="3">
         <v>2020</v>
       </c>
       <c r="D28" s="2">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E28" s="2">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -1514,47 +1510,51 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="C29" s="3">
-        <v>2023</v>
+        <v>2014</v>
       </c>
       <c r="D29" s="2">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="E29" s="2">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2">
-        <v>30</v>
-      </c>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="I29" s="2">
+        <v>15</v>
+      </c>
+      <c r="J29" s="2">
+        <v>16</v>
+      </c>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="C30" s="3">
-        <v>2024</v>
+        <v>9999</v>
       </c>
       <c r="D30" s="2">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E30" s="2">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -1564,21 +1564,21 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="C31" s="3">
-        <v>2025</v>
+        <v>9999</v>
       </c>
       <c r="D31" s="2">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E31" s="2">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -1588,31 +1588,33 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="C32" s="3">
         <v>9999</v>
       </c>
       <c r="D32" s="2">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E32" s="2">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="H32" s="2">
+        <v>11</v>
+      </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>65</v>
       </c>
@@ -1634,7 +1636,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>67</v>
       </c>
@@ -1658,7 +1660,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>69</v>
       </c>
@@ -1684,7 +1686,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>71</v>
       </c>
@@ -1708,7 +1710,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>73</v>
       </c>
@@ -1732,7 +1734,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="3"/>
@@ -1748,7 +1750,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="3"/>
@@ -1764,7 +1766,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
@@ -1780,7 +1782,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
@@ -1796,7 +1798,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
@@ -1812,7 +1814,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
@@ -1828,7 +1830,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
@@ -1844,7 +1846,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="3"/>
@@ -1860,7 +1862,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="3"/>
@@ -1876,7 +1878,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="3"/>
@@ -1892,7 +1894,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="3"/>
@@ -1908,7 +1910,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="3"/>
@@ -1924,7 +1926,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="3"/>
@@ -1940,7 +1942,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="3"/>
@@ -1956,7 +1958,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="3"/>
@@ -1972,7 +1974,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="3"/>
@@ -1988,7 +1990,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="3"/>
@@ -2004,7 +2006,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="3"/>
@@ -2020,7 +2022,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="3"/>
@@ -2036,7 +2038,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="3"/>
@@ -2052,7 +2054,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="3"/>
@@ -2068,7 +2070,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="3"/>
@@ -2084,7 +2086,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="3"/>
@@ -2100,7 +2102,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="3"/>
@@ -2116,7 +2118,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="3"/>
@@ -2132,7 +2134,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="3"/>
@@ -2148,7 +2150,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="3"/>
@@ -2164,7 +2166,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="3"/>
@@ -2180,7 +2182,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="3"/>
@@ -2196,7 +2198,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="3"/>
@@ -2212,7 +2214,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="3"/>
@@ -2228,7 +2230,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="3"/>
@@ -2244,7 +2246,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="3"/>
@@ -2260,7 +2262,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="3"/>
@@ -2276,7 +2278,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="3"/>
@@ -2292,7 +2294,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="3"/>
@@ -2308,7 +2310,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="3"/>
@@ -2324,7 +2326,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="3"/>
@@ -2340,7 +2342,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="3"/>
@@ -2356,7 +2358,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="3"/>
@@ -2372,7 +2374,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="3"/>
@@ -2388,7 +2390,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="3"/>
@@ -2404,7 +2406,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="3"/>
@@ -2420,7 +2422,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="3"/>
@@ -2436,7 +2438,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="3"/>
@@ -2452,7 +2454,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="3"/>
@@ -2468,7 +2470,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="3"/>
@@ -2484,7 +2486,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="3"/>
@@ -2500,7 +2502,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="3"/>
@@ -2516,7 +2518,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="3"/>
@@ -2532,7 +2534,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="3"/>
@@ -2548,7 +2550,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="3"/>
@@ -2564,7 +2566,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="3"/>
@@ -2580,7 +2582,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="3"/>
@@ -2596,7 +2598,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="3"/>
@@ -2612,7 +2614,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="3"/>
@@ -2628,7 +2630,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="3"/>
@@ -2644,7 +2646,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="3"/>
@@ -2660,7 +2662,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="3"/>
@@ -2676,7 +2678,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="3"/>
@@ -2692,7 +2694,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="3"/>
@@ -2708,7 +2710,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="3"/>
@@ -2724,7 +2726,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="3"/>
@@ -2740,7 +2742,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="3"/>
@@ -2756,7 +2758,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="3"/>
@@ -2772,7 +2774,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="3"/>
@@ -2788,7 +2790,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="3"/>
@@ -2804,7 +2806,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="3"/>
@@ -2820,7 +2822,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="3"/>
@@ -2836,7 +2838,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="3"/>
@@ -2852,7 +2854,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="3"/>
@@ -2868,7 +2870,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="3"/>
@@ -2884,7 +2886,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="3"/>
@@ -2900,7 +2902,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="3"/>
@@ -2916,7 +2918,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="3"/>
@@ -2932,7 +2934,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="3"/>
@@ -2948,7 +2950,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="3"/>
@@ -2964,7 +2966,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="3"/>
@@ -2980,7 +2982,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="3"/>
@@ -2996,7 +2998,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="3"/>
@@ -3012,7 +3014,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="3"/>
@@ -3028,7 +3030,7 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="3"/>
@@ -3044,7 +3046,7 @@
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="3"/>
@@ -3060,7 +3062,7 @@
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="3"/>
@@ -3076,7 +3078,7 @@
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="3"/>
@@ -3092,7 +3094,7 @@
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="3"/>
@@ -3108,7 +3110,7 @@
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="3"/>
@@ -3124,7 +3126,7 @@
       <c r="K124" s="2"/>
       <c r="L124" s="2"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="3"/>
@@ -3140,7 +3142,7 @@
       <c r="K125" s="2"/>
       <c r="L125" s="2"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="3"/>
@@ -3156,7 +3158,7 @@
       <c r="K126" s="2"/>
       <c r="L126" s="2"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="3"/>
@@ -3172,7 +3174,7 @@
       <c r="K127" s="2"/>
       <c r="L127" s="2"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="3"/>
@@ -3188,7 +3190,7 @@
       <c r="K128" s="2"/>
       <c r="L128" s="2"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="3"/>
@@ -3204,7 +3206,7 @@
       <c r="K129" s="2"/>
       <c r="L129" s="2"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="3"/>
@@ -3220,7 +3222,7 @@
       <c r="K130" s="2"/>
       <c r="L130" s="2"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="3"/>
@@ -3236,7 +3238,7 @@
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="3"/>
@@ -3252,7 +3254,7 @@
       <c r="K132" s="2"/>
       <c r="L132" s="2"/>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="3"/>
@@ -3268,7 +3270,7 @@
       <c r="K133" s="2"/>
       <c r="L133" s="2"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="3"/>
@@ -3284,7 +3286,7 @@
       <c r="K134" s="2"/>
       <c r="L134" s="2"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="3"/>
@@ -3300,7 +3302,7 @@
       <c r="K135" s="2"/>
       <c r="L135" s="2"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="3"/>
@@ -3316,7 +3318,7 @@
       <c r="K136" s="2"/>
       <c r="L136" s="2"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="3"/>
@@ -3332,7 +3334,7 @@
       <c r="K137" s="2"/>
       <c r="L137" s="2"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="3"/>
@@ -3348,7 +3350,7 @@
       <c r="K138" s="2"/>
       <c r="L138" s="2"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="3"/>
@@ -3364,7 +3366,7 @@
       <c r="K139" s="2"/>
       <c r="L139" s="2"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="3"/>
@@ -3380,7 +3382,7 @@
       <c r="K140" s="2"/>
       <c r="L140" s="2"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="3"/>
@@ -3396,7 +3398,7 @@
       <c r="K141" s="2"/>
       <c r="L141" s="2"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="3"/>
@@ -3412,7 +3414,7 @@
       <c r="K142" s="2"/>
       <c r="L142" s="2"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="3"/>
@@ -3428,7 +3430,7 @@
       <c r="K143" s="2"/>
       <c r="L143" s="2"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="3"/>
@@ -3444,7 +3446,7 @@
       <c r="K144" s="2"/>
       <c r="L144" s="2"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="3"/>
@@ -3460,7 +3462,7 @@
       <c r="K145" s="2"/>
       <c r="L145" s="2"/>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="3"/>
@@ -3476,7 +3478,7 @@
       <c r="K146" s="2"/>
       <c r="L146" s="2"/>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="3"/>
@@ -3492,7 +3494,7 @@
       <c r="K147" s="2"/>
       <c r="L147" s="2"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="3"/>
@@ -3508,7 +3510,7 @@
       <c r="K148" s="2"/>
       <c r="L148" s="2"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="3"/>
@@ -3524,7 +3526,7 @@
       <c r="K149" s="2"/>
       <c r="L149" s="2"/>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="3"/>
@@ -3540,7 +3542,7 @@
       <c r="K150" s="2"/>
       <c r="L150" s="2"/>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="3"/>

</xml_diff>

<commit_message>
changed a parent id to null
</commit_message>
<xml_diff>
--- a/family-tree-data.xlsx
+++ b/family-tree-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Family-Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECB7941-E3D4-4C2E-BC7B-708263E8B01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F675D8-EA04-416A-A37B-E86B37BEC3A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5250" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -476,7 +476,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{11C3A996-264D-49A5-B58C-4848FCDD6F03}" name="Table2" displayName="Table2" ref="A1:L151" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
   <autoFilter ref="A1:L151" xr:uid="{11C3A996-264D-49A5-B58C-4848FCDD6F03}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L151">
-    <sortCondition ref="B1:B151"/>
+    <sortCondition ref="D1:D151"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{5EDD3C60-3C2C-40F1-97A9-01DC19C6B82F}" name="First Name" dataDxfId="11"/>
@@ -763,7 +763,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,78 +814,82 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="3">
-        <v>2017</v>
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>9999</v>
       </c>
       <c r="D2" s="2">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2">
-        <v>8</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2">
-        <v>17</v>
-      </c>
-      <c r="I2" s="2">
-        <v>18</v>
-      </c>
-      <c r="J2" s="2">
-        <v>19</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="3">
-        <v>9999</v>
+        <v>15</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2008</v>
       </c>
       <c r="D3" s="2">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2">
-        <v>19</v>
-      </c>
-      <c r="F3" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>32</v>
+      </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="H3" s="2">
+        <v>3</v>
+      </c>
+      <c r="I3" s="2">
+        <v>4</v>
+      </c>
+      <c r="J3" s="2">
+        <v>5</v>
+      </c>
+      <c r="K3" s="2">
+        <v>6</v>
+      </c>
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="3">
-        <v>2016</v>
+        <v>18</v>
+      </c>
+      <c r="C4" s="1">
+        <v>9999</v>
       </c>
       <c r="D4" s="2">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -894,23 +898,25 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2020</v>
+        <v>20</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9999</v>
       </c>
       <c r="D5" s="2">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="E5" s="2">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="H5" s="2">
+        <v>8</v>
+      </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -918,19 +924,19 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2021</v>
+        <v>22</v>
+      </c>
+      <c r="C6" s="1">
+        <v>9999</v>
       </c>
       <c r="D6" s="2">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="E6" s="2">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -942,25 +948,23 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="3">
-        <v>2020</v>
+        <v>24</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9999</v>
       </c>
       <c r="D7" s="2">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E7" s="2">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2">
-        <v>24</v>
-      </c>
+      <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -968,24 +972,24 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="3">
-        <v>2022</v>
+        <v>26</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2013</v>
       </c>
       <c r="D8" s="2">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -994,23 +998,25 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3">
         <v>9999</v>
       </c>
       <c r="D9" s="2">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2">
+        <v>11</v>
+      </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -1018,131 +1024,133 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="C10" s="3">
-        <v>2025</v>
+        <v>9999</v>
       </c>
       <c r="D10" s="2">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="H10" s="2">
+        <v>12</v>
+      </c>
+      <c r="I10" s="2">
+        <v>13</v>
+      </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2008</v>
+        <v>31</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2014</v>
       </c>
       <c r="D11" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E11" s="2">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2">
-        <v>32</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="I11" s="2">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="J11" s="2">
-        <v>5</v>
-      </c>
-      <c r="K11" s="2">
-        <v>6</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1">
-        <v>9999</v>
+        <v>33</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2017</v>
       </c>
       <c r="D12" s="2">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E12" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2">
-        <v>7</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="I12" s="2">
+        <v>18</v>
+      </c>
+      <c r="J12" s="2">
+        <v>19</v>
+      </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C13" s="3">
-        <v>2008</v>
+        <v>9999</v>
       </c>
       <c r="D13" s="2">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E13" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2">
-        <v>23</v>
-      </c>
-      <c r="I13" s="2">
-        <v>22</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="C14" s="3">
-        <v>2024</v>
+        <v>9999</v>
       </c>
       <c r="D14" s="2">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="E14" s="2">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1154,23 +1162,25 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C15" s="3">
-        <v>9999</v>
+        <v>2016</v>
       </c>
       <c r="D15" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E15" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="H15" s="2">
+        <v>21</v>
+      </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -1178,25 +1188,23 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="C16" s="3">
-        <v>2023</v>
+        <v>9999</v>
       </c>
       <c r="D16" s="2">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E16" s="2">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2">
-        <v>29</v>
-      </c>
+      <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1204,25 +1212,23 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="C17" s="3">
-        <v>2023</v>
+        <v>9999</v>
       </c>
       <c r="D17" s="2">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E17" s="2">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="2">
-        <v>30</v>
-      </c>
+      <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1230,16 +1236,16 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C18" s="3">
-        <v>2020</v>
+        <v>2008</v>
       </c>
       <c r="D18" s="2">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E18" s="2">
         <v>11</v>
@@ -1247,10 +1253,10 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I18" s="2">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -1258,24 +1264,24 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="4">
-        <v>9999</v>
+        <v>42</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2020</v>
       </c>
       <c r="D19" s="2">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E19" s="2">
-        <v>99999</v>
+        <v>11</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1284,26 +1290,28 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="1">
-        <v>9999</v>
-      </c>
-      <c r="D20" s="2">
-        <v>4</v>
-      </c>
       <c r="E20" s="2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2">
-        <v>8</v>
-      </c>
-      <c r="I20" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="I20" s="2">
+        <v>26</v>
+      </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -1313,22 +1321,20 @@
         <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C21" s="3">
         <v>9999</v>
       </c>
       <c r="D21" s="2">
+        <v>20</v>
+      </c>
+      <c r="E21" s="2">
         <v>12</v>
-      </c>
-      <c r="E21" s="2">
-        <v>9</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2">
-        <v>20</v>
-      </c>
+      <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -1336,23 +1342,25 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C22" s="3">
-        <v>9999</v>
+        <v>2017</v>
       </c>
       <c r="D22" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E22" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="H22" s="2">
+        <v>27</v>
+      </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -1360,53 +1368,47 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C23" s="3">
-        <v>9999</v>
+        <v>2020</v>
       </c>
       <c r="D23" s="2">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E23" s="2">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="2">
-        <v>12</v>
-      </c>
-      <c r="I23" s="2">
-        <v>13</v>
-      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C24" s="3">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="D24" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E24" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="2">
-        <v>27</v>
-      </c>
+      <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -1414,24 +1416,24 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="1">
-        <v>2013</v>
+        <v>53</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2022</v>
       </c>
       <c r="D25" s="2">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E25" s="2">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -1440,19 +1442,19 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="1">
+        <v>54</v>
+      </c>
+      <c r="C26" s="3">
         <v>9999</v>
       </c>
       <c r="D26" s="2">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E26" s="2">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1464,23 +1466,25 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="1">
-        <v>9999</v>
+        <v>56</v>
+      </c>
+      <c r="C27" s="3">
+        <v>2023</v>
       </c>
       <c r="D27" s="2">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="E27" s="2">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="H27" s="2">
+        <v>29</v>
+      </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
@@ -1488,19 +1492,19 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C28" s="3">
         <v>2020</v>
       </c>
       <c r="D28" s="2">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E28" s="2">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -1512,49 +1516,45 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="C29" s="3">
-        <v>2014</v>
+        <v>2023</v>
       </c>
       <c r="D29" s="2">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="E29" s="2">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2">
-        <v>14</v>
-      </c>
-      <c r="I29" s="2">
-        <v>15</v>
-      </c>
-      <c r="J29" s="2">
-        <v>16</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="C30" s="3">
-        <v>9999</v>
+        <v>2024</v>
       </c>
       <c r="D30" s="2">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="E30" s="2">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -1566,19 +1566,19 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="C31" s="3">
-        <v>9999</v>
+        <v>2025</v>
       </c>
       <c r="D31" s="2">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E31" s="2">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -1590,25 +1590,23 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="C32" s="3">
         <v>9999</v>
       </c>
       <c r="D32" s="2">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E32" s="2">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="2">
-        <v>11</v>
-      </c>
+      <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>

</xml_diff>

<commit_message>
Empty values in column 1 break read_excel_data, replaced null with NONE. Gonna try and fix that now
</commit_message>
<xml_diff>
--- a/family-tree-data.xlsx
+++ b/family-tree-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASHil\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASHil\PycharmProjects\Family-Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2B7A33-0C7C-4FE4-8B28-4777F2B987A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1ECC166-6C78-4AD9-9F2B-F3201F4EF2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="198">
   <si>
     <t>Class Year</t>
   </si>
@@ -627,6 +627,9 @@
   </si>
   <si>
     <t>Zach</t>
+  </si>
+  <si>
+    <t>NONE</t>
   </si>
 </sst>
 </file>
@@ -1131,8 +1134,8 @@
   <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I39" sqref="I39"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1380,7 +1383,9 @@
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
@@ -1464,7 +1469,9 @@
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1486,7 +1493,9 @@
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
@@ -1660,7 +1669,9 @@
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="B21" s="1" t="s">
         <v>44</v>
       </c>
@@ -1780,7 +1791,9 @@
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="B26" s="1" t="s">
         <v>53</v>
       </c>
@@ -1924,7 +1937,9 @@
       <c r="L31" s="2"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="B32" s="1" t="s">
         <v>63</v>
       </c>
@@ -2756,7 +2771,9 @@
       <c r="L64" s="2"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A65" s="1"/>
+      <c r="A65" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="B65" s="1" t="s">
         <v>120</v>
       </c>
@@ -2828,7 +2845,9 @@
       <c r="L67" s="2"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A68" s="1"/>
+      <c r="A68" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="B68" s="1" t="s">
         <v>124</v>
       </c>
@@ -2878,7 +2897,9 @@
       <c r="L69" s="2"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A70" s="1"/>
+      <c r="A70" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="B70" s="1" t="s">
         <v>127</v>
       </c>
@@ -2896,7 +2917,9 @@
       <c r="L70" s="2"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A71" s="1"/>
+      <c r="A71" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="B71" s="1" t="s">
         <v>128</v>
       </c>

</xml_diff>

<commit_message>
search for and replace None values
</commit_message>
<xml_diff>
--- a/family-tree-data.xlsx
+++ b/family-tree-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASHil\PycharmProjects\Family-Tree\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Family-Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206E5717-024F-44EE-A0BF-776989DC55F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84F2236-57AA-466E-BC23-BA30D007D0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5250" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="231">
   <si>
     <t>Class Year</t>
   </si>
@@ -702,9 +702,6 @@
   </si>
   <si>
     <t>Love</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Jose</t>
@@ -1236,19 +1233,19 @@
   <dimension ref="A1:L350"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F133" sqref="F133"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="12" customWidth="1"/>
-    <col min="5" max="11" width="17.6640625" customWidth="1"/>
+    <col min="1" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="12" customWidth="1"/>
+    <col min="5" max="11" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
@@ -1286,7 +1283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1308,7 +1305,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1342,7 +1339,7 @@
       </c>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1366,7 +1363,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1390,7 +1387,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -1412,7 +1409,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1434,7 +1431,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -1460,7 +1457,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -1484,7 +1481,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>194</v>
       </c>
@@ -1510,7 +1507,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1540,7 +1537,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -1570,7 +1567,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>194</v>
       </c>
@@ -1594,7 +1591,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>205</v>
       </c>
@@ -1618,7 +1615,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
@@ -1644,7 +1641,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
@@ -1676,7 +1673,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
@@ -1698,7 +1695,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
@@ -1726,7 +1723,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1752,7 +1749,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
@@ -1780,7 +1777,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>194</v>
       </c>
@@ -1802,7 +1799,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
@@ -1828,7 +1825,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
@@ -1852,7 +1849,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>49</v>
       </c>
@@ -1876,7 +1873,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
@@ -1902,7 +1899,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>194</v>
       </c>
@@ -1924,7 +1921,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>54</v>
       </c>
@@ -1950,7 +1947,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>56</v>
       </c>
@@ -1974,7 +1971,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>58</v>
       </c>
@@ -2000,7 +1997,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>60</v>
       </c>
@@ -2024,7 +2021,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
@@ -2048,7 +2045,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>194</v>
       </c>
@@ -2070,7 +2067,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
@@ -2090,7 +2087,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
@@ -2114,7 +2111,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
@@ -2140,7 +2137,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>70</v>
       </c>
@@ -2164,7 +2161,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
@@ -2188,7 +2185,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>75</v>
       </c>
@@ -2210,7 +2207,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>22</v>
       </c>
@@ -2232,7 +2229,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>78</v>
       </c>
@@ -2266,7 +2263,7 @@
       </c>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>80</v>
       </c>
@@ -2294,7 +2291,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>12</v>
       </c>
@@ -2320,7 +2317,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>83</v>
       </c>
@@ -2348,7 +2345,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>85</v>
       </c>
@@ -2376,7 +2373,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>89</v>
       </c>
@@ -2402,7 +2399,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>16</v>
       </c>
@@ -2428,7 +2425,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>90</v>
       </c>
@@ -2454,7 +2451,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>92</v>
       </c>
@@ -2480,7 +2477,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>38</v>
       </c>
@@ -2504,7 +2501,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>95</v>
       </c>
@@ -2528,7 +2525,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>97</v>
       </c>
@@ -2552,7 +2549,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>99</v>
       </c>
@@ -2578,7 +2575,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>101</v>
       </c>
@@ -2602,7 +2599,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>103</v>
       </c>
@@ -2626,7 +2623,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>105</v>
       </c>
@@ -2652,7 +2649,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>107</v>
       </c>
@@ -2682,7 +2679,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>109</v>
       </c>
@@ -2708,7 +2705,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>111</v>
       </c>
@@ -2732,7 +2729,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>73</v>
       </c>
@@ -2756,7 +2753,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>113</v>
       </c>
@@ -2780,7 +2777,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>103</v>
       </c>
@@ -2808,7 +2805,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>38</v>
       </c>
@@ -2830,7 +2827,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>117</v>
       </c>
@@ -2856,7 +2853,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>47</v>
       </c>
@@ -2880,7 +2877,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>194</v>
       </c>
@@ -2900,7 +2897,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>190</v>
       </c>
@@ -2928,7 +2925,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>122</v>
       </c>
@@ -2954,7 +2951,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>194</v>
       </c>
@@ -2976,7 +2973,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>125</v>
       </c>
@@ -3006,7 +3003,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>194</v>
       </c>
@@ -3026,7 +3023,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>194</v>
       </c>
@@ -3046,7 +3043,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>129</v>
       </c>
@@ -3072,7 +3069,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>131</v>
       </c>
@@ -3094,7 +3091,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>95</v>
       </c>
@@ -3120,7 +3117,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>134</v>
       </c>
@@ -3144,7 +3141,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>26</v>
       </c>
@@ -3168,7 +3165,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>89</v>
       </c>
@@ -3192,7 +3189,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>26</v>
       </c>
@@ -3216,7 +3213,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>139</v>
       </c>
@@ -3240,7 +3237,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>191</v>
       </c>
@@ -3262,7 +3259,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>142</v>
       </c>
@@ -3290,7 +3287,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>158</v>
       </c>
@@ -3316,7 +3313,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>145</v>
       </c>
@@ -3346,7 +3343,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>51</v>
       </c>
@@ -3370,7 +3367,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>147</v>
       </c>
@@ -3398,7 +3395,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>149</v>
       </c>
@@ -3424,7 +3421,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>151</v>
       </c>
@@ -3456,7 +3453,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>153</v>
       </c>
@@ -3480,7 +3477,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>80</v>
       </c>
@@ -3506,7 +3503,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>156</v>
       </c>
@@ -3530,7 +3527,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>159</v>
       </c>
@@ -3554,7 +3551,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>161</v>
       </c>
@@ -3582,7 +3579,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>163</v>
       </c>
@@ -3606,7 +3603,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>164</v>
       </c>
@@ -3630,7 +3627,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>35</v>
       </c>
@@ -3654,7 +3651,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>167</v>
       </c>
@@ -3678,7 +3675,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>164</v>
       </c>
@@ -3702,7 +3699,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>170</v>
       </c>
@@ -3726,7 +3723,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>73</v>
       </c>
@@ -3750,7 +3747,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>175</v>
       </c>
@@ -3774,7 +3771,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>172</v>
       </c>
@@ -3798,7 +3795,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>173</v>
       </c>
@@ -3822,7 +3819,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>121</v>
       </c>
@@ -3850,7 +3847,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>177</v>
       </c>
@@ -3876,7 +3873,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>153</v>
       </c>
@@ -3900,7 +3897,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>180</v>
       </c>
@@ -3924,7 +3921,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>114</v>
       </c>
@@ -3954,7 +3951,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>147</v>
       </c>
@@ -3978,7 +3975,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>183</v>
       </c>
@@ -4004,7 +4001,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>186</v>
       </c>
@@ -4028,7 +4025,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>188</v>
       </c>
@@ -4052,7 +4049,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>192</v>
       </c>
@@ -4074,7 +4071,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>163</v>
       </c>
@@ -4098,7 +4095,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>195</v>
       </c>
@@ -4120,7 +4117,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>15</v>
       </c>
@@ -4148,7 +4145,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>15</v>
       </c>
@@ -4172,7 +4169,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>156</v>
       </c>
@@ -4194,7 +4191,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>199</v>
       </c>
@@ -4216,7 +4213,7 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>201</v>
       </c>
@@ -4240,7 +4237,7 @@
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>194</v>
       </c>
@@ -4262,7 +4259,7 @@
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>16</v>
       </c>
@@ -4286,7 +4283,7 @@
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>194</v>
       </c>
@@ -4308,7 +4305,7 @@
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>207</v>
       </c>
@@ -4332,7 +4329,7 @@
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>209</v>
       </c>
@@ -4358,7 +4355,7 @@
       <c r="K124" s="2"/>
       <c r="L124" s="2"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>211</v>
       </c>
@@ -4384,7 +4381,7 @@
       <c r="K125" s="2"/>
       <c r="L125" s="2"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>16</v>
       </c>
@@ -4408,7 +4405,7 @@
       <c r="K126" s="2"/>
       <c r="L126" s="2"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>214</v>
       </c>
@@ -4436,7 +4433,7 @@
       <c r="K127" s="2"/>
       <c r="L127" s="2"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>216</v>
       </c>
@@ -4458,7 +4455,7 @@
       <c r="K128" s="2"/>
       <c r="L128" s="2"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>172</v>
       </c>
@@ -4480,7 +4477,7 @@
       <c r="K129" s="2"/>
       <c r="L129" s="2"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>47</v>
       </c>
@@ -4502,7 +4499,7 @@
       <c r="K130" s="2"/>
       <c r="L130" s="2"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>35</v>
       </c>
@@ -4524,7 +4521,7 @@
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>177</v>
       </c>
@@ -4546,16 +4543,14 @@
       <c r="K132" s="2"/>
       <c r="L132" s="2"/>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C133" s="3" t="s">
-        <v>222</v>
-      </c>
+      <c r="C133" s="3"/>
       <c r="D133" s="2">
         <v>132</v>
       </c>
@@ -4568,9 +4563,9 @@
       <c r="K133" s="2"/>
       <c r="L133" s="2"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>200</v>
@@ -4590,7 +4585,7 @@
       <c r="K134" s="2"/>
       <c r="L134" s="2"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>16</v>
       </c>
@@ -4612,12 +4607,12 @@
       <c r="K135" s="2"/>
       <c r="L135" s="2"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C136" s="3">
         <v>2023</v>
@@ -4634,12 +4629,12 @@
       <c r="K136" s="2"/>
       <c r="L136" s="2"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B137" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="C137" s="3">
         <v>2022</v>
@@ -4656,12 +4651,12 @@
       <c r="K137" s="2"/>
       <c r="L137" s="2"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C138" s="3">
         <v>2022</v>
@@ -4678,12 +4673,12 @@
       <c r="K138" s="2"/>
       <c r="L138" s="2"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C139" s="3">
         <v>2020</v>
@@ -4700,12 +4695,12 @@
       <c r="K139" s="2"/>
       <c r="L139" s="2"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C140" s="3">
         <v>2025</v>
@@ -4722,12 +4717,12 @@
       <c r="K140" s="2"/>
       <c r="L140" s="2"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="C141" s="3">
         <v>2025</v>
@@ -4744,7 +4739,7 @@
       <c r="K141" s="2"/>
       <c r="L141" s="2"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="3"/>
@@ -4760,7 +4755,7 @@
       <c r="K142" s="2"/>
       <c r="L142" s="2"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="3"/>
@@ -4776,7 +4771,7 @@
       <c r="K143" s="2"/>
       <c r="L143" s="2"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="3"/>
@@ -4792,7 +4787,7 @@
       <c r="K144" s="2"/>
       <c r="L144" s="2"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="3"/>
@@ -4808,7 +4803,7 @@
       <c r="K145" s="2"/>
       <c r="L145" s="2"/>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="3"/>
@@ -4824,7 +4819,7 @@
       <c r="K146" s="2"/>
       <c r="L146" s="2"/>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="3"/>
@@ -4840,7 +4835,7 @@
       <c r="K147" s="2"/>
       <c r="L147" s="2"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="3"/>
@@ -4856,7 +4851,7 @@
       <c r="K148" s="2"/>
       <c r="L148" s="2"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="3"/>
@@ -4872,7 +4867,7 @@
       <c r="K149" s="2"/>
       <c r="L149" s="2"/>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="3"/>
@@ -4888,7 +4883,7 @@
       <c r="K150" s="2"/>
       <c r="L150" s="2"/>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="3"/>
@@ -4904,7 +4899,7 @@
       <c r="K151" s="2"/>
       <c r="L151" s="2"/>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="3"/>
@@ -4918,7 +4913,7 @@
       <c r="K152" s="2"/>
       <c r="L152" s="2"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="3"/>
@@ -4932,7 +4927,7 @@
       <c r="K153" s="2"/>
       <c r="L153" s="2"/>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="3"/>
@@ -4946,7 +4941,7 @@
       <c r="K154" s="2"/>
       <c r="L154" s="2"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="3"/>
@@ -4960,7 +4955,7 @@
       <c r="K155" s="2"/>
       <c r="L155" s="2"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="3"/>
@@ -4974,7 +4969,7 @@
       <c r="K156" s="2"/>
       <c r="L156" s="2"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="3"/>
@@ -4988,7 +4983,7 @@
       <c r="K157" s="2"/>
       <c r="L157" s="2"/>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="3"/>
@@ -5002,7 +4997,7 @@
       <c r="K158" s="2"/>
       <c r="L158" s="2"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="3"/>
@@ -5016,7 +5011,7 @@
       <c r="K159" s="2"/>
       <c r="L159" s="2"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="3"/>
@@ -5030,7 +5025,7 @@
       <c r="K160" s="2"/>
       <c r="L160" s="2"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="3"/>
@@ -5044,7 +5039,7 @@
       <c r="K161" s="2"/>
       <c r="L161" s="2"/>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="3"/>
@@ -5058,7 +5053,7 @@
       <c r="K162" s="2"/>
       <c r="L162" s="2"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="3"/>
@@ -5072,7 +5067,7 @@
       <c r="K163" s="2"/>
       <c r="L163" s="2"/>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="3"/>
@@ -5086,7 +5081,7 @@
       <c r="K164" s="2"/>
       <c r="L164" s="2"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="3"/>
@@ -5100,7 +5095,7 @@
       <c r="K165" s="2"/>
       <c r="L165" s="2"/>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="3"/>
@@ -5114,7 +5109,7 @@
       <c r="K166" s="2"/>
       <c r="L166" s="2"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="3"/>
@@ -5128,7 +5123,7 @@
       <c r="K167" s="2"/>
       <c r="L167" s="2"/>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="3"/>
@@ -5142,7 +5137,7 @@
       <c r="K168" s="2"/>
       <c r="L168" s="2"/>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="3"/>
@@ -5156,7 +5151,7 @@
       <c r="K169" s="2"/>
       <c r="L169" s="2"/>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="3"/>
@@ -5170,7 +5165,7 @@
       <c r="K170" s="2"/>
       <c r="L170" s="2"/>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="3"/>
@@ -5184,7 +5179,7 @@
       <c r="K171" s="2"/>
       <c r="L171" s="2"/>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="3"/>
@@ -5198,7 +5193,7 @@
       <c r="K172" s="2"/>
       <c r="L172" s="2"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="3"/>
@@ -5212,7 +5207,7 @@
       <c r="K173" s="2"/>
       <c r="L173" s="2"/>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="3"/>
@@ -5226,7 +5221,7 @@
       <c r="K174" s="2"/>
       <c r="L174" s="2"/>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="3"/>
@@ -5240,7 +5235,7 @@
       <c r="K175" s="2"/>
       <c r="L175" s="2"/>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="3"/>
@@ -5254,7 +5249,7 @@
       <c r="K176" s="2"/>
       <c r="L176" s="2"/>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="3"/>
@@ -5268,7 +5263,7 @@
       <c r="K177" s="2"/>
       <c r="L177" s="2"/>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="3"/>
@@ -5282,7 +5277,7 @@
       <c r="K178" s="2"/>
       <c r="L178" s="2"/>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="3"/>
@@ -5296,7 +5291,7 @@
       <c r="K179" s="2"/>
       <c r="L179" s="2"/>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="3"/>
@@ -5310,7 +5305,7 @@
       <c r="K180" s="2"/>
       <c r="L180" s="2"/>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="3"/>
@@ -5324,7 +5319,7 @@
       <c r="K181" s="2"/>
       <c r="L181" s="2"/>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="3"/>
@@ -5338,7 +5333,7 @@
       <c r="K182" s="2"/>
       <c r="L182" s="2"/>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="3"/>
@@ -5352,7 +5347,7 @@
       <c r="K183" s="2"/>
       <c r="L183" s="2"/>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="3"/>
@@ -5366,7 +5361,7 @@
       <c r="K184" s="2"/>
       <c r="L184" s="2"/>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="3"/>
@@ -5380,7 +5375,7 @@
       <c r="K185" s="2"/>
       <c r="L185" s="2"/>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="3"/>
@@ -5394,7 +5389,7 @@
       <c r="K186" s="2"/>
       <c r="L186" s="2"/>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="3"/>
@@ -5408,7 +5403,7 @@
       <c r="K187" s="2"/>
       <c r="L187" s="2"/>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="3"/>
@@ -5422,7 +5417,7 @@
       <c r="K188" s="2"/>
       <c r="L188" s="2"/>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="3"/>
@@ -5436,7 +5431,7 @@
       <c r="K189" s="2"/>
       <c r="L189" s="2"/>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="3"/>
@@ -5450,7 +5445,7 @@
       <c r="K190" s="2"/>
       <c r="L190" s="2"/>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="3"/>
@@ -5464,7 +5459,7 @@
       <c r="K191" s="2"/>
       <c r="L191" s="2"/>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="3"/>
@@ -5478,7 +5473,7 @@
       <c r="K192" s="2"/>
       <c r="L192" s="2"/>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="3"/>
@@ -5492,7 +5487,7 @@
       <c r="K193" s="2"/>
       <c r="L193" s="2"/>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="3"/>
@@ -5506,7 +5501,7 @@
       <c r="K194" s="2"/>
       <c r="L194" s="2"/>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="3"/>
@@ -5520,7 +5515,7 @@
       <c r="K195" s="2"/>
       <c r="L195" s="2"/>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="3"/>
@@ -5534,7 +5529,7 @@
       <c r="K196" s="2"/>
       <c r="L196" s="2"/>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="3"/>
@@ -5548,7 +5543,7 @@
       <c r="K197" s="2"/>
       <c r="L197" s="2"/>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="3"/>
@@ -5562,7 +5557,7 @@
       <c r="K198" s="2"/>
       <c r="L198" s="2"/>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="3"/>
@@ -5576,7 +5571,7 @@
       <c r="K199" s="2"/>
       <c r="L199" s="2"/>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="3"/>
@@ -5590,7 +5585,7 @@
       <c r="K200" s="2"/>
       <c r="L200" s="2"/>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="3"/>
@@ -5604,7 +5599,7 @@
       <c r="K201" s="2"/>
       <c r="L201" s="2"/>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="3"/>
@@ -5618,7 +5613,7 @@
       <c r="K202" s="2"/>
       <c r="L202" s="2"/>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="3"/>
@@ -5632,7 +5627,7 @@
       <c r="K203" s="2"/>
       <c r="L203" s="2"/>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="3"/>
@@ -5646,7 +5641,7 @@
       <c r="K204" s="2"/>
       <c r="L204" s="2"/>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="3"/>
@@ -5660,7 +5655,7 @@
       <c r="K205" s="2"/>
       <c r="L205" s="2"/>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="3"/>
@@ -5674,7 +5669,7 @@
       <c r="K206" s="2"/>
       <c r="L206" s="2"/>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="3"/>
@@ -5688,7 +5683,7 @@
       <c r="K207" s="2"/>
       <c r="L207" s="2"/>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="3"/>
@@ -5702,7 +5697,7 @@
       <c r="K208" s="2"/>
       <c r="L208" s="2"/>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="3"/>
@@ -5716,7 +5711,7 @@
       <c r="K209" s="2"/>
       <c r="L209" s="2"/>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="3"/>
@@ -5730,7 +5725,7 @@
       <c r="K210" s="2"/>
       <c r="L210" s="2"/>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
       <c r="C211" s="3"/>
@@ -5744,7 +5739,7 @@
       <c r="K211" s="2"/>
       <c r="L211" s="2"/>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
       <c r="B212" s="1"/>
       <c r="C212" s="3"/>
@@ -5758,7 +5753,7 @@
       <c r="K212" s="2"/>
       <c r="L212" s="2"/>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A213" s="1"/>
       <c r="B213" s="1"/>
       <c r="C213" s="3"/>
@@ -5772,7 +5767,7 @@
       <c r="K213" s="2"/>
       <c r="L213" s="2"/>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A214" s="1"/>
       <c r="B214" s="1"/>
       <c r="C214" s="3"/>
@@ -5786,7 +5781,7 @@
       <c r="K214" s="2"/>
       <c r="L214" s="2"/>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A215" s="1"/>
       <c r="B215" s="1"/>
       <c r="C215" s="3"/>
@@ -5800,7 +5795,7 @@
       <c r="K215" s="2"/>
       <c r="L215" s="2"/>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A216" s="1"/>
       <c r="B216" s="1"/>
       <c r="C216" s="3"/>
@@ -5814,7 +5809,7 @@
       <c r="K216" s="2"/>
       <c r="L216" s="2"/>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A217" s="1"/>
       <c r="B217" s="1"/>
       <c r="C217" s="3"/>
@@ -5828,7 +5823,7 @@
       <c r="K217" s="2"/>
       <c r="L217" s="2"/>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A218" s="1"/>
       <c r="B218" s="1"/>
       <c r="C218" s="3"/>
@@ -5842,7 +5837,7 @@
       <c r="K218" s="2"/>
       <c r="L218" s="2"/>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A219" s="1"/>
       <c r="B219" s="1"/>
       <c r="C219" s="3"/>
@@ -5856,7 +5851,7 @@
       <c r="K219" s="2"/>
       <c r="L219" s="2"/>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A220" s="1"/>
       <c r="B220" s="1"/>
       <c r="C220" s="3"/>
@@ -5870,7 +5865,7 @@
       <c r="K220" s="2"/>
       <c r="L220" s="2"/>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A221" s="1"/>
       <c r="B221" s="1"/>
       <c r="C221" s="3"/>
@@ -5884,7 +5879,7 @@
       <c r="K221" s="2"/>
       <c r="L221" s="2"/>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A222" s="1"/>
       <c r="B222" s="1"/>
       <c r="C222" s="3"/>
@@ -5898,7 +5893,7 @@
       <c r="K222" s="2"/>
       <c r="L222" s="2"/>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
       <c r="B223" s="1"/>
       <c r="C223" s="3"/>
@@ -5912,7 +5907,7 @@
       <c r="K223" s="2"/>
       <c r="L223" s="2"/>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
       <c r="B224" s="1"/>
       <c r="C224" s="3"/>
@@ -5926,7 +5921,7 @@
       <c r="K224" s="2"/>
       <c r="L224" s="2"/>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A225" s="1"/>
       <c r="B225" s="1"/>
       <c r="C225" s="3"/>
@@ -5940,7 +5935,7 @@
       <c r="K225" s="2"/>
       <c r="L225" s="2"/>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A226" s="1"/>
       <c r="B226" s="1"/>
       <c r="C226" s="3"/>
@@ -5954,7 +5949,7 @@
       <c r="K226" s="2"/>
       <c r="L226" s="2"/>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A227" s="1"/>
       <c r="B227" s="1"/>
       <c r="C227" s="3"/>
@@ -5968,7 +5963,7 @@
       <c r="K227" s="2"/>
       <c r="L227" s="2"/>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A228" s="1"/>
       <c r="B228" s="1"/>
       <c r="C228" s="3"/>
@@ -5982,7 +5977,7 @@
       <c r="K228" s="2"/>
       <c r="L228" s="2"/>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A229" s="1"/>
       <c r="B229" s="1"/>
       <c r="C229" s="3"/>
@@ -5996,7 +5991,7 @@
       <c r="K229" s="2"/>
       <c r="L229" s="2"/>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A230" s="1"/>
       <c r="B230" s="1"/>
       <c r="C230" s="3"/>
@@ -6010,7 +6005,7 @@
       <c r="K230" s="2"/>
       <c r="L230" s="2"/>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A231" s="1"/>
       <c r="B231" s="1"/>
       <c r="C231" s="3"/>
@@ -6024,7 +6019,7 @@
       <c r="K231" s="2"/>
       <c r="L231" s="2"/>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A232" s="1"/>
       <c r="B232" s="1"/>
       <c r="C232" s="3"/>
@@ -6038,7 +6033,7 @@
       <c r="K232" s="2"/>
       <c r="L232" s="2"/>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A233" s="1"/>
       <c r="B233" s="1"/>
       <c r="C233" s="3"/>
@@ -6052,7 +6047,7 @@
       <c r="K233" s="2"/>
       <c r="L233" s="2"/>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A234" s="1"/>
       <c r="B234" s="1"/>
       <c r="C234" s="3"/>
@@ -6066,7 +6061,7 @@
       <c r="K234" s="2"/>
       <c r="L234" s="2"/>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A235" s="1"/>
       <c r="B235" s="1"/>
       <c r="C235" s="3"/>
@@ -6080,7 +6075,7 @@
       <c r="K235" s="2"/>
       <c r="L235" s="2"/>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A236" s="1"/>
       <c r="B236" s="1"/>
       <c r="C236" s="3"/>
@@ -6094,7 +6089,7 @@
       <c r="K236" s="2"/>
       <c r="L236" s="2"/>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A237" s="1"/>
       <c r="B237" s="1"/>
       <c r="C237" s="3"/>
@@ -6108,7 +6103,7 @@
       <c r="K237" s="2"/>
       <c r="L237" s="2"/>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A238" s="1"/>
       <c r="B238" s="1"/>
       <c r="C238" s="3"/>
@@ -6122,7 +6117,7 @@
       <c r="K238" s="2"/>
       <c r="L238" s="2"/>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A239" s="1"/>
       <c r="B239" s="1"/>
       <c r="C239" s="3"/>
@@ -6136,7 +6131,7 @@
       <c r="K239" s="2"/>
       <c r="L239" s="2"/>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A240" s="1"/>
       <c r="B240" s="1"/>
       <c r="C240" s="3"/>
@@ -6150,7 +6145,7 @@
       <c r="K240" s="2"/>
       <c r="L240" s="2"/>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A241" s="1"/>
       <c r="B241" s="1"/>
       <c r="C241" s="3"/>
@@ -6164,7 +6159,7 @@
       <c r="K241" s="2"/>
       <c r="L241" s="2"/>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A242" s="1"/>
       <c r="B242" s="1"/>
       <c r="C242" s="3"/>
@@ -6178,7 +6173,7 @@
       <c r="K242" s="2"/>
       <c r="L242" s="2"/>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A243" s="1"/>
       <c r="B243" s="1"/>
       <c r="C243" s="3"/>
@@ -6192,7 +6187,7 @@
       <c r="K243" s="2"/>
       <c r="L243" s="2"/>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A244" s="1"/>
       <c r="B244" s="1"/>
       <c r="C244" s="3"/>
@@ -6206,7 +6201,7 @@
       <c r="K244" s="2"/>
       <c r="L244" s="2"/>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A245" s="1"/>
       <c r="B245" s="1"/>
       <c r="C245" s="3"/>
@@ -6220,7 +6215,7 @@
       <c r="K245" s="2"/>
       <c r="L245" s="2"/>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A246" s="1"/>
       <c r="B246" s="1"/>
       <c r="C246" s="3"/>
@@ -6234,7 +6229,7 @@
       <c r="K246" s="2"/>
       <c r="L246" s="2"/>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A247" s="1"/>
       <c r="B247" s="1"/>
       <c r="C247" s="3"/>
@@ -6248,7 +6243,7 @@
       <c r="K247" s="2"/>
       <c r="L247" s="2"/>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A248" s="1"/>
       <c r="B248" s="1"/>
       <c r="C248" s="3"/>
@@ -6262,7 +6257,7 @@
       <c r="K248" s="2"/>
       <c r="L248" s="2"/>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A249" s="1"/>
       <c r="B249" s="1"/>
       <c r="C249" s="3"/>
@@ -6276,7 +6271,7 @@
       <c r="K249" s="2"/>
       <c r="L249" s="2"/>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A250" s="1"/>
       <c r="B250" s="1"/>
       <c r="C250" s="3"/>
@@ -6290,7 +6285,7 @@
       <c r="K250" s="2"/>
       <c r="L250" s="2"/>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A251" s="1"/>
       <c r="B251" s="1"/>
       <c r="C251" s="3"/>
@@ -6304,7 +6299,7 @@
       <c r="K251" s="2"/>
       <c r="L251" s="2"/>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A252" s="1"/>
       <c r="B252" s="1"/>
       <c r="C252" s="3"/>
@@ -6318,7 +6313,7 @@
       <c r="K252" s="2"/>
       <c r="L252" s="2"/>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A253" s="1"/>
       <c r="B253" s="1"/>
       <c r="C253" s="3"/>
@@ -6332,7 +6327,7 @@
       <c r="K253" s="2"/>
       <c r="L253" s="2"/>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A254" s="1"/>
       <c r="B254" s="1"/>
       <c r="C254" s="3"/>
@@ -6346,7 +6341,7 @@
       <c r="K254" s="2"/>
       <c r="L254" s="2"/>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A255" s="1"/>
       <c r="B255" s="1"/>
       <c r="C255" s="3"/>
@@ -6360,7 +6355,7 @@
       <c r="K255" s="2"/>
       <c r="L255" s="2"/>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A256" s="1"/>
       <c r="B256" s="1"/>
       <c r="C256" s="3"/>
@@ -6374,7 +6369,7 @@
       <c r="K256" s="2"/>
       <c r="L256" s="2"/>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A257" s="1"/>
       <c r="B257" s="1"/>
       <c r="C257" s="3"/>
@@ -6388,7 +6383,7 @@
       <c r="K257" s="2"/>
       <c r="L257" s="2"/>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A258" s="1"/>
       <c r="B258" s="1"/>
       <c r="C258" s="3"/>
@@ -6402,7 +6397,7 @@
       <c r="K258" s="2"/>
       <c r="L258" s="2"/>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A259" s="1"/>
       <c r="B259" s="1"/>
       <c r="C259" s="3"/>
@@ -6416,7 +6411,7 @@
       <c r="K259" s="2"/>
       <c r="L259" s="2"/>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A260" s="1"/>
       <c r="B260" s="1"/>
       <c r="C260" s="3"/>
@@ -6430,7 +6425,7 @@
       <c r="K260" s="2"/>
       <c r="L260" s="2"/>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A261" s="1"/>
       <c r="B261" s="1"/>
       <c r="C261" s="3"/>
@@ -6444,7 +6439,7 @@
       <c r="K261" s="2"/>
       <c r="L261" s="2"/>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A262" s="1"/>
       <c r="B262" s="1"/>
       <c r="C262" s="3"/>
@@ -6458,7 +6453,7 @@
       <c r="K262" s="2"/>
       <c r="L262" s="2"/>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A263" s="1"/>
       <c r="B263" s="1"/>
       <c r="C263" s="3"/>
@@ -6472,7 +6467,7 @@
       <c r="K263" s="2"/>
       <c r="L263" s="2"/>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A264" s="1"/>
       <c r="B264" s="1"/>
       <c r="C264" s="3"/>
@@ -6486,7 +6481,7 @@
       <c r="K264" s="2"/>
       <c r="L264" s="2"/>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A265" s="1"/>
       <c r="B265" s="1"/>
       <c r="C265" s="3"/>
@@ -6500,7 +6495,7 @@
       <c r="K265" s="2"/>
       <c r="L265" s="2"/>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A266" s="1"/>
       <c r="B266" s="1"/>
       <c r="C266" s="3"/>
@@ -6514,7 +6509,7 @@
       <c r="K266" s="2"/>
       <c r="L266" s="2"/>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A267" s="1"/>
       <c r="B267" s="1"/>
       <c r="C267" s="3"/>
@@ -6528,7 +6523,7 @@
       <c r="K267" s="2"/>
       <c r="L267" s="2"/>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A268" s="1"/>
       <c r="B268" s="1"/>
       <c r="C268" s="3"/>
@@ -6542,7 +6537,7 @@
       <c r="K268" s="2"/>
       <c r="L268" s="2"/>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A269" s="1"/>
       <c r="B269" s="1"/>
       <c r="C269" s="3"/>
@@ -6556,7 +6551,7 @@
       <c r="K269" s="2"/>
       <c r="L269" s="2"/>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A270" s="1"/>
       <c r="B270" s="1"/>
       <c r="C270" s="3"/>
@@ -6570,7 +6565,7 @@
       <c r="K270" s="2"/>
       <c r="L270" s="2"/>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A271" s="1"/>
       <c r="B271" s="1"/>
       <c r="C271" s="3"/>
@@ -6584,7 +6579,7 @@
       <c r="K271" s="2"/>
       <c r="L271" s="2"/>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A272" s="1"/>
       <c r="B272" s="1"/>
       <c r="C272" s="3"/>
@@ -6598,7 +6593,7 @@
       <c r="K272" s="2"/>
       <c r="L272" s="2"/>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A273" s="1"/>
       <c r="B273" s="1"/>
       <c r="C273" s="3"/>
@@ -6612,7 +6607,7 @@
       <c r="K273" s="2"/>
       <c r="L273" s="2"/>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A274" s="1"/>
       <c r="B274" s="1"/>
       <c r="C274" s="3"/>
@@ -6626,7 +6621,7 @@
       <c r="K274" s="2"/>
       <c r="L274" s="2"/>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A275" s="1"/>
       <c r="B275" s="1"/>
       <c r="C275" s="3"/>
@@ -6640,7 +6635,7 @@
       <c r="K275" s="2"/>
       <c r="L275" s="2"/>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A276" s="1"/>
       <c r="B276" s="1"/>
       <c r="C276" s="3"/>
@@ -6654,7 +6649,7 @@
       <c r="K276" s="2"/>
       <c r="L276" s="2"/>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A277" s="1"/>
       <c r="B277" s="1"/>
       <c r="C277" s="3"/>
@@ -6668,7 +6663,7 @@
       <c r="K277" s="2"/>
       <c r="L277" s="2"/>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A278" s="1"/>
       <c r="B278" s="1"/>
       <c r="C278" s="3"/>
@@ -6682,7 +6677,7 @@
       <c r="K278" s="2"/>
       <c r="L278" s="2"/>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A279" s="1"/>
       <c r="B279" s="1"/>
       <c r="C279" s="3"/>
@@ -6696,7 +6691,7 @@
       <c r="K279" s="2"/>
       <c r="L279" s="2"/>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A280" s="1"/>
       <c r="B280" s="1"/>
       <c r="C280" s="3"/>
@@ -6710,7 +6705,7 @@
       <c r="K280" s="2"/>
       <c r="L280" s="2"/>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A281" s="1"/>
       <c r="B281" s="1"/>
       <c r="C281" s="3"/>
@@ -6724,7 +6719,7 @@
       <c r="K281" s="2"/>
       <c r="L281" s="2"/>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A282" s="1"/>
       <c r="B282" s="1"/>
       <c r="C282" s="3"/>
@@ -6738,7 +6733,7 @@
       <c r="K282" s="2"/>
       <c r="L282" s="2"/>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A283" s="1"/>
       <c r="B283" s="1"/>
       <c r="C283" s="3"/>
@@ -6752,7 +6747,7 @@
       <c r="K283" s="2"/>
       <c r="L283" s="2"/>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A284" s="1"/>
       <c r="B284" s="1"/>
       <c r="C284" s="3"/>
@@ -6766,7 +6761,7 @@
       <c r="K284" s="2"/>
       <c r="L284" s="2"/>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A285" s="1"/>
       <c r="B285" s="1"/>
       <c r="C285" s="3"/>
@@ -6780,7 +6775,7 @@
       <c r="K285" s="2"/>
       <c r="L285" s="2"/>
     </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A286" s="1"/>
       <c r="B286" s="1"/>
       <c r="C286" s="3"/>
@@ -6794,7 +6789,7 @@
       <c r="K286" s="2"/>
       <c r="L286" s="2"/>
     </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A287" s="1"/>
       <c r="B287" s="1"/>
       <c r="C287" s="3"/>
@@ -6808,7 +6803,7 @@
       <c r="K287" s="2"/>
       <c r="L287" s="2"/>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A288" s="1"/>
       <c r="B288" s="1"/>
       <c r="C288" s="3"/>
@@ -6822,7 +6817,7 @@
       <c r="K288" s="2"/>
       <c r="L288" s="2"/>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A289" s="1"/>
       <c r="B289" s="1"/>
       <c r="C289" s="3"/>
@@ -6836,7 +6831,7 @@
       <c r="K289" s="2"/>
       <c r="L289" s="2"/>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A290" s="1"/>
       <c r="B290" s="1"/>
       <c r="C290" s="3"/>
@@ -6850,7 +6845,7 @@
       <c r="K290" s="2"/>
       <c r="L290" s="2"/>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A291" s="1"/>
       <c r="B291" s="1"/>
       <c r="C291" s="3"/>
@@ -6864,7 +6859,7 @@
       <c r="K291" s="2"/>
       <c r="L291" s="2"/>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A292" s="1"/>
       <c r="B292" s="1"/>
       <c r="C292" s="3"/>
@@ -6878,7 +6873,7 @@
       <c r="K292" s="2"/>
       <c r="L292" s="2"/>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A293" s="1"/>
       <c r="B293" s="1"/>
       <c r="C293" s="3"/>
@@ -6892,7 +6887,7 @@
       <c r="K293" s="2"/>
       <c r="L293" s="2"/>
     </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A294" s="1"/>
       <c r="B294" s="1"/>
       <c r="C294" s="3"/>
@@ -6906,7 +6901,7 @@
       <c r="K294" s="2"/>
       <c r="L294" s="2"/>
     </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A295" s="1"/>
       <c r="B295" s="1"/>
       <c r="C295" s="3"/>
@@ -6920,7 +6915,7 @@
       <c r="K295" s="2"/>
       <c r="L295" s="2"/>
     </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A296" s="1"/>
       <c r="B296" s="1"/>
       <c r="C296" s="3"/>
@@ -6934,7 +6929,7 @@
       <c r="K296" s="2"/>
       <c r="L296" s="2"/>
     </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A297" s="1"/>
       <c r="B297" s="1"/>
       <c r="C297" s="3"/>
@@ -6948,7 +6943,7 @@
       <c r="K297" s="2"/>
       <c r="L297" s="2"/>
     </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A298" s="1"/>
       <c r="B298" s="1"/>
       <c r="C298" s="3"/>
@@ -6962,7 +6957,7 @@
       <c r="K298" s="2"/>
       <c r="L298" s="2"/>
     </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A299" s="1"/>
       <c r="B299" s="1"/>
       <c r="C299" s="3"/>
@@ -6976,7 +6971,7 @@
       <c r="K299" s="2"/>
       <c r="L299" s="2"/>
     </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A300" s="1"/>
       <c r="B300" s="1"/>
       <c r="C300" s="3"/>
@@ -6990,7 +6985,7 @@
       <c r="K300" s="2"/>
       <c r="L300" s="2"/>
     </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A301" s="1"/>
       <c r="B301" s="1"/>
       <c r="C301" s="3"/>
@@ -7004,7 +6999,7 @@
       <c r="K301" s="2"/>
       <c r="L301" s="2"/>
     </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A302" s="1"/>
       <c r="B302" s="1"/>
       <c r="C302" s="3"/>
@@ -7018,7 +7013,7 @@
       <c r="K302" s="2"/>
       <c r="L302" s="2"/>
     </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A303" s="1"/>
       <c r="B303" s="1"/>
       <c r="C303" s="3"/>
@@ -7032,7 +7027,7 @@
       <c r="K303" s="2"/>
       <c r="L303" s="2"/>
     </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A304" s="1"/>
       <c r="B304" s="1"/>
       <c r="C304" s="3"/>
@@ -7046,7 +7041,7 @@
       <c r="K304" s="2"/>
       <c r="L304" s="2"/>
     </row>
-    <row r="305" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A305" s="1"/>
       <c r="B305" s="1"/>
       <c r="C305" s="3"/>
@@ -7060,7 +7055,7 @@
       <c r="K305" s="2"/>
       <c r="L305" s="2"/>
     </row>
-    <row r="306" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A306" s="1"/>
       <c r="B306" s="1"/>
       <c r="C306" s="3"/>
@@ -7074,7 +7069,7 @@
       <c r="K306" s="2"/>
       <c r="L306" s="2"/>
     </row>
-    <row r="307" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A307" s="1"/>
       <c r="B307" s="1"/>
       <c r="C307" s="3"/>
@@ -7088,7 +7083,7 @@
       <c r="K307" s="2"/>
       <c r="L307" s="2"/>
     </row>
-    <row r="308" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A308" s="1"/>
       <c r="B308" s="1"/>
       <c r="C308" s="3"/>
@@ -7102,7 +7097,7 @@
       <c r="K308" s="2"/>
       <c r="L308" s="2"/>
     </row>
-    <row r="309" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A309" s="1"/>
       <c r="B309" s="1"/>
       <c r="C309" s="3"/>
@@ -7116,7 +7111,7 @@
       <c r="K309" s="2"/>
       <c r="L309" s="2"/>
     </row>
-    <row r="310" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A310" s="1"/>
       <c r="B310" s="1"/>
       <c r="C310" s="3"/>
@@ -7130,7 +7125,7 @@
       <c r="K310" s="2"/>
       <c r="L310" s="2"/>
     </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A311" s="1"/>
       <c r="B311" s="1"/>
       <c r="C311" s="3"/>
@@ -7144,7 +7139,7 @@
       <c r="K311" s="2"/>
       <c r="L311" s="2"/>
     </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A312" s="1"/>
       <c r="B312" s="1"/>
       <c r="C312" s="3"/>
@@ -7158,7 +7153,7 @@
       <c r="K312" s="2"/>
       <c r="L312" s="2"/>
     </row>
-    <row r="313" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A313" s="1"/>
       <c r="B313" s="1"/>
       <c r="C313" s="3"/>
@@ -7172,7 +7167,7 @@
       <c r="K313" s="2"/>
       <c r="L313" s="2"/>
     </row>
-    <row r="314" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A314" s="1"/>
       <c r="B314" s="1"/>
       <c r="C314" s="3"/>
@@ -7186,7 +7181,7 @@
       <c r="K314" s="2"/>
       <c r="L314" s="2"/>
     </row>
-    <row r="315" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A315" s="1"/>
       <c r="B315" s="1"/>
       <c r="C315" s="3"/>
@@ -7200,7 +7195,7 @@
       <c r="K315" s="2"/>
       <c r="L315" s="2"/>
     </row>
-    <row r="316" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A316" s="1"/>
       <c r="B316" s="1"/>
       <c r="C316" s="3"/>
@@ -7214,7 +7209,7 @@
       <c r="K316" s="2"/>
       <c r="L316" s="2"/>
     </row>
-    <row r="317" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A317" s="1"/>
       <c r="B317" s="1"/>
       <c r="C317" s="3"/>
@@ -7228,7 +7223,7 @@
       <c r="K317" s="2"/>
       <c r="L317" s="2"/>
     </row>
-    <row r="318" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A318" s="1"/>
       <c r="B318" s="1"/>
       <c r="C318" s="3"/>
@@ -7242,7 +7237,7 @@
       <c r="K318" s="2"/>
       <c r="L318" s="2"/>
     </row>
-    <row r="319" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A319" s="1"/>
       <c r="B319" s="1"/>
       <c r="C319" s="3"/>
@@ -7256,7 +7251,7 @@
       <c r="K319" s="2"/>
       <c r="L319" s="2"/>
     </row>
-    <row r="320" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A320" s="1"/>
       <c r="B320" s="1"/>
       <c r="C320" s="3"/>
@@ -7270,7 +7265,7 @@
       <c r="K320" s="2"/>
       <c r="L320" s="2"/>
     </row>
-    <row r="321" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A321" s="1"/>
       <c r="B321" s="1"/>
       <c r="C321" s="3"/>
@@ -7284,7 +7279,7 @@
       <c r="K321" s="2"/>
       <c r="L321" s="2"/>
     </row>
-    <row r="322" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A322" s="1"/>
       <c r="B322" s="1"/>
       <c r="C322" s="3"/>
@@ -7298,7 +7293,7 @@
       <c r="K322" s="2"/>
       <c r="L322" s="2"/>
     </row>
-    <row r="323" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A323" s="1"/>
       <c r="B323" s="1"/>
       <c r="C323" s="3"/>
@@ -7312,7 +7307,7 @@
       <c r="K323" s="2"/>
       <c r="L323" s="2"/>
     </row>
-    <row r="324" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A324" s="1"/>
       <c r="B324" s="1"/>
       <c r="C324" s="3"/>
@@ -7326,7 +7321,7 @@
       <c r="K324" s="2"/>
       <c r="L324" s="2"/>
     </row>
-    <row r="325" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A325" s="1"/>
       <c r="B325" s="1"/>
       <c r="C325" s="3"/>
@@ -7340,7 +7335,7 @@
       <c r="K325" s="2"/>
       <c r="L325" s="2"/>
     </row>
-    <row r="326" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A326" s="1"/>
       <c r="B326" s="1"/>
       <c r="C326" s="3"/>
@@ -7354,7 +7349,7 @@
       <c r="K326" s="2"/>
       <c r="L326" s="2"/>
     </row>
-    <row r="327" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A327" s="1"/>
       <c r="B327" s="1"/>
       <c r="C327" s="3"/>
@@ -7368,7 +7363,7 @@
       <c r="K327" s="2"/>
       <c r="L327" s="2"/>
     </row>
-    <row r="328" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A328" s="1"/>
       <c r="B328" s="1"/>
       <c r="C328" s="3"/>
@@ -7382,7 +7377,7 @@
       <c r="K328" s="2"/>
       <c r="L328" s="2"/>
     </row>
-    <row r="329" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A329" s="1"/>
       <c r="B329" s="1"/>
       <c r="C329" s="3"/>
@@ -7396,7 +7391,7 @@
       <c r="K329" s="2"/>
       <c r="L329" s="2"/>
     </row>
-    <row r="330" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A330" s="1"/>
       <c r="B330" s="1"/>
       <c r="C330" s="3"/>
@@ -7410,7 +7405,7 @@
       <c r="K330" s="2"/>
       <c r="L330" s="2"/>
     </row>
-    <row r="331" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A331" s="1"/>
       <c r="B331" s="1"/>
       <c r="C331" s="3"/>
@@ -7424,7 +7419,7 @@
       <c r="K331" s="2"/>
       <c r="L331" s="2"/>
     </row>
-    <row r="332" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A332" s="1"/>
       <c r="B332" s="1"/>
       <c r="C332" s="3"/>
@@ -7438,7 +7433,7 @@
       <c r="K332" s="2"/>
       <c r="L332" s="2"/>
     </row>
-    <row r="333" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A333" s="1"/>
       <c r="B333" s="1"/>
       <c r="C333" s="3"/>
@@ -7452,7 +7447,7 @@
       <c r="K333" s="2"/>
       <c r="L333" s="2"/>
     </row>
-    <row r="334" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A334" s="1"/>
       <c r="B334" s="1"/>
       <c r="C334" s="3"/>
@@ -7466,7 +7461,7 @@
       <c r="K334" s="2"/>
       <c r="L334" s="2"/>
     </row>
-    <row r="335" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A335" s="1"/>
       <c r="B335" s="1"/>
       <c r="C335" s="3"/>
@@ -7480,7 +7475,7 @@
       <c r="K335" s="2"/>
       <c r="L335" s="2"/>
     </row>
-    <row r="336" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A336" s="1"/>
       <c r="B336" s="1"/>
       <c r="C336" s="3"/>
@@ -7494,7 +7489,7 @@
       <c r="K336" s="2"/>
       <c r="L336" s="2"/>
     </row>
-    <row r="337" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A337" s="1"/>
       <c r="B337" s="1"/>
       <c r="C337" s="3"/>
@@ -7508,7 +7503,7 @@
       <c r="K337" s="2"/>
       <c r="L337" s="2"/>
     </row>
-    <row r="338" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A338" s="1"/>
       <c r="B338" s="1"/>
       <c r="C338" s="3"/>
@@ -7522,7 +7517,7 @@
       <c r="K338" s="2"/>
       <c r="L338" s="2"/>
     </row>
-    <row r="339" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A339" s="1"/>
       <c r="B339" s="1"/>
       <c r="C339" s="3"/>
@@ -7536,7 +7531,7 @@
       <c r="K339" s="2"/>
       <c r="L339" s="2"/>
     </row>
-    <row r="340" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A340" s="1"/>
       <c r="B340" s="1"/>
       <c r="C340" s="3"/>
@@ -7550,7 +7545,7 @@
       <c r="K340" s="2"/>
       <c r="L340" s="2"/>
     </row>
-    <row r="341" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A341" s="1"/>
       <c r="B341" s="1"/>
       <c r="C341" s="3"/>
@@ -7564,7 +7559,7 @@
       <c r="K341" s="2"/>
       <c r="L341" s="2"/>
     </row>
-    <row r="342" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A342" s="1"/>
       <c r="B342" s="1"/>
       <c r="C342" s="3"/>
@@ -7578,7 +7573,7 @@
       <c r="K342" s="2"/>
       <c r="L342" s="2"/>
     </row>
-    <row r="343" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A343" s="1"/>
       <c r="B343" s="1"/>
       <c r="C343" s="3"/>
@@ -7592,7 +7587,7 @@
       <c r="K343" s="2"/>
       <c r="L343" s="2"/>
     </row>
-    <row r="344" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A344" s="1"/>
       <c r="B344" s="1"/>
       <c r="C344" s="3"/>
@@ -7606,7 +7601,7 @@
       <c r="K344" s="2"/>
       <c r="L344" s="2"/>
     </row>
-    <row r="345" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A345" s="1"/>
       <c r="B345" s="1"/>
       <c r="C345" s="3"/>
@@ -7620,7 +7615,7 @@
       <c r="K345" s="2"/>
       <c r="L345" s="2"/>
     </row>
-    <row r="346" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A346" s="1"/>
       <c r="B346" s="1"/>
       <c r="C346" s="3"/>
@@ -7634,7 +7629,7 @@
       <c r="K346" s="2"/>
       <c r="L346" s="2"/>
     </row>
-    <row r="347" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A347" s="1"/>
       <c r="B347" s="1"/>
       <c r="C347" s="3"/>
@@ -7648,7 +7643,7 @@
       <c r="K347" s="2"/>
       <c r="L347" s="2"/>
     </row>
-    <row r="348" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A348" s="1"/>
       <c r="B348" s="1"/>
       <c r="C348" s="3"/>
@@ -7662,7 +7657,7 @@
       <c r="K348" s="2"/>
       <c r="L348" s="2"/>
     </row>
-    <row r="349" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A349" s="1"/>
       <c r="B349" s="1"/>
       <c r="C349" s="3"/>
@@ -7676,7 +7671,7 @@
       <c r="K349" s="2"/>
       <c r="L349" s="2"/>
     </row>
-    <row r="350" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A350" s="1"/>
       <c r="B350" s="1"/>
       <c r="C350" s="3"/>

</xml_diff>

<commit_message>
Completed logging of data in the Google Sheet
</commit_message>
<xml_diff>
--- a/family-tree-data.xlsx
+++ b/family-tree-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASHil\PycharmProjects\Family-Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206E5717-024F-44EE-A0BF-776989DC55F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10BE6E2-E4C3-4EA5-91BD-29CAC80E562D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="315">
   <si>
     <t>Class Year</t>
   </si>
@@ -704,9 +704,6 @@
     <t>Love</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Jose</t>
   </si>
   <si>
@@ -732,6 +729,258 @@
   </si>
   <si>
     <t>Brown</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Bass</t>
+  </si>
+  <si>
+    <t>Addison</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>Flores</t>
+  </si>
+  <si>
+    <t>Blake</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Leonardo</t>
+  </si>
+  <si>
+    <t>Rex</t>
+  </si>
+  <si>
+    <t>Luke</t>
+  </si>
+  <si>
+    <t>Harrison</t>
+  </si>
+  <si>
+    <t>Kabell</t>
+  </si>
+  <si>
+    <t>John Luke</t>
+  </si>
+  <si>
+    <t>Spitler</t>
+  </si>
+  <si>
+    <t>Childress</t>
+  </si>
+  <si>
+    <t>Justin</t>
+  </si>
+  <si>
+    <t>Estes</t>
+  </si>
+  <si>
+    <t>Rogers</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Hayes</t>
+  </si>
+  <si>
+    <t>Zach</t>
+  </si>
+  <si>
+    <t>Harvey</t>
+  </si>
+  <si>
+    <t>Randal</t>
+  </si>
+  <si>
+    <t>Cousins</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Giese</t>
+  </si>
+  <si>
+    <t>Clint</t>
+  </si>
+  <si>
+    <t>Milner</t>
+  </si>
+  <si>
+    <t>Ortega</t>
+  </si>
+  <si>
+    <t>Lamkin</t>
+  </si>
+  <si>
+    <t>Kriger</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Rutter</t>
+  </si>
+  <si>
+    <t>Oberg</t>
+  </si>
+  <si>
+    <t>Sean</t>
+  </si>
+  <si>
+    <t>Corjay</t>
+  </si>
+  <si>
+    <t>Valencia</t>
+  </si>
+  <si>
+    <t>Andy</t>
+  </si>
+  <si>
+    <t>Zac</t>
+  </si>
+  <si>
+    <t>Caraway</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Timbol</t>
+  </si>
+  <si>
+    <t>Davidson</t>
+  </si>
+  <si>
+    <t>Seth</t>
+  </si>
+  <si>
+    <t>Ndumbe</t>
+  </si>
+  <si>
+    <t>Rudy</t>
+  </si>
+  <si>
+    <t>Gonzales</t>
+  </si>
+  <si>
+    <t>Mitch</t>
+  </si>
+  <si>
+    <t>Pace</t>
+  </si>
+  <si>
+    <t>Jimenez</t>
+  </si>
+  <si>
+    <t>Theimer</t>
+  </si>
+  <si>
+    <t>Noah</t>
+  </si>
+  <si>
+    <t>Reese</t>
+  </si>
+  <si>
+    <t>Lastrapes</t>
+  </si>
+  <si>
+    <t>Colton</t>
+  </si>
+  <si>
+    <t>Craft</t>
+  </si>
+  <si>
+    <t>Jakob</t>
+  </si>
+  <si>
+    <t>Schwartzenburg</t>
+  </si>
+  <si>
+    <t>Jonah</t>
+  </si>
+  <si>
+    <t>Snyder</t>
+  </si>
+  <si>
+    <t>Micah</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Lewis</t>
+  </si>
+  <si>
+    <t>Hall</t>
+  </si>
+  <si>
+    <t>Curto</t>
+  </si>
+  <si>
+    <t>Souris</t>
+  </si>
+  <si>
+    <t>Richard</t>
+  </si>
+  <si>
+    <t>Thornton</t>
+  </si>
+  <si>
+    <t>Sheridan</t>
+  </si>
+  <si>
+    <t>Fredrick</t>
+  </si>
+  <si>
+    <t>Hodge</t>
+  </si>
+  <si>
+    <t>Kevin?</t>
+  </si>
+  <si>
+    <t>2018?</t>
+  </si>
+  <si>
+    <t>Abu</t>
+  </si>
+  <si>
+    <t>Akki</t>
+  </si>
+  <si>
+    <t>Stephens</t>
+  </si>
+  <si>
+    <t>Harper</t>
+  </si>
+  <si>
+    <t>MuNos</t>
+  </si>
+  <si>
+    <t>Ty</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Revering</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Torruella</t>
   </si>
 </sst>
 </file>
@@ -1236,13 +1485,14 @@
   <dimension ref="A1:L350"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F133" sqref="F133"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H194" sqref="H194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="5" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" style="12" customWidth="1"/>
     <col min="5" max="11" width="17.6640625" customWidth="1"/>
@@ -2084,7 +2334,9 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
+      <c r="H33" s="2">
+        <v>2</v>
+      </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
@@ -2103,13 +2355,17 @@
       <c r="D34" s="2">
         <v>33</v>
       </c>
-      <c r="E34" s="2"/>
+      <c r="E34" s="2">
+        <v>193</v>
+      </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2">
+        <v>36</v>
+      </c>
+      <c r="I34" s="2">
         <v>34</v>
       </c>
-      <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -2195,19 +2451,29 @@
       <c r="B38" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="3"/>
+      <c r="C38" s="3">
+        <v>2015</v>
+      </c>
       <c r="D38" s="2">
         <v>37</v>
       </c>
-      <c r="E38" s="2"/>
+      <c r="E38" s="2">
+        <v>157</v>
+      </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2">
+        <v>164</v>
+      </c>
+      <c r="I38" s="2">
         <v>39</v>
       </c>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
+      <c r="J38" s="2">
+        <v>165</v>
+      </c>
+      <c r="K38" s="2">
+        <v>166</v>
+      </c>
       <c r="L38" s="2"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -2217,7 +2483,9 @@
       <c r="B39" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="3"/>
+      <c r="C39" s="3" t="s">
+        <v>206</v>
+      </c>
       <c r="D39" s="2">
         <v>38</v>
       </c>
@@ -3008,16 +3276,20 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>194</v>
+        <v>149</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C70" s="3"/>
+      <c r="C70" s="3">
+        <v>2022</v>
+      </c>
       <c r="D70" s="2">
         <v>69</v>
       </c>
-      <c r="E70" s="2"/>
+      <c r="E70" s="2">
+        <v>145</v>
+      </c>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
@@ -3208,7 +3480,9 @@
       <c r="E78" s="2">
         <v>68</v>
       </c>
-      <c r="F78" s="2"/>
+      <c r="F78" s="2">
+        <v>187</v>
+      </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
@@ -3863,7 +4137,9 @@
       <c r="D104" s="2">
         <v>103</v>
       </c>
-      <c r="E104" s="2"/>
+      <c r="E104" s="2">
+        <v>114</v>
+      </c>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
       <c r="H104" s="2">
@@ -3889,7 +4165,9 @@
       <c r="D105" s="2">
         <v>104</v>
       </c>
-      <c r="E105" s="2"/>
+      <c r="E105" s="2">
+        <v>136</v>
+      </c>
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
       <c r="H105" s="2">
@@ -3913,14 +4191,20 @@
       <c r="D106" s="2">
         <v>105</v>
       </c>
-      <c r="E106" s="2"/>
+      <c r="E106" s="2">
+        <v>145</v>
+      </c>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
-      <c r="H106" s="2"/>
+      <c r="H106" s="2">
+        <v>147</v>
+      </c>
       <c r="I106" s="2">
+        <v>116</v>
+      </c>
+      <c r="J106" s="2">
         <v>100</v>
       </c>
-      <c r="J106" s="2"/>
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
@@ -4161,7 +4445,9 @@
       <c r="D116" s="2">
         <v>115</v>
       </c>
-      <c r="E116" s="2"/>
+      <c r="E116" s="2">
+        <v>114</v>
+      </c>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
       <c r="H116" s="2">
@@ -4185,8 +4471,12 @@
       <c r="D117" s="2">
         <v>116</v>
       </c>
-      <c r="E117" s="2"/>
-      <c r="F117" s="2"/>
+      <c r="E117" s="2">
+        <v>91</v>
+      </c>
+      <c r="F117" s="2">
+        <v>105</v>
+      </c>
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
@@ -4207,7 +4497,9 @@
       <c r="D118" s="2">
         <v>117</v>
       </c>
-      <c r="E118" s="2"/>
+      <c r="E118" s="2">
+        <v>103</v>
+      </c>
       <c r="F118" s="2"/>
       <c r="G118" s="2"/>
       <c r="H118" s="2"/>
@@ -4280,8 +4572,12 @@
       </c>
       <c r="F121" s="2"/>
       <c r="G121" s="2"/>
-      <c r="H121" s="2"/>
-      <c r="I121" s="2"/>
+      <c r="H121" s="2">
+        <v>121</v>
+      </c>
+      <c r="I121" s="2">
+        <v>122</v>
+      </c>
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
@@ -4374,7 +4670,9 @@
       <c r="E125" s="2">
         <v>123</v>
       </c>
-      <c r="F125" s="2"/>
+      <c r="F125" s="2">
+        <v>174</v>
+      </c>
       <c r="G125" s="2"/>
       <c r="H125" s="2">
         <v>125</v>
@@ -4421,19 +4719,23 @@
       <c r="D127" s="2">
         <v>126</v>
       </c>
-      <c r="E127" s="2"/>
+      <c r="E127" s="2">
+        <v>170</v>
+      </c>
       <c r="F127" s="2"/>
       <c r="G127" s="2"/>
       <c r="H127" s="2">
+        <v>129</v>
+      </c>
+      <c r="I127" s="2">
         <v>15</v>
-      </c>
-      <c r="I127" s="2">
-        <v>129</v>
       </c>
       <c r="J127" s="2">
         <v>130</v>
       </c>
-      <c r="K127" s="2"/>
+      <c r="K127" s="2">
+        <v>171</v>
+      </c>
       <c r="L127" s="2"/>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.3">
@@ -4449,7 +4751,9 @@
       <c r="D128" s="2">
         <v>127</v>
       </c>
-      <c r="E128" s="2"/>
+      <c r="E128" s="2">
+        <v>15</v>
+      </c>
       <c r="F128" s="2"/>
       <c r="G128" s="2"/>
       <c r="H128" s="2"/>
@@ -4471,10 +4775,14 @@
       <c r="D129" s="2">
         <v>128</v>
       </c>
-      <c r="E129" s="2"/>
+      <c r="E129" s="2">
+        <v>15</v>
+      </c>
       <c r="F129" s="2"/>
       <c r="G129" s="2"/>
-      <c r="H129" s="2"/>
+      <c r="H129" s="2">
+        <v>133</v>
+      </c>
       <c r="I129" s="2"/>
       <c r="J129" s="2"/>
       <c r="K129" s="2"/>
@@ -4493,10 +4801,14 @@
       <c r="D130" s="2">
         <v>129</v>
       </c>
-      <c r="E130" s="2"/>
+      <c r="E130" s="2">
+        <v>126</v>
+      </c>
       <c r="F130" s="2"/>
       <c r="G130" s="2"/>
-      <c r="H130" s="2"/>
+      <c r="H130" s="2">
+        <v>131</v>
+      </c>
       <c r="I130" s="2"/>
       <c r="J130" s="2"/>
       <c r="K130" s="2"/>
@@ -4515,11 +4827,17 @@
       <c r="D131" s="2">
         <v>130</v>
       </c>
-      <c r="E131" s="2"/>
+      <c r="E131" s="2">
+        <v>126</v>
+      </c>
       <c r="F131" s="2"/>
       <c r="G131" s="2"/>
-      <c r="H131" s="2"/>
-      <c r="I131" s="2"/>
+      <c r="H131" s="2">
+        <v>75</v>
+      </c>
+      <c r="I131" s="2">
+        <v>132</v>
+      </c>
       <c r="J131" s="2"/>
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
@@ -4537,10 +4855,14 @@
       <c r="D132" s="2">
         <v>131</v>
       </c>
-      <c r="E132" s="2"/>
+      <c r="E132" s="2">
+        <v>129</v>
+      </c>
       <c r="F132" s="2"/>
       <c r="G132" s="2"/>
-      <c r="H132" s="2"/>
+      <c r="H132" s="2">
+        <v>134</v>
+      </c>
       <c r="I132" s="2"/>
       <c r="J132" s="2"/>
       <c r="K132" s="2"/>
@@ -4553,13 +4875,15 @@
       <c r="B133" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C133" s="3" t="s">
-        <v>222</v>
+      <c r="C133" s="3">
+        <v>2021</v>
       </c>
       <c r="D133" s="2">
         <v>132</v>
       </c>
-      <c r="E133" s="2"/>
+      <c r="E133" s="2">
+        <v>130</v>
+      </c>
       <c r="F133" s="2"/>
       <c r="G133" s="2"/>
       <c r="H133" s="2"/>
@@ -4570,7 +4894,7 @@
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>200</v>
@@ -4581,13 +4905,23 @@
       <c r="D134" s="2">
         <v>133</v>
       </c>
-      <c r="E134" s="2"/>
+      <c r="E134" s="2">
+        <v>128</v>
+      </c>
       <c r="F134" s="2"/>
       <c r="G134" s="2"/>
-      <c r="H134" s="2"/>
-      <c r="I134" s="2"/>
-      <c r="J134" s="2"/>
-      <c r="K134" s="2"/>
+      <c r="H134" s="2">
+        <v>141</v>
+      </c>
+      <c r="I134" s="2">
+        <v>143</v>
+      </c>
+      <c r="J134" s="2">
+        <v>135</v>
+      </c>
+      <c r="K134" s="2">
+        <v>144</v>
+      </c>
       <c r="L134" s="2"/>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.3">
@@ -4603,10 +4937,14 @@
       <c r="D135" s="2">
         <v>134</v>
       </c>
-      <c r="E135" s="2"/>
+      <c r="E135" s="2">
+        <v>131</v>
+      </c>
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
-      <c r="H135" s="2"/>
+      <c r="H135" s="2">
+        <v>136</v>
+      </c>
       <c r="I135" s="2"/>
       <c r="J135" s="2"/>
       <c r="K135" s="2"/>
@@ -4617,7 +4955,7 @@
         <v>49</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C136" s="3">
         <v>2023</v>
@@ -4625,7 +4963,9 @@
       <c r="D136" s="2">
         <v>135</v>
       </c>
-      <c r="E136" s="2"/>
+      <c r="E136" s="2">
+        <v>133</v>
+      </c>
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
       <c r="H136" s="2"/>
@@ -4636,10 +4976,10 @@
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B137" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="C137" s="3">
         <v>2022</v>
@@ -4647,11 +4987,17 @@
       <c r="D137" s="2">
         <v>136</v>
       </c>
-      <c r="E137" s="2"/>
+      <c r="E137" s="2">
+        <v>134</v>
+      </c>
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
-      <c r="H137" s="2"/>
-      <c r="I137" s="2"/>
+      <c r="H137" s="2">
+        <v>137</v>
+      </c>
+      <c r="I137" s="2">
+        <v>104</v>
+      </c>
       <c r="J137" s="2"/>
       <c r="K137" s="2"/>
       <c r="L137" s="2"/>
@@ -4661,7 +5007,7 @@
         <v>80</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C138" s="3">
         <v>2022</v>
@@ -4669,11 +5015,17 @@
       <c r="D138" s="2">
         <v>137</v>
       </c>
-      <c r="E138" s="2"/>
+      <c r="E138" s="2">
+        <v>136</v>
+      </c>
       <c r="F138" s="2"/>
       <c r="G138" s="2"/>
-      <c r="H138" s="2"/>
-      <c r="I138" s="2"/>
+      <c r="H138" s="2">
+        <v>138</v>
+      </c>
+      <c r="I138" s="2">
+        <v>139</v>
+      </c>
       <c r="J138" s="2"/>
       <c r="K138" s="2"/>
       <c r="L138" s="2"/>
@@ -4683,7 +5035,7 @@
         <v>64</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C139" s="3">
         <v>2020</v>
@@ -4691,7 +5043,9 @@
       <c r="D139" s="2">
         <v>138</v>
       </c>
-      <c r="E139" s="2"/>
+      <c r="E139" s="2">
+        <v>137</v>
+      </c>
       <c r="F139" s="2"/>
       <c r="G139" s="2"/>
       <c r="H139" s="2"/>
@@ -4705,7 +5059,7 @@
         <v>25</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C140" s="3">
         <v>2025</v>
@@ -4713,7 +5067,9 @@
       <c r="D140" s="2">
         <v>139</v>
       </c>
-      <c r="E140" s="2"/>
+      <c r="E140" s="2">
+        <v>137</v>
+      </c>
       <c r="F140" s="2"/>
       <c r="G140" s="2"/>
       <c r="H140" s="2"/>
@@ -4724,10 +5080,10 @@
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="C141" s="3">
         <v>2025</v>
@@ -4735,7 +5091,9 @@
       <c r="D141" s="2">
         <v>140</v>
       </c>
-      <c r="E141" s="2"/>
+      <c r="E141" s="2">
+        <v>104</v>
+      </c>
       <c r="F141" s="2"/>
       <c r="G141" s="2"/>
       <c r="H141" s="2"/>
@@ -4745,29 +5103,47 @@
       <c r="L141" s="2"/>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A142" s="1"/>
-      <c r="B142" s="1"/>
-      <c r="C142" s="3"/>
+      <c r="A142" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C142" s="3">
+        <v>2023</v>
+      </c>
       <c r="D142" s="2">
         <v>141</v>
       </c>
-      <c r="E142" s="2"/>
+      <c r="E142" s="2">
+        <v>133</v>
+      </c>
       <c r="F142" s="2"/>
       <c r="G142" s="2"/>
-      <c r="H142" s="2"/>
+      <c r="H142" s="2">
+        <v>142</v>
+      </c>
       <c r="I142" s="2"/>
       <c r="J142" s="2"/>
       <c r="K142" s="2"/>
       <c r="L142" s="2"/>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A143" s="1"/>
-      <c r="B143" s="1"/>
-      <c r="C143" s="3"/>
+      <c r="A143" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C143" s="3">
+        <v>2023</v>
+      </c>
       <c r="D143" s="2">
         <v>142</v>
       </c>
-      <c r="E143" s="2"/>
+      <c r="E143" s="2">
+        <v>141</v>
+      </c>
       <c r="F143" s="2"/>
       <c r="G143" s="2"/>
       <c r="H143" s="2"/>
@@ -4777,13 +5153,21 @@
       <c r="L143" s="2"/>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A144" s="1"/>
-      <c r="B144" s="1"/>
-      <c r="C144" s="3"/>
+      <c r="A144" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C144" s="3">
+        <v>2024</v>
+      </c>
       <c r="D144" s="2">
         <v>143</v>
       </c>
-      <c r="E144" s="2"/>
+      <c r="E144" s="2">
+        <v>133</v>
+      </c>
       <c r="F144" s="2"/>
       <c r="G144" s="2"/>
       <c r="H144" s="2"/>
@@ -4793,13 +5177,21 @@
       <c r="L144" s="2"/>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A145" s="1"/>
-      <c r="B145" s="1"/>
-      <c r="C145" s="3"/>
+      <c r="A145" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C145" s="3">
+        <v>2022</v>
+      </c>
       <c r="D145" s="2">
         <v>144</v>
       </c>
-      <c r="E145" s="2"/>
+      <c r="E145" s="2">
+        <v>133</v>
+      </c>
       <c r="F145" s="2"/>
       <c r="G145" s="2"/>
       <c r="H145" s="2"/>
@@ -4809,29 +5201,49 @@
       <c r="L145" s="2"/>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A146" s="1"/>
-      <c r="B146" s="1"/>
-      <c r="C146" s="3"/>
+      <c r="A146" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C146" s="3">
+        <v>2020</v>
+      </c>
       <c r="D146" s="2">
         <v>145</v>
       </c>
       <c r="E146" s="2"/>
       <c r="F146" s="2"/>
       <c r="G146" s="2"/>
-      <c r="H146" s="2"/>
-      <c r="I146" s="2"/>
-      <c r="J146" s="2"/>
+      <c r="H146" s="2">
+        <v>146</v>
+      </c>
+      <c r="I146" s="2">
+        <v>69</v>
+      </c>
+      <c r="J146" s="2">
+        <v>105</v>
+      </c>
       <c r="K146" s="2"/>
       <c r="L146" s="2"/>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A147" s="1"/>
-      <c r="B147" s="1"/>
-      <c r="C147" s="3"/>
+      <c r="A147" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C147" s="3">
+        <v>2021</v>
+      </c>
       <c r="D147" s="2">
         <v>146</v>
       </c>
-      <c r="E147" s="2"/>
+      <c r="E147" s="2">
+        <v>145</v>
+      </c>
       <c r="F147" s="2"/>
       <c r="G147" s="2"/>
       <c r="H147" s="2"/>
@@ -4841,13 +5253,21 @@
       <c r="L147" s="2"/>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A148" s="1"/>
-      <c r="B148" s="1"/>
-      <c r="C148" s="3"/>
+      <c r="A148" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C148" s="3">
+        <v>2024</v>
+      </c>
       <c r="D148" s="2">
         <v>147</v>
       </c>
-      <c r="E148" s="2"/>
+      <c r="E148" s="2">
+        <v>105</v>
+      </c>
       <c r="F148" s="2"/>
       <c r="G148" s="2"/>
       <c r="H148" s="2"/>
@@ -4857,73 +5277,131 @@
       <c r="L148" s="2"/>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A149" s="1"/>
-      <c r="B149" s="1"/>
-      <c r="C149" s="3"/>
+      <c r="A149" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C149" s="3">
+        <v>1999</v>
+      </c>
       <c r="D149" s="2">
         <v>148</v>
       </c>
       <c r="E149" s="2"/>
       <c r="F149" s="2"/>
       <c r="G149" s="2"/>
-      <c r="H149" s="2"/>
+      <c r="H149" s="2">
+        <v>149</v>
+      </c>
       <c r="I149" s="2"/>
       <c r="J149" s="2"/>
       <c r="K149" s="2"/>
       <c r="L149" s="2"/>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A150" s="1"/>
-      <c r="B150" s="1"/>
-      <c r="C150" s="3"/>
+      <c r="A150" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C150" s="3">
+        <v>2001</v>
+      </c>
       <c r="D150" s="2">
         <v>149</v>
       </c>
-      <c r="E150" s="2"/>
+      <c r="E150" s="2">
+        <v>148</v>
+      </c>
       <c r="F150" s="2"/>
       <c r="G150" s="2"/>
-      <c r="H150" s="2"/>
+      <c r="H150" s="2">
+        <v>150</v>
+      </c>
       <c r="I150" s="2"/>
       <c r="J150" s="2"/>
       <c r="K150" s="2"/>
       <c r="L150" s="2"/>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A151" s="1"/>
-      <c r="B151" s="1"/>
-      <c r="C151" s="3"/>
+      <c r="A151" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C151" s="3">
+        <v>2005</v>
+      </c>
       <c r="D151" s="2">
         <v>150</v>
       </c>
-      <c r="E151" s="2"/>
+      <c r="E151" s="2">
+        <v>149</v>
+      </c>
       <c r="F151" s="2"/>
       <c r="G151" s="2"/>
-      <c r="H151" s="2"/>
-      <c r="I151" s="2"/>
-      <c r="J151" s="2"/>
+      <c r="H151" s="2">
+        <v>151</v>
+      </c>
+      <c r="I151" s="2">
+        <v>152</v>
+      </c>
+      <c r="J151" s="2">
+        <v>153</v>
+      </c>
       <c r="K151" s="2"/>
       <c r="L151" s="2"/>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A152" s="1"/>
-      <c r="B152" s="1"/>
-      <c r="C152" s="3"/>
-      <c r="D152" s="2"/>
-      <c r="E152" s="2"/>
+      <c r="A152" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C152" s="3">
+        <v>2006</v>
+      </c>
+      <c r="D152" s="2">
+        <v>151</v>
+      </c>
+      <c r="E152" s="2">
+        <v>150</v>
+      </c>
       <c r="F152" s="2"/>
       <c r="G152" s="2"/>
-      <c r="H152" s="2"/>
-      <c r="I152" s="2"/>
-      <c r="J152" s="2"/>
+      <c r="H152" s="2">
+        <v>154</v>
+      </c>
+      <c r="I152" s="2">
+        <v>155</v>
+      </c>
+      <c r="J152" s="2">
+        <v>156</v>
+      </c>
       <c r="K152" s="2"/>
       <c r="L152" s="2"/>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A153" s="1"/>
-      <c r="B153" s="1"/>
-      <c r="C153" s="3"/>
-      <c r="D153" s="2"/>
-      <c r="E153" s="2"/>
+      <c r="A153" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C153" s="3">
+        <v>2007</v>
+      </c>
+      <c r="D153" s="2">
+        <v>152</v>
+      </c>
+      <c r="E153" s="2">
+        <v>150</v>
+      </c>
       <c r="F153" s="2"/>
       <c r="G153" s="2"/>
       <c r="H153" s="2"/>
@@ -4933,11 +5411,19 @@
       <c r="L153" s="2"/>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A154" s="1"/>
-      <c r="B154" s="1"/>
+      <c r="A154" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>252</v>
+      </c>
       <c r="C154" s="3"/>
-      <c r="D154" s="2"/>
-      <c r="E154" s="2"/>
+      <c r="D154" s="2">
+        <v>153</v>
+      </c>
+      <c r="E154" s="2">
+        <v>150</v>
+      </c>
       <c r="F154" s="2"/>
       <c r="G154" s="2"/>
       <c r="H154" s="2"/>
@@ -4947,11 +5433,21 @@
       <c r="L154" s="2"/>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A155" s="1"/>
-      <c r="B155" s="1"/>
-      <c r="C155" s="3"/>
-      <c r="D155" s="2"/>
-      <c r="E155" s="2"/>
+      <c r="A155" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C155" s="3">
+        <v>2006</v>
+      </c>
+      <c r="D155" s="2">
+        <v>154</v>
+      </c>
+      <c r="E155" s="2">
+        <v>151</v>
+      </c>
       <c r="F155" s="2"/>
       <c r="G155" s="2"/>
       <c r="H155" s="2"/>
@@ -4961,11 +5457,21 @@
       <c r="L155" s="2"/>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A156" s="1"/>
-      <c r="B156" s="1"/>
-      <c r="C156" s="3"/>
-      <c r="D156" s="2"/>
-      <c r="E156" s="2"/>
+      <c r="A156" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C156" s="3">
+        <v>2008</v>
+      </c>
+      <c r="D156" s="2">
+        <v>155</v>
+      </c>
+      <c r="E156" s="2">
+        <v>151</v>
+      </c>
       <c r="F156" s="2"/>
       <c r="G156" s="2"/>
       <c r="H156" s="2"/>
@@ -4975,39 +5481,85 @@
       <c r="L156" s="2"/>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A157" s="1"/>
-      <c r="B157" s="1"/>
-      <c r="C157" s="3"/>
-      <c r="D157" s="2"/>
-      <c r="E157" s="2"/>
+      <c r="A157" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C157" s="3">
+        <v>2009</v>
+      </c>
+      <c r="D157" s="2">
+        <v>156</v>
+      </c>
+      <c r="E157" s="2">
+        <v>151</v>
+      </c>
       <c r="F157" s="2"/>
       <c r="G157" s="2"/>
-      <c r="H157" s="2"/>
-      <c r="I157" s="2"/>
-      <c r="J157" s="2"/>
-      <c r="K157" s="2"/>
-      <c r="L157" s="2"/>
+      <c r="H157" s="2">
+        <v>157</v>
+      </c>
+      <c r="I157" s="2">
+        <v>158</v>
+      </c>
+      <c r="J157" s="2">
+        <v>159</v>
+      </c>
+      <c r="K157" s="2">
+        <v>160</v>
+      </c>
+      <c r="L157" s="2">
+        <v>161</v>
+      </c>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A158" s="1"/>
-      <c r="B158" s="1"/>
-      <c r="C158" s="3"/>
-      <c r="D158" s="2"/>
-      <c r="E158" s="2"/>
+      <c r="A158" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C158" s="3">
+        <v>2013</v>
+      </c>
+      <c r="D158" s="2">
+        <v>157</v>
+      </c>
+      <c r="E158" s="2">
+        <v>156</v>
+      </c>
       <c r="F158" s="2"/>
       <c r="G158" s="2"/>
-      <c r="H158" s="2"/>
-      <c r="I158" s="2"/>
-      <c r="J158" s="2"/>
+      <c r="H158" s="2">
+        <v>37</v>
+      </c>
+      <c r="I158" s="2">
+        <v>162</v>
+      </c>
+      <c r="J158" s="2">
+        <v>163</v>
+      </c>
       <c r="K158" s="2"/>
       <c r="L158" s="2"/>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A159" s="1"/>
-      <c r="B159" s="1"/>
-      <c r="C159" s="3"/>
-      <c r="D159" s="2"/>
-      <c r="E159" s="2"/>
+      <c r="A159" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C159" s="3">
+        <v>2010</v>
+      </c>
+      <c r="D159" s="2">
+        <v>158</v>
+      </c>
+      <c r="E159" s="2">
+        <v>156</v>
+      </c>
       <c r="F159" s="2"/>
       <c r="G159" s="2"/>
       <c r="H159" s="2"/>
@@ -5017,11 +5569,21 @@
       <c r="L159" s="2"/>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A160" s="1"/>
-      <c r="B160" s="1"/>
-      <c r="C160" s="3"/>
-      <c r="D160" s="2"/>
-      <c r="E160" s="2"/>
+      <c r="A160" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C160" s="3">
+        <v>2010</v>
+      </c>
+      <c r="D160" s="2">
+        <v>159</v>
+      </c>
+      <c r="E160" s="2">
+        <v>156</v>
+      </c>
       <c r="F160" s="2"/>
       <c r="G160" s="2"/>
       <c r="H160" s="2"/>
@@ -5031,53 +5593,105 @@
       <c r="L160" s="2"/>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A161" s="1"/>
-      <c r="B161" s="1"/>
-      <c r="C161" s="3"/>
-      <c r="D161" s="2"/>
-      <c r="E161" s="2"/>
+      <c r="A161" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C161" s="3">
+        <v>2011</v>
+      </c>
+      <c r="D161" s="2">
+        <v>160</v>
+      </c>
+      <c r="E161" s="2">
+        <v>156</v>
+      </c>
       <c r="F161" s="2"/>
       <c r="G161" s="2"/>
-      <c r="H161" s="2"/>
-      <c r="I161" s="2"/>
+      <c r="H161" s="2">
+        <v>180</v>
+      </c>
+      <c r="I161" s="2">
+        <v>181</v>
+      </c>
       <c r="J161" s="2"/>
       <c r="K161" s="2"/>
       <c r="L161" s="2"/>
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A162" s="1"/>
-      <c r="B162" s="1"/>
-      <c r="C162" s="3"/>
-      <c r="D162" s="2"/>
-      <c r="E162" s="2"/>
+      <c r="A162" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C162" s="3">
+        <v>2012</v>
+      </c>
+      <c r="D162" s="2">
+        <v>161</v>
+      </c>
+      <c r="E162" s="2">
+        <v>156</v>
+      </c>
       <c r="F162" s="2"/>
       <c r="G162" s="2"/>
-      <c r="H162" s="2"/>
-      <c r="I162" s="2"/>
-      <c r="J162" s="2"/>
+      <c r="H162" s="2">
+        <v>183</v>
+      </c>
+      <c r="I162" s="2">
+        <v>184</v>
+      </c>
+      <c r="J162" s="2">
+        <v>185</v>
+      </c>
       <c r="K162" s="2"/>
       <c r="L162" s="2"/>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A163" s="1"/>
-      <c r="B163" s="1"/>
-      <c r="C163" s="3"/>
-      <c r="D163" s="2"/>
-      <c r="E163" s="2"/>
+      <c r="A163" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C163" s="3">
+        <v>2016</v>
+      </c>
+      <c r="D163" s="2">
+        <v>162</v>
+      </c>
+      <c r="E163" s="2">
+        <v>157</v>
+      </c>
       <c r="F163" s="2"/>
       <c r="G163" s="2"/>
-      <c r="H163" s="2"/>
+      <c r="H163" s="2">
+        <v>169</v>
+      </c>
       <c r="I163" s="2"/>
       <c r="J163" s="2"/>
       <c r="K163" s="2"/>
       <c r="L163" s="2"/>
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A164" s="1"/>
-      <c r="B164" s="1"/>
-      <c r="C164" s="3"/>
-      <c r="D164" s="2"/>
-      <c r="E164" s="2"/>
+      <c r="A164" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C164" s="3">
+        <v>2017</v>
+      </c>
+      <c r="D164" s="2">
+        <v>163</v>
+      </c>
+      <c r="E164" s="2">
+        <v>157</v>
+      </c>
       <c r="F164" s="2"/>
       <c r="G164" s="2"/>
       <c r="H164" s="2"/>
@@ -5087,11 +5701,21 @@
       <c r="L164" s="2"/>
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A165" s="1"/>
-      <c r="B165" s="1"/>
-      <c r="C165" s="3"/>
-      <c r="D165" s="2"/>
-      <c r="E165" s="2"/>
+      <c r="A165" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C165" s="3">
+        <v>2017</v>
+      </c>
+      <c r="D165" s="2">
+        <v>164</v>
+      </c>
+      <c r="E165" s="2">
+        <v>37</v>
+      </c>
       <c r="F165" s="2"/>
       <c r="G165" s="2"/>
       <c r="H165" s="2"/>
@@ -5101,11 +5725,21 @@
       <c r="L165" s="2"/>
     </row>
     <row r="166" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A166" s="1"/>
-      <c r="B166" s="1"/>
-      <c r="C166" s="3"/>
-      <c r="D166" s="2"/>
-      <c r="E166" s="2"/>
+      <c r="A166" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C166" s="3">
+        <v>2013</v>
+      </c>
+      <c r="D166" s="2">
+        <v>165</v>
+      </c>
+      <c r="E166" s="2">
+        <v>37</v>
+      </c>
       <c r="F166" s="2"/>
       <c r="G166" s="2"/>
       <c r="H166" s="2"/>
@@ -5115,11 +5749,21 @@
       <c r="L166" s="2"/>
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A167" s="1"/>
-      <c r="B167" s="1"/>
-      <c r="C167" s="3"/>
-      <c r="D167" s="2"/>
-      <c r="E167" s="2"/>
+      <c r="A167" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C167" s="3">
+        <v>2016</v>
+      </c>
+      <c r="D167" s="2">
+        <v>166</v>
+      </c>
+      <c r="E167" s="2">
+        <v>37</v>
+      </c>
       <c r="F167" s="2"/>
       <c r="G167" s="2"/>
       <c r="H167" s="2"/>
@@ -5129,25 +5773,47 @@
       <c r="L167" s="2"/>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A168" s="1"/>
-      <c r="B168" s="1"/>
-      <c r="C168" s="3"/>
-      <c r="D168" s="2"/>
-      <c r="E168" s="2"/>
+      <c r="A168" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C168" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D168" s="2">
+        <v>167</v>
+      </c>
+      <c r="E168" s="2">
+        <v>164</v>
+      </c>
       <c r="F168" s="2"/>
       <c r="G168" s="2"/>
-      <c r="H168" s="2"/>
+      <c r="H168" s="2">
+        <v>168</v>
+      </c>
       <c r="I168" s="2"/>
       <c r="J168" s="2"/>
       <c r="K168" s="2"/>
       <c r="L168" s="2"/>
     </row>
     <row r="169" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A169" s="1"/>
-      <c r="B169" s="1"/>
-      <c r="C169" s="3"/>
-      <c r="D169" s="2"/>
-      <c r="E169" s="2"/>
+      <c r="A169" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C169" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D169" s="2">
+        <v>168</v>
+      </c>
+      <c r="E169" s="2">
+        <v>167</v>
+      </c>
       <c r="F169" s="2"/>
       <c r="G169" s="2"/>
       <c r="H169" s="2"/>
@@ -5157,12 +5823,24 @@
       <c r="L169" s="2"/>
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A170" s="1"/>
-      <c r="B170" s="1"/>
-      <c r="C170" s="3"/>
-      <c r="D170" s="2"/>
-      <c r="E170" s="2"/>
-      <c r="F170" s="2"/>
+      <c r="A170" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C170" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D170" s="2">
+        <v>169</v>
+      </c>
+      <c r="E170" s="2">
+        <v>162</v>
+      </c>
+      <c r="F170" s="2">
+        <v>163</v>
+      </c>
       <c r="G170" s="2"/>
       <c r="H170" s="2"/>
       <c r="I170" s="2"/>
@@ -5171,25 +5849,43 @@
       <c r="L170" s="2"/>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A171" s="1"/>
-      <c r="B171" s="1"/>
-      <c r="C171" s="3"/>
-      <c r="D171" s="2"/>
+      <c r="A171" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C171" s="3">
+        <v>2012</v>
+      </c>
+      <c r="D171" s="2">
+        <v>170</v>
+      </c>
       <c r="E171" s="2"/>
       <c r="F171" s="2"/>
       <c r="G171" s="2"/>
-      <c r="H171" s="2"/>
+      <c r="H171" s="2">
+        <v>126</v>
+      </c>
       <c r="I171" s="2"/>
       <c r="J171" s="2"/>
       <c r="K171" s="2"/>
       <c r="L171" s="2"/>
     </row>
     <row r="172" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A172" s="1"/>
-      <c r="B172" s="1"/>
+      <c r="A172" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>280</v>
+      </c>
       <c r="C172" s="3"/>
-      <c r="D172" s="2"/>
-      <c r="E172" s="2"/>
+      <c r="D172" s="2">
+        <v>171</v>
+      </c>
+      <c r="E172" s="2">
+        <v>126</v>
+      </c>
       <c r="F172" s="2"/>
       <c r="G172" s="2"/>
       <c r="H172" s="2"/>
@@ -5199,25 +5895,51 @@
       <c r="L172" s="2"/>
     </row>
     <row r="173" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A173" s="1"/>
-      <c r="B173" s="1"/>
-      <c r="C173" s="3"/>
-      <c r="D173" s="2"/>
-      <c r="E173" s="2"/>
+      <c r="A173" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C173" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D173" s="2">
+        <v>172</v>
+      </c>
+      <c r="E173" s="2">
+        <v>169</v>
+      </c>
       <c r="F173" s="2"/>
       <c r="G173" s="2"/>
-      <c r="H173" s="2"/>
-      <c r="I173" s="2"/>
-      <c r="J173" s="2"/>
+      <c r="H173" s="2">
+        <v>174</v>
+      </c>
+      <c r="I173" s="2">
+        <v>175</v>
+      </c>
+      <c r="J173" s="2">
+        <v>176</v>
+      </c>
       <c r="K173" s="2"/>
       <c r="L173" s="2"/>
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A174" s="1"/>
-      <c r="B174" s="1"/>
-      <c r="C174" s="3"/>
-      <c r="D174" s="2"/>
-      <c r="E174" s="2"/>
+      <c r="A174" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C174" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D174" s="2">
+        <v>173</v>
+      </c>
+      <c r="E174" s="2">
+        <v>169</v>
+      </c>
       <c r="F174" s="2"/>
       <c r="G174" s="2"/>
       <c r="H174" s="2"/>
@@ -5227,25 +5949,49 @@
       <c r="L174" s="2"/>
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A175" s="1"/>
-      <c r="B175" s="1"/>
-      <c r="C175" s="3"/>
-      <c r="D175" s="2"/>
-      <c r="E175" s="2"/>
+      <c r="A175" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C175" s="3">
+        <v>2022</v>
+      </c>
+      <c r="D175" s="2">
+        <v>174</v>
+      </c>
+      <c r="E175" s="2">
+        <v>172</v>
+      </c>
       <c r="F175" s="2"/>
       <c r="G175" s="2"/>
-      <c r="H175" s="2"/>
-      <c r="I175" s="2"/>
+      <c r="H175" s="2">
+        <v>124</v>
+      </c>
+      <c r="I175" s="2">
+        <v>177</v>
+      </c>
       <c r="J175" s="2"/>
       <c r="K175" s="2"/>
       <c r="L175" s="2"/>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A176" s="1"/>
-      <c r="B176" s="1"/>
-      <c r="C176" s="3"/>
-      <c r="D176" s="2"/>
-      <c r="E176" s="2"/>
+      <c r="A176" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C176" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D176" s="2">
+        <v>175</v>
+      </c>
+      <c r="E176" s="2">
+        <v>172</v>
+      </c>
       <c r="F176" s="2"/>
       <c r="G176" s="2"/>
       <c r="H176" s="2"/>
@@ -5255,25 +6001,47 @@
       <c r="L176" s="2"/>
     </row>
     <row r="177" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A177" s="1"/>
-      <c r="B177" s="1"/>
-      <c r="C177" s="3"/>
-      <c r="D177" s="2"/>
-      <c r="E177" s="2"/>
+      <c r="A177" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C177" s="3">
+        <v>2024</v>
+      </c>
+      <c r="D177" s="2">
+        <v>176</v>
+      </c>
+      <c r="E177" s="2">
+        <v>172</v>
+      </c>
       <c r="F177" s="2"/>
       <c r="G177" s="2"/>
-      <c r="H177" s="2"/>
+      <c r="H177" s="2">
+        <v>178</v>
+      </c>
       <c r="I177" s="2"/>
       <c r="J177" s="2"/>
       <c r="K177" s="2"/>
       <c r="L177" s="2"/>
     </row>
     <row r="178" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A178" s="1"/>
-      <c r="B178" s="1"/>
-      <c r="C178" s="3"/>
-      <c r="D178" s="2"/>
-      <c r="E178" s="2"/>
+      <c r="A178" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C178" s="3">
+        <v>2025</v>
+      </c>
+      <c r="D178" s="2">
+        <v>177</v>
+      </c>
+      <c r="E178" s="2">
+        <v>174</v>
+      </c>
       <c r="F178" s="2"/>
       <c r="G178" s="2"/>
       <c r="H178" s="2"/>
@@ -5283,11 +6051,21 @@
       <c r="L178" s="2"/>
     </row>
     <row r="179" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A179" s="1"/>
-      <c r="B179" s="1"/>
-      <c r="C179" s="3"/>
-      <c r="D179" s="2"/>
-      <c r="E179" s="2"/>
+      <c r="A179" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C179" s="3">
+        <v>2025</v>
+      </c>
+      <c r="D179" s="2">
+        <v>178</v>
+      </c>
+      <c r="E179" s="2">
+        <v>176</v>
+      </c>
       <c r="F179" s="2"/>
       <c r="G179" s="2"/>
       <c r="H179" s="2"/>
@@ -5297,11 +6075,19 @@
       <c r="L179" s="2"/>
     </row>
     <row r="180" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A180" s="1"/>
-      <c r="B180" s="1"/>
+      <c r="A180" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>293</v>
+      </c>
       <c r="C180" s="3"/>
-      <c r="D180" s="2"/>
-      <c r="E180" s="2"/>
+      <c r="D180" s="2">
+        <v>179</v>
+      </c>
+      <c r="E180" s="2">
+        <v>163</v>
+      </c>
       <c r="F180" s="2"/>
       <c r="G180" s="2"/>
       <c r="H180" s="2"/>
@@ -5311,25 +6097,43 @@
       <c r="L180" s="2"/>
     </row>
     <row r="181" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A181" s="1"/>
-      <c r="B181" s="1"/>
+      <c r="A181" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>294</v>
+      </c>
       <c r="C181" s="3"/>
-      <c r="D181" s="2"/>
-      <c r="E181" s="2"/>
+      <c r="D181" s="2">
+        <v>180</v>
+      </c>
+      <c r="E181" s="2">
+        <v>160</v>
+      </c>
       <c r="F181" s="2"/>
       <c r="G181" s="2"/>
-      <c r="H181" s="2"/>
+      <c r="H181" s="2">
+        <v>182</v>
+      </c>
       <c r="I181" s="2"/>
       <c r="J181" s="2"/>
       <c r="K181" s="2"/>
       <c r="L181" s="2"/>
     </row>
     <row r="182" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A182" s="1"/>
-      <c r="B182" s="1"/>
+      <c r="A182" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="C182" s="3"/>
-      <c r="D182" s="2"/>
-      <c r="E182" s="2"/>
+      <c r="D182" s="2">
+        <v>181</v>
+      </c>
+      <c r="E182" s="2">
+        <v>160</v>
+      </c>
       <c r="F182" s="2"/>
       <c r="G182" s="2"/>
       <c r="H182" s="2"/>
@@ -5339,11 +6143,19 @@
       <c r="L182" s="2"/>
     </row>
     <row r="183" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A183" s="1"/>
-      <c r="B183" s="1"/>
+      <c r="A183" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>295</v>
+      </c>
       <c r="C183" s="3"/>
-      <c r="D183" s="2"/>
-      <c r="E183" s="2"/>
+      <c r="D183" s="2">
+        <v>182</v>
+      </c>
+      <c r="E183" s="2">
+        <v>180</v>
+      </c>
       <c r="F183" s="2"/>
       <c r="G183" s="2"/>
       <c r="H183" s="2"/>
@@ -5353,11 +6165,19 @@
       <c r="L183" s="2"/>
     </row>
     <row r="184" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A184" s="1"/>
-      <c r="B184" s="1"/>
+      <c r="A184" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="C184" s="3"/>
-      <c r="D184" s="2"/>
-      <c r="E184" s="2"/>
+      <c r="D184" s="2">
+        <v>183</v>
+      </c>
+      <c r="E184" s="2">
+        <v>161</v>
+      </c>
       <c r="F184" s="2"/>
       <c r="G184" s="2"/>
       <c r="H184" s="2"/>
@@ -5367,11 +6187,19 @@
       <c r="L184" s="2"/>
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A185" s="1"/>
-      <c r="B185" s="1"/>
+      <c r="A185" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>298</v>
+      </c>
       <c r="C185" s="3"/>
-      <c r="D185" s="2"/>
-      <c r="E185" s="2"/>
+      <c r="D185" s="2">
+        <v>184</v>
+      </c>
+      <c r="E185" s="2">
+        <v>161</v>
+      </c>
       <c r="F185" s="2"/>
       <c r="G185" s="2"/>
       <c r="H185" s="2"/>
@@ -5381,67 +6209,133 @@
       <c r="L185" s="2"/>
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A186" s="1"/>
-      <c r="B186" s="1"/>
+      <c r="A186" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C186" s="3"/>
-      <c r="D186" s="2"/>
-      <c r="E186" s="2"/>
+      <c r="D186" s="2">
+        <v>185</v>
+      </c>
+      <c r="E186" s="2">
+        <v>161</v>
+      </c>
       <c r="F186" s="2"/>
       <c r="G186" s="2"/>
-      <c r="H186" s="2"/>
-      <c r="I186" s="2"/>
+      <c r="H186" s="2">
+        <v>186</v>
+      </c>
+      <c r="I186" s="2">
+        <v>187</v>
+      </c>
       <c r="J186" s="2"/>
       <c r="K186" s="2"/>
       <c r="L186" s="2"/>
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A187" s="1"/>
-      <c r="B187" s="1"/>
-      <c r="C187" s="3"/>
-      <c r="D187" s="2"/>
-      <c r="E187" s="2"/>
+      <c r="A187" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C187" s="3">
+        <v>2013</v>
+      </c>
+      <c r="D187" s="2">
+        <v>186</v>
+      </c>
+      <c r="E187" s="2">
+        <v>185</v>
+      </c>
       <c r="F187" s="2"/>
       <c r="G187" s="2"/>
-      <c r="H187" s="2"/>
-      <c r="I187" s="2"/>
+      <c r="H187" s="2">
+        <v>188</v>
+      </c>
+      <c r="I187" s="2">
+        <v>189</v>
+      </c>
       <c r="J187" s="2"/>
       <c r="K187" s="2"/>
       <c r="L187" s="2"/>
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A188" s="1"/>
-      <c r="B188" s="1"/>
-      <c r="C188" s="3"/>
-      <c r="D188" s="2"/>
-      <c r="E188" s="2"/>
+      <c r="A188" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C188" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D188" s="2">
+        <v>187</v>
+      </c>
+      <c r="E188" s="2">
+        <v>185</v>
+      </c>
       <c r="F188" s="2"/>
       <c r="G188" s="2"/>
-      <c r="H188" s="2"/>
-      <c r="I188" s="2"/>
-      <c r="J188" s="2"/>
+      <c r="H188" s="2">
+        <v>193</v>
+      </c>
+      <c r="I188" s="2">
+        <v>194</v>
+      </c>
+      <c r="J188" s="2">
+        <v>77</v>
+      </c>
       <c r="K188" s="2"/>
       <c r="L188" s="2"/>
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A189" s="1"/>
-      <c r="B189" s="1"/>
-      <c r="C189" s="3"/>
-      <c r="D189" s="2"/>
-      <c r="E189" s="2"/>
+      <c r="A189" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="D189" s="2">
+        <v>188</v>
+      </c>
+      <c r="E189" s="2">
+        <v>186</v>
+      </c>
       <c r="F189" s="2"/>
       <c r="G189" s="2"/>
-      <c r="H189" s="2"/>
-      <c r="I189" s="2"/>
+      <c r="H189" s="2">
+        <v>190</v>
+      </c>
+      <c r="I189" s="2">
+        <v>191</v>
+      </c>
       <c r="J189" s="2"/>
       <c r="K189" s="2"/>
       <c r="L189" s="2"/>
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A190" s="1"/>
-      <c r="B190" s="1"/>
-      <c r="C190" s="3"/>
-      <c r="D190" s="2"/>
-      <c r="E190" s="2"/>
+      <c r="A190" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C190" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D190" s="2">
+        <v>189</v>
+      </c>
+      <c r="E190" s="2">
+        <v>186</v>
+      </c>
       <c r="F190" s="2"/>
       <c r="G190" s="2"/>
       <c r="H190" s="2"/>
@@ -5452,10 +6346,16 @@
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A191" s="1"/>
-      <c r="B191" s="1"/>
+      <c r="B191" s="1" t="s">
+        <v>306</v>
+      </c>
       <c r="C191" s="3"/>
-      <c r="D191" s="2"/>
-      <c r="E191" s="2"/>
+      <c r="D191" s="2">
+        <v>190</v>
+      </c>
+      <c r="E191" s="2">
+        <v>188</v>
+      </c>
       <c r="F191" s="2"/>
       <c r="G191" s="2"/>
       <c r="H191" s="2"/>
@@ -5466,13 +6366,21 @@
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A192" s="1"/>
-      <c r="B192" s="1"/>
+      <c r="B192" s="1" t="s">
+        <v>307</v>
+      </c>
       <c r="C192" s="3"/>
-      <c r="D192" s="2"/>
-      <c r="E192" s="2"/>
+      <c r="D192" s="2">
+        <v>191</v>
+      </c>
+      <c r="E192" s="2">
+        <v>188</v>
+      </c>
       <c r="F192" s="2"/>
       <c r="G192" s="2"/>
-      <c r="H192" s="2"/>
+      <c r="H192" s="2">
+        <v>192</v>
+      </c>
       <c r="I192" s="2"/>
       <c r="J192" s="2"/>
       <c r="K192" s="2"/>
@@ -5480,10 +6388,16 @@
     </row>
     <row r="193" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A193" s="1"/>
-      <c r="B193" s="1"/>
+      <c r="B193" s="1" t="s">
+        <v>308</v>
+      </c>
       <c r="C193" s="3"/>
-      <c r="D193" s="2"/>
-      <c r="E193" s="2"/>
+      <c r="D193" s="2">
+        <v>192</v>
+      </c>
+      <c r="E193" s="2">
+        <v>191</v>
+      </c>
       <c r="F193" s="2"/>
       <c r="G193" s="2"/>
       <c r="H193" s="2"/>
@@ -5493,11 +6407,21 @@
       <c r="L193" s="2"/>
     </row>
     <row r="194" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A194" s="1"/>
-      <c r="B194" s="1"/>
-      <c r="C194" s="3"/>
-      <c r="D194" s="2"/>
-      <c r="E194" s="2"/>
+      <c r="A194" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C194" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D194" s="2">
+        <v>193</v>
+      </c>
+      <c r="E194" s="2">
+        <v>187</v>
+      </c>
       <c r="F194" s="2"/>
       <c r="G194" s="2"/>
       <c r="H194" s="2"/>
@@ -5507,11 +6431,21 @@
       <c r="L194" s="2"/>
     </row>
     <row r="195" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A195" s="1"/>
-      <c r="B195" s="1"/>
-      <c r="C195" s="3"/>
-      <c r="D195" s="2"/>
-      <c r="E195" s="2"/>
+      <c r="A195" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C195" s="3">
+        <v>2022</v>
+      </c>
+      <c r="D195" s="2">
+        <v>194</v>
+      </c>
+      <c r="E195" s="2">
+        <v>187</v>
+      </c>
       <c r="F195" s="2"/>
       <c r="G195" s="2"/>
       <c r="H195" s="2"/>
@@ -5521,25 +6455,47 @@
       <c r="L195" s="2"/>
     </row>
     <row r="196" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A196" s="1"/>
-      <c r="B196" s="1"/>
-      <c r="C196" s="3"/>
-      <c r="D196" s="2"/>
-      <c r="E196" s="2"/>
+      <c r="A196" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C196" s="3">
+        <v>2022</v>
+      </c>
+      <c r="D196" s="2">
+        <v>195</v>
+      </c>
+      <c r="E196" s="2">
+        <v>193</v>
+      </c>
       <c r="F196" s="2"/>
       <c r="G196" s="2"/>
-      <c r="H196" s="2"/>
+      <c r="H196" s="2">
+        <v>196</v>
+      </c>
       <c r="I196" s="2"/>
       <c r="J196" s="2"/>
       <c r="K196" s="2"/>
       <c r="L196" s="2"/>
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A197" s="1"/>
-      <c r="B197" s="1"/>
-      <c r="C197" s="3"/>
-      <c r="D197" s="2"/>
-      <c r="E197" s="2"/>
+      <c r="A197" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C197" s="3">
+        <v>2024</v>
+      </c>
+      <c r="D197" s="2">
+        <v>196</v>
+      </c>
+      <c r="E197" s="2">
+        <v>195</v>
+      </c>
       <c r="F197" s="2"/>
       <c r="G197" s="2"/>
       <c r="H197" s="2"/>
@@ -5552,7 +6508,9 @@
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="3"/>
-      <c r="D198" s="2"/>
+      <c r="D198" s="2">
+        <v>197</v>
+      </c>
       <c r="E198" s="2"/>
       <c r="F198" s="2"/>
       <c r="G198" s="2"/>
@@ -5566,7 +6524,9 @@
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="3"/>
-      <c r="D199" s="2"/>
+      <c r="D199" s="2">
+        <v>198</v>
+      </c>
       <c r="E199" s="2"/>
       <c r="F199" s="2"/>
       <c r="G199" s="2"/>
@@ -5580,7 +6540,9 @@
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="3"/>
-      <c r="D200" s="2"/>
+      <c r="D200" s="2">
+        <v>199</v>
+      </c>
       <c r="E200" s="2"/>
       <c r="F200" s="2"/>
       <c r="G200" s="2"/>
@@ -5594,7 +6556,9 @@
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="3"/>
-      <c r="D201" s="2"/>
+      <c r="D201" s="2">
+        <v>200</v>
+      </c>
       <c r="E201" s="2"/>
       <c r="F201" s="2"/>
       <c r="G201" s="2"/>
@@ -5608,7 +6572,9 @@
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="3"/>
-      <c r="D202" s="2"/>
+      <c r="D202" s="2">
+        <v>201</v>
+      </c>
       <c r="E202" s="2"/>
       <c r="F202" s="2"/>
       <c r="G202" s="2"/>
@@ -5622,7 +6588,9 @@
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="3"/>
-      <c r="D203" s="2"/>
+      <c r="D203" s="2">
+        <v>202</v>
+      </c>
       <c r="E203" s="2"/>
       <c r="F203" s="2"/>
       <c r="G203" s="2"/>
@@ -5636,7 +6604,9 @@
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="3"/>
-      <c r="D204" s="2"/>
+      <c r="D204" s="2">
+        <v>203</v>
+      </c>
       <c r="E204" s="2"/>
       <c r="F204" s="2"/>
       <c r="G204" s="2"/>
@@ -5650,7 +6620,9 @@
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="3"/>
-      <c r="D205" s="2"/>
+      <c r="D205" s="2">
+        <v>204</v>
+      </c>
       <c r="E205" s="2"/>
       <c r="F205" s="2"/>
       <c r="G205" s="2"/>
@@ -5664,7 +6636,9 @@
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="3"/>
-      <c r="D206" s="2"/>
+      <c r="D206" s="2">
+        <v>205</v>
+      </c>
       <c r="E206" s="2"/>
       <c r="F206" s="2"/>
       <c r="G206" s="2"/>
@@ -5678,7 +6652,9 @@
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="3"/>
-      <c r="D207" s="2"/>
+      <c r="D207" s="2">
+        <v>206</v>
+      </c>
       <c r="E207" s="2"/>
       <c r="F207" s="2"/>
       <c r="G207" s="2"/>
@@ -5692,7 +6668,9 @@
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="3"/>
-      <c r="D208" s="2"/>
+      <c r="D208" s="2">
+        <v>207</v>
+      </c>
       <c r="E208" s="2"/>
       <c r="F208" s="2"/>
       <c r="G208" s="2"/>
@@ -5706,7 +6684,9 @@
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="3"/>
-      <c r="D209" s="2"/>
+      <c r="D209" s="2">
+        <v>208</v>
+      </c>
       <c r="E209" s="2"/>
       <c r="F209" s="2"/>
       <c r="G209" s="2"/>
@@ -5720,7 +6700,9 @@
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="3"/>
-      <c r="D210" s="2"/>
+      <c r="D210" s="2">
+        <v>209</v>
+      </c>
       <c r="E210" s="2"/>
       <c r="F210" s="2"/>
       <c r="G210" s="2"/>
@@ -5734,7 +6716,9 @@
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
       <c r="C211" s="3"/>
-      <c r="D211" s="2"/>
+      <c r="D211" s="2">
+        <v>210</v>
+      </c>
       <c r="E211" s="2"/>
       <c r="F211" s="2"/>
       <c r="G211" s="2"/>
@@ -5748,7 +6732,9 @@
       <c r="A212" s="1"/>
       <c r="B212" s="1"/>
       <c r="C212" s="3"/>
-      <c r="D212" s="2"/>
+      <c r="D212" s="2">
+        <v>211</v>
+      </c>
       <c r="E212" s="2"/>
       <c r="F212" s="2"/>
       <c r="G212" s="2"/>
@@ -5762,7 +6748,9 @@
       <c r="A213" s="1"/>
       <c r="B213" s="1"/>
       <c r="C213" s="3"/>
-      <c r="D213" s="2"/>
+      <c r="D213" s="2">
+        <v>212</v>
+      </c>
       <c r="E213" s="2"/>
       <c r="F213" s="2"/>
       <c r="G213" s="2"/>
@@ -5776,7 +6764,9 @@
       <c r="A214" s="1"/>
       <c r="B214" s="1"/>
       <c r="C214" s="3"/>
-      <c r="D214" s="2"/>
+      <c r="D214" s="2">
+        <v>213</v>
+      </c>
       <c r="E214" s="2"/>
       <c r="F214" s="2"/>
       <c r="G214" s="2"/>
@@ -5790,7 +6780,9 @@
       <c r="A215" s="1"/>
       <c r="B215" s="1"/>
       <c r="C215" s="3"/>
-      <c r="D215" s="2"/>
+      <c r="D215" s="2">
+        <v>214</v>
+      </c>
       <c r="E215" s="2"/>
       <c r="F215" s="2"/>
       <c r="G215" s="2"/>
@@ -5804,7 +6796,9 @@
       <c r="A216" s="1"/>
       <c r="B216" s="1"/>
       <c r="C216" s="3"/>
-      <c r="D216" s="2"/>
+      <c r="D216" s="2">
+        <v>215</v>
+      </c>
       <c r="E216" s="2"/>
       <c r="F216" s="2"/>
       <c r="G216" s="2"/>
@@ -5818,7 +6812,9 @@
       <c r="A217" s="1"/>
       <c r="B217" s="1"/>
       <c r="C217" s="3"/>
-      <c r="D217" s="2"/>
+      <c r="D217" s="2">
+        <v>216</v>
+      </c>
       <c r="E217" s="2"/>
       <c r="F217" s="2"/>
       <c r="G217" s="2"/>
@@ -5832,7 +6828,9 @@
       <c r="A218" s="1"/>
       <c r="B218" s="1"/>
       <c r="C218" s="3"/>
-      <c r="D218" s="2"/>
+      <c r="D218" s="2">
+        <v>217</v>
+      </c>
       <c r="E218" s="2"/>
       <c r="F218" s="2"/>
       <c r="G218" s="2"/>
@@ -5846,7 +6844,9 @@
       <c r="A219" s="1"/>
       <c r="B219" s="1"/>
       <c r="C219" s="3"/>
-      <c r="D219" s="2"/>
+      <c r="D219" s="2">
+        <v>218</v>
+      </c>
       <c r="E219" s="2"/>
       <c r="F219" s="2"/>
       <c r="G219" s="2"/>
@@ -5860,7 +6860,9 @@
       <c r="A220" s="1"/>
       <c r="B220" s="1"/>
       <c r="C220" s="3"/>
-      <c r="D220" s="2"/>
+      <c r="D220" s="2">
+        <v>219</v>
+      </c>
       <c r="E220" s="2"/>
       <c r="F220" s="2"/>
       <c r="G220" s="2"/>
@@ -5874,7 +6876,9 @@
       <c r="A221" s="1"/>
       <c r="B221" s="1"/>
       <c r="C221" s="3"/>
-      <c r="D221" s="2"/>
+      <c r="D221" s="2">
+        <v>220</v>
+      </c>
       <c r="E221" s="2"/>
       <c r="F221" s="2"/>
       <c r="G221" s="2"/>
@@ -5888,7 +6892,9 @@
       <c r="A222" s="1"/>
       <c r="B222" s="1"/>
       <c r="C222" s="3"/>
-      <c r="D222" s="2"/>
+      <c r="D222" s="2">
+        <v>221</v>
+      </c>
       <c r="E222" s="2"/>
       <c r="F222" s="2"/>
       <c r="G222" s="2"/>
@@ -5902,7 +6908,9 @@
       <c r="A223" s="1"/>
       <c r="B223" s="1"/>
       <c r="C223" s="3"/>
-      <c r="D223" s="2"/>
+      <c r="D223" s="2">
+        <v>222</v>
+      </c>
       <c r="E223" s="2"/>
       <c r="F223" s="2"/>
       <c r="G223" s="2"/>
@@ -5916,7 +6924,9 @@
       <c r="A224" s="1"/>
       <c r="B224" s="1"/>
       <c r="C224" s="3"/>
-      <c r="D224" s="2"/>
+      <c r="D224" s="2">
+        <v>223</v>
+      </c>
       <c r="E224" s="2"/>
       <c r="F224" s="2"/>
       <c r="G224" s="2"/>
@@ -5930,7 +6940,9 @@
       <c r="A225" s="1"/>
       <c r="B225" s="1"/>
       <c r="C225" s="3"/>
-      <c r="D225" s="2"/>
+      <c r="D225" s="2">
+        <v>224</v>
+      </c>
       <c r="E225" s="2"/>
       <c r="F225" s="2"/>
       <c r="G225" s="2"/>
@@ -5944,7 +6956,9 @@
       <c r="A226" s="1"/>
       <c r="B226" s="1"/>
       <c r="C226" s="3"/>
-      <c r="D226" s="2"/>
+      <c r="D226" s="2">
+        <v>225</v>
+      </c>
       <c r="E226" s="2"/>
       <c r="F226" s="2"/>
       <c r="G226" s="2"/>
@@ -5958,7 +6972,9 @@
       <c r="A227" s="1"/>
       <c r="B227" s="1"/>
       <c r="C227" s="3"/>
-      <c r="D227" s="2"/>
+      <c r="D227" s="2">
+        <v>226</v>
+      </c>
       <c r="E227" s="2"/>
       <c r="F227" s="2"/>
       <c r="G227" s="2"/>
@@ -5972,7 +6988,9 @@
       <c r="A228" s="1"/>
       <c r="B228" s="1"/>
       <c r="C228" s="3"/>
-      <c r="D228" s="2"/>
+      <c r="D228" s="2">
+        <v>227</v>
+      </c>
       <c r="E228" s="2"/>
       <c r="F228" s="2"/>
       <c r="G228" s="2"/>
@@ -5986,7 +7004,9 @@
       <c r="A229" s="1"/>
       <c r="B229" s="1"/>
       <c r="C229" s="3"/>
-      <c r="D229" s="2"/>
+      <c r="D229" s="2">
+        <v>228</v>
+      </c>
       <c r="E229" s="2"/>
       <c r="F229" s="2"/>
       <c r="G229" s="2"/>
@@ -6000,7 +7020,9 @@
       <c r="A230" s="1"/>
       <c r="B230" s="1"/>
       <c r="C230" s="3"/>
-      <c r="D230" s="2"/>
+      <c r="D230" s="2">
+        <v>229</v>
+      </c>
       <c r="E230" s="2"/>
       <c r="F230" s="2"/>
       <c r="G230" s="2"/>
@@ -6014,7 +7036,9 @@
       <c r="A231" s="1"/>
       <c r="B231" s="1"/>
       <c r="C231" s="3"/>
-      <c r="D231" s="2"/>
+      <c r="D231" s="2">
+        <v>230</v>
+      </c>
       <c r="E231" s="2"/>
       <c r="F231" s="2"/>
       <c r="G231" s="2"/>
@@ -6028,7 +7052,9 @@
       <c r="A232" s="1"/>
       <c r="B232" s="1"/>
       <c r="C232" s="3"/>
-      <c r="D232" s="2"/>
+      <c r="D232" s="2">
+        <v>231</v>
+      </c>
       <c r="E232" s="2"/>
       <c r="F232" s="2"/>
       <c r="G232" s="2"/>
@@ -6042,7 +7068,9 @@
       <c r="A233" s="1"/>
       <c r="B233" s="1"/>
       <c r="C233" s="3"/>
-      <c r="D233" s="2"/>
+      <c r="D233" s="2">
+        <v>232</v>
+      </c>
       <c r="E233" s="2"/>
       <c r="F233" s="2"/>
       <c r="G233" s="2"/>
@@ -6056,7 +7084,9 @@
       <c r="A234" s="1"/>
       <c r="B234" s="1"/>
       <c r="C234" s="3"/>
-      <c r="D234" s="2"/>
+      <c r="D234" s="2">
+        <v>233</v>
+      </c>
       <c r="E234" s="2"/>
       <c r="F234" s="2"/>
       <c r="G234" s="2"/>
@@ -6070,7 +7100,9 @@
       <c r="A235" s="1"/>
       <c r="B235" s="1"/>
       <c r="C235" s="3"/>
-      <c r="D235" s="2"/>
+      <c r="D235" s="2">
+        <v>234</v>
+      </c>
       <c r="E235" s="2"/>
       <c r="F235" s="2"/>
       <c r="G235" s="2"/>
@@ -6084,7 +7116,9 @@
       <c r="A236" s="1"/>
       <c r="B236" s="1"/>
       <c r="C236" s="3"/>
-      <c r="D236" s="2"/>
+      <c r="D236" s="2">
+        <v>235</v>
+      </c>
       <c r="E236" s="2"/>
       <c r="F236" s="2"/>
       <c r="G236" s="2"/>
@@ -6098,7 +7132,9 @@
       <c r="A237" s="1"/>
       <c r="B237" s="1"/>
       <c r="C237" s="3"/>
-      <c r="D237" s="2"/>
+      <c r="D237" s="2">
+        <v>236</v>
+      </c>
       <c r="E237" s="2"/>
       <c r="F237" s="2"/>
       <c r="G237" s="2"/>
@@ -6112,7 +7148,9 @@
       <c r="A238" s="1"/>
       <c r="B238" s="1"/>
       <c r="C238" s="3"/>
-      <c r="D238" s="2"/>
+      <c r="D238" s="2">
+        <v>237</v>
+      </c>
       <c r="E238" s="2"/>
       <c r="F238" s="2"/>
       <c r="G238" s="2"/>
@@ -6126,7 +7164,9 @@
       <c r="A239" s="1"/>
       <c r="B239" s="1"/>
       <c r="C239" s="3"/>
-      <c r="D239" s="2"/>
+      <c r="D239" s="2">
+        <v>238</v>
+      </c>
       <c r="E239" s="2"/>
       <c r="F239" s="2"/>
       <c r="G239" s="2"/>
@@ -6140,7 +7180,9 @@
       <c r="A240" s="1"/>
       <c r="B240" s="1"/>
       <c r="C240" s="3"/>
-      <c r="D240" s="2"/>
+      <c r="D240" s="2">
+        <v>239</v>
+      </c>
       <c r="E240" s="2"/>
       <c r="F240" s="2"/>
       <c r="G240" s="2"/>
@@ -6154,7 +7196,9 @@
       <c r="A241" s="1"/>
       <c r="B241" s="1"/>
       <c r="C241" s="3"/>
-      <c r="D241" s="2"/>
+      <c r="D241" s="2">
+        <v>240</v>
+      </c>
       <c r="E241" s="2"/>
       <c r="F241" s="2"/>
       <c r="G241" s="2"/>
@@ -6168,7 +7212,9 @@
       <c r="A242" s="1"/>
       <c r="B242" s="1"/>
       <c r="C242" s="3"/>
-      <c r="D242" s="2"/>
+      <c r="D242" s="2">
+        <v>241</v>
+      </c>
       <c r="E242" s="2"/>
       <c r="F242" s="2"/>
       <c r="G242" s="2"/>
@@ -6182,7 +7228,9 @@
       <c r="A243" s="1"/>
       <c r="B243" s="1"/>
       <c r="C243" s="3"/>
-      <c r="D243" s="2"/>
+      <c r="D243" s="2">
+        <v>242</v>
+      </c>
       <c r="E243" s="2"/>
       <c r="F243" s="2"/>
       <c r="G243" s="2"/>
@@ -6196,7 +7244,9 @@
       <c r="A244" s="1"/>
       <c r="B244" s="1"/>
       <c r="C244" s="3"/>
-      <c r="D244" s="2"/>
+      <c r="D244" s="2">
+        <v>243</v>
+      </c>
       <c r="E244" s="2"/>
       <c r="F244" s="2"/>
       <c r="G244" s="2"/>
@@ -6210,7 +7260,9 @@
       <c r="A245" s="1"/>
       <c r="B245" s="1"/>
       <c r="C245" s="3"/>
-      <c r="D245" s="2"/>
+      <c r="D245" s="2">
+        <v>244</v>
+      </c>
       <c r="E245" s="2"/>
       <c r="F245" s="2"/>
       <c r="G245" s="2"/>
@@ -6224,7 +7276,9 @@
       <c r="A246" s="1"/>
       <c r="B246" s="1"/>
       <c r="C246" s="3"/>
-      <c r="D246" s="2"/>
+      <c r="D246" s="2">
+        <v>245</v>
+      </c>
       <c r="E246" s="2"/>
       <c r="F246" s="2"/>
       <c r="G246" s="2"/>
@@ -6238,7 +7292,9 @@
       <c r="A247" s="1"/>
       <c r="B247" s="1"/>
       <c r="C247" s="3"/>
-      <c r="D247" s="2"/>
+      <c r="D247" s="2">
+        <v>246</v>
+      </c>
       <c r="E247" s="2"/>
       <c r="F247" s="2"/>
       <c r="G247" s="2"/>
@@ -6252,7 +7308,9 @@
       <c r="A248" s="1"/>
       <c r="B248" s="1"/>
       <c r="C248" s="3"/>
-      <c r="D248" s="2"/>
+      <c r="D248" s="2">
+        <v>247</v>
+      </c>
       <c r="E248" s="2"/>
       <c r="F248" s="2"/>
       <c r="G248" s="2"/>
@@ -6266,7 +7324,9 @@
       <c r="A249" s="1"/>
       <c r="B249" s="1"/>
       <c r="C249" s="3"/>
-      <c r="D249" s="2"/>
+      <c r="D249" s="2">
+        <v>248</v>
+      </c>
       <c r="E249" s="2"/>
       <c r="F249" s="2"/>
       <c r="G249" s="2"/>
@@ -6280,7 +7340,9 @@
       <c r="A250" s="1"/>
       <c r="B250" s="1"/>
       <c r="C250" s="3"/>
-      <c r="D250" s="2"/>
+      <c r="D250" s="2">
+        <v>249</v>
+      </c>
       <c r="E250" s="2"/>
       <c r="F250" s="2"/>
       <c r="G250" s="2"/>
@@ -6294,7 +7356,9 @@
       <c r="A251" s="1"/>
       <c r="B251" s="1"/>
       <c r="C251" s="3"/>
-      <c r="D251" s="2"/>
+      <c r="D251" s="2">
+        <v>250</v>
+      </c>
       <c r="E251" s="2"/>
       <c r="F251" s="2"/>
       <c r="G251" s="2"/>

</xml_diff>

<commit_message>
Fixed missing first names
</commit_message>
<xml_diff>
--- a/family-tree-data.xlsx
+++ b/family-tree-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASHil\PycharmProjects\Family-Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BD8D02-94A4-475E-A018-3286E16C635E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C054E6-2E9F-4CB8-A239-3E9D70E5EE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="314">
   <si>
     <t>Class Year</t>
   </si>
@@ -1483,7 +1483,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I190" sqref="I190"/>
+      <selection pane="bottomLeft" activeCell="D190" sqref="D190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6342,7 +6342,9 @@
       <c r="L190" s="2"/>
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A191" s="1"/>
+      <c r="A191" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="B191" s="1" t="s">
         <v>303</v>
       </c>
@@ -6362,7 +6364,9 @@
       <c r="L191" s="2"/>
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A192" s="1"/>
+      <c r="A192" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="B192" s="1" t="s">
         <v>304</v>
       </c>
@@ -6384,7 +6388,9 @@
       <c r="L192" s="2"/>
     </row>
     <row r="193" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A193" s="1"/>
+      <c r="A193" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="B193" s="1" t="s">
         <v>305</v>
       </c>

</xml_diff>

<commit_message>
Added Ozuna as parent of Ho
</commit_message>
<xml_diff>
--- a/family-tree-data.xlsx
+++ b/family-tree-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASHil\PycharmProjects\Family-Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C054E6-2E9F-4CB8-A239-3E9D70E5EE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7B88B7-0282-4F19-8CF5-962ADF536DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="316">
   <si>
     <t>Class Year</t>
   </si>
@@ -380,9 +380,6 @@
     <t>Drew</t>
   </si>
   <si>
-    <t>Ontati</t>
-  </si>
-  <si>
     <t>Evan</t>
   </si>
   <si>
@@ -978,6 +975,15 @@
   </si>
   <si>
     <t>Parker</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>Ozuna</t>
+  </si>
+  <si>
+    <t>Ontai</t>
   </si>
 </sst>
 </file>
@@ -1482,8 +1488,8 @@
   <dimension ref="A1:L350"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D190" sqref="D190"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1733,7 +1739,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>28</v>
@@ -1819,7 +1825,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>33</v>
@@ -1843,13 +1849,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D14" s="2">
         <v>13</v>
@@ -2029,7 +2035,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>44</v>
@@ -2151,7 +2157,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>53</v>
@@ -2235,9 +2241,11 @@
         <v>28</v>
       </c>
       <c r="E29" s="2">
+        <v>197</v>
+      </c>
+      <c r="F29" s="2">
         <v>24</v>
       </c>
-      <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2">
         <v>30</v>
@@ -2297,7 +2305,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>63</v>
@@ -2481,7 +2489,7 @@
         <v>77</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D39" s="2">
         <v>38</v>
@@ -2978,7 +2986,7 @@
         <v>111</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C58" s="3">
         <v>2026</v>
@@ -3050,7 +3058,7 @@
         <v>103</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C61" s="3">
         <v>2020</v>
@@ -3078,9 +3086,11 @@
         <v>38</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C62" s="3"/>
+        <v>315</v>
+      </c>
+      <c r="C62" s="3">
+        <v>2020</v>
+      </c>
       <c r="D62" s="2">
         <v>61</v>
       </c>
@@ -3097,10 +3107,10 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="C63" s="3">
         <v>2023</v>
@@ -3126,7 +3136,7 @@
         <v>47</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C64" s="3">
         <v>2024</v>
@@ -3147,10 +3157,10 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="2">
@@ -3167,10 +3177,10 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C66" s="3">
         <v>2016</v>
@@ -3195,10 +3205,10 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="C67" s="3">
         <v>2018</v>
@@ -3221,10 +3231,10 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="2">
@@ -3243,10 +3253,10 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="C69" s="3">
         <v>2019</v>
@@ -3273,10 +3283,10 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C70" s="3">
         <v>2022</v>
@@ -3297,10 +3307,10 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="2">
@@ -3317,10 +3327,10 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="C72" s="3">
         <v>2022</v>
@@ -3343,10 +3353,10 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="C73" s="3">
         <v>2022</v>
@@ -3368,7 +3378,7 @@
         <v>95</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C74" s="3">
         <v>2025</v>
@@ -3391,10 +3401,10 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="C75" s="3">
         <v>2025</v>
@@ -3418,7 +3428,7 @@
         <v>26</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C76" s="3">
         <v>2019</v>
@@ -3442,7 +3452,7 @@
         <v>89</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C77" s="3">
         <v>2019</v>
@@ -3466,7 +3476,7 @@
         <v>26</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C78" s="3">
         <v>2023</v>
@@ -3489,10 +3499,10 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="C79" s="3">
         <v>2025</v>
@@ -3513,10 +3523,10 @@
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="2">
@@ -3535,10 +3545,10 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="C81" s="3">
         <v>2017</v>
@@ -3563,10 +3573,10 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C82" s="3">
         <v>2018</v>
@@ -3589,7 +3599,7 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>47</v>
@@ -3622,7 +3632,7 @@
         <v>51</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C84" s="3">
         <v>2020</v>
@@ -3643,10 +3653,10 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="C85" s="3">
         <v>2022</v>
@@ -3671,10 +3681,10 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="C86" s="3">
         <v>2023</v>
@@ -3697,10 +3707,10 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="C87" s="3">
         <v>2023</v>
@@ -3729,10 +3739,10 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="C88" s="3">
         <v>2025</v>
@@ -3756,7 +3766,7 @@
         <v>80</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C89" s="3">
         <v>2025</v>
@@ -3779,10 +3789,10 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="C90" s="3">
         <v>2024</v>
@@ -3803,10 +3813,10 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="C91" s="3">
         <v>2021</v>
@@ -3827,10 +3837,10 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="C92" s="3">
         <v>2022</v>
@@ -3855,10 +3865,10 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C93" s="3">
         <v>2025</v>
@@ -3879,10 +3889,10 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="C94" s="3">
         <v>2026</v>
@@ -3906,7 +3916,7 @@
         <v>35</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C95" s="3">
         <v>2017</v>
@@ -3927,10 +3937,10 @@
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="C96" s="3">
         <v>2026</v>
@@ -3951,10 +3961,10 @@
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C97" s="3">
         <v>2026</v>
@@ -3975,10 +3985,10 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="C98" s="3">
         <v>2026</v>
@@ -4023,7 +4033,7 @@
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>21</v>
@@ -4047,7 +4057,7 @@
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>30</v>
@@ -4071,10 +4081,10 @@
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="C102" s="3">
         <v>2026</v>
@@ -4095,10 +4105,10 @@
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C103" s="3">
         <v>2023</v>
@@ -4123,10 +4133,10 @@
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="C104" s="3">
         <v>2023</v>
@@ -4151,10 +4161,10 @@
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C105" s="3">
         <v>2023</v>
@@ -4177,10 +4187,10 @@
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="C106" s="3">
         <v>2023</v>
@@ -4210,7 +4220,7 @@
         <v>113</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C107" s="3">
         <v>2022</v>
@@ -4237,10 +4247,10 @@
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C108" s="3">
         <v>2024</v>
@@ -4261,10 +4271,10 @@
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C109" s="3">
         <v>2026</v>
@@ -4287,10 +4297,10 @@
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="C110" s="3">
         <v>2025</v>
@@ -4311,10 +4321,10 @@
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="C111" s="3">
         <v>2025</v>
@@ -4335,10 +4345,10 @@
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="C112" s="3">
         <v>2019</v>
@@ -4357,10 +4367,10 @@
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C113" s="3">
         <v>2019</v>
@@ -4381,10 +4391,10 @@
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="C114" s="3"/>
       <c r="D114" s="2">
@@ -4406,7 +4416,7 @@
         <v>15</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C115" s="3">
         <v>2020</v>
@@ -4434,7 +4444,7 @@
         <v>15</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C116" s="3">
         <v>2021</v>
@@ -4457,10 +4467,10 @@
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C117" s="3">
         <v>2022</v>
@@ -4483,10 +4493,10 @@
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B118" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="C118" s="3">
         <v>2025</v>
@@ -4507,10 +4517,10 @@
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C119" s="3"/>
       <c r="D119" s="2">
@@ -4531,10 +4541,10 @@
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C120" s="3"/>
       <c r="D120" s="2">
@@ -4556,7 +4566,7 @@
         <v>16</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C121" s="3">
         <v>2016</v>
@@ -4581,10 +4591,10 @@
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C122" s="3"/>
       <c r="D122" s="2">
@@ -4603,10 +4613,10 @@
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B123" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="C123" s="3"/>
       <c r="D123" s="2">
@@ -4627,10 +4637,10 @@
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B124" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="C124" s="3">
         <v>2019</v>
@@ -4653,10 +4663,10 @@
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B125" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="C125" s="3">
         <v>2022</v>
@@ -4684,7 +4694,7 @@
         <v>16</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C126" s="3">
         <v>2025</v>
@@ -4705,10 +4715,10 @@
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B127" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="C127" s="3">
         <v>2015</v>
@@ -4737,10 +4747,10 @@
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B128" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="C128" s="3">
         <v>2018</v>
@@ -4761,10 +4771,10 @@
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C129" s="3">
         <v>2019</v>
@@ -4790,7 +4800,7 @@
         <v>47</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C130" s="3">
         <v>2016</v>
@@ -4816,7 +4826,7 @@
         <v>35</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C131" s="3">
         <v>2017</v>
@@ -4841,10 +4851,10 @@
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C132" s="3">
         <v>2017</v>
@@ -4870,7 +4880,7 @@
         <v>45</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C133" s="3">
         <v>2021</v>
@@ -4891,10 +4901,10 @@
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C134" s="3">
         <v>2021</v>
@@ -4952,7 +4962,7 @@
         <v>49</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C136" s="3">
         <v>2023</v>
@@ -4973,10 +4983,10 @@
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B137" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="C137" s="3">
         <v>2022</v>
@@ -5004,7 +5014,7 @@
         <v>80</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C138" s="3">
         <v>2022</v>
@@ -5032,7 +5042,7 @@
         <v>64</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C139" s="3">
         <v>2020</v>
@@ -5056,7 +5066,7 @@
         <v>25</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C140" s="3">
         <v>2025</v>
@@ -5077,10 +5087,10 @@
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="C141" s="3">
         <v>2025</v>
@@ -5101,10 +5111,10 @@
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B142" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="C142" s="3">
         <v>2023</v>
@@ -5127,10 +5137,10 @@
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B143" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="C143" s="3">
         <v>2023</v>
@@ -5151,10 +5161,10 @@
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C144" s="3">
         <v>2024</v>
@@ -5175,10 +5185,10 @@
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B145" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="C145" s="3">
         <v>2022</v>
@@ -5199,10 +5209,10 @@
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C146" s="3">
         <v>2020</v>
@@ -5227,10 +5237,10 @@
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B147" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="C147" s="3">
         <v>2021</v>
@@ -5251,10 +5261,10 @@
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C148" s="3">
         <v>2024</v>
@@ -5275,10 +5285,10 @@
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B149" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="C149" s="3">
         <v>1999</v>
@@ -5299,10 +5309,10 @@
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C150" s="3">
         <v>2001</v>
@@ -5325,10 +5335,10 @@
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B151" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="C151" s="3">
         <v>2005</v>
@@ -5355,10 +5365,10 @@
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C152" s="3">
         <v>2006</v>
@@ -5385,10 +5395,10 @@
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="C153" s="3">
         <v>2007</v>
@@ -5409,10 +5419,10 @@
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B154" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="C154" s="3"/>
       <c r="D154" s="2">
@@ -5431,10 +5441,10 @@
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B155" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>251</v>
       </c>
       <c r="C155" s="3">
         <v>2006</v>
@@ -5455,10 +5465,10 @@
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B156" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="C156" s="3">
         <v>2008</v>
@@ -5479,10 +5489,10 @@
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B157" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>255</v>
       </c>
       <c r="C157" s="3">
         <v>2009</v>
@@ -5513,10 +5523,10 @@
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C158" s="3">
         <v>2013</v>
@@ -5543,10 +5553,10 @@
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C159" s="3">
         <v>2010</v>
@@ -5567,10 +5577,10 @@
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C160" s="3">
         <v>2010</v>
@@ -5591,10 +5601,10 @@
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B161" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>260</v>
       </c>
       <c r="C161" s="3">
         <v>2011</v>
@@ -5619,10 +5629,10 @@
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C162" s="3">
         <v>2012</v>
@@ -5649,10 +5659,10 @@
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B163" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>263</v>
       </c>
       <c r="C163" s="3">
         <v>2016</v>
@@ -5675,10 +5685,10 @@
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C164" s="3">
         <v>2017</v>
@@ -5699,10 +5709,10 @@
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B165" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>267</v>
       </c>
       <c r="C165" s="3">
         <v>2017</v>
@@ -5723,10 +5733,10 @@
     </row>
     <row r="166" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B166" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="C166" s="3">
         <v>2013</v>
@@ -5747,10 +5757,10 @@
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C167" s="3">
         <v>2016</v>
@@ -5774,7 +5784,7 @@
         <v>38</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C168" s="3">
         <v>2018</v>
@@ -5797,10 +5807,10 @@
     </row>
     <row r="169" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B169" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>272</v>
       </c>
       <c r="C169" s="3">
         <v>2019</v>
@@ -5821,10 +5831,10 @@
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B170" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>274</v>
       </c>
       <c r="C170" s="3">
         <v>2019</v>
@@ -5847,10 +5857,10 @@
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B171" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>276</v>
       </c>
       <c r="C171" s="3">
         <v>2012</v>
@@ -5871,10 +5881,10 @@
     </row>
     <row r="172" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C172" s="3"/>
       <c r="D172" s="2">
@@ -5893,10 +5903,10 @@
     </row>
     <row r="173" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C173" s="3">
         <v>2021</v>
@@ -5923,7 +5933,7 @@
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>69</v>
@@ -5947,10 +5957,10 @@
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B175" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>281</v>
       </c>
       <c r="C175" s="3">
         <v>2022</v>
@@ -5975,10 +5985,10 @@
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B176" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>283</v>
       </c>
       <c r="C176" s="3">
         <v>2023</v>
@@ -5999,10 +6009,10 @@
     </row>
     <row r="177" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B177" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>285</v>
       </c>
       <c r="C177" s="3">
         <v>2024</v>
@@ -6025,10 +6035,10 @@
     </row>
     <row r="178" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B178" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="C178" s="3">
         <v>2025</v>
@@ -6049,10 +6059,10 @@
     </row>
     <row r="179" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B179" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="C179" s="3">
         <v>2025</v>
@@ -6073,10 +6083,10 @@
     </row>
     <row r="180" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C180" s="3"/>
       <c r="D180" s="2">
@@ -6098,7 +6108,7 @@
         <v>47</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C181" s="3"/>
       <c r="D181" s="2">
@@ -6119,10 +6129,10 @@
     </row>
     <row r="182" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C182" s="3"/>
       <c r="D182" s="2">
@@ -6141,10 +6151,10 @@
     </row>
     <row r="183" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C183" s="3"/>
       <c r="D183" s="2">
@@ -6163,10 +6173,10 @@
     </row>
     <row r="184" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C184" s="3"/>
       <c r="D184" s="2">
@@ -6185,10 +6195,10 @@
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B185" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="B185" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="C185" s="3"/>
       <c r="D185" s="2">
@@ -6236,7 +6246,7 @@
         <v>12</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C187" s="3">
         <v>2013</v>
@@ -6264,7 +6274,7 @@
         <v>75</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C188" s="3">
         <v>2018</v>
@@ -6291,13 +6301,13 @@
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C189" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="B189" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="C189" s="3" t="s">
-        <v>300</v>
       </c>
       <c r="D189" s="2">
         <v>188</v>
@@ -6319,10 +6329,10 @@
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B190" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="B190" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="C190" s="3">
         <v>2019</v>
@@ -6343,10 +6353,10 @@
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C191" s="3"/>
       <c r="D191" s="2">
@@ -6365,10 +6375,10 @@
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C192" s="3"/>
       <c r="D192" s="2">
@@ -6389,10 +6399,10 @@
     </row>
     <row r="193" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C193" s="3"/>
       <c r="D193" s="2">
@@ -6411,10 +6421,10 @@
     </row>
     <row r="194" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B194" s="1" t="s">
         <v>306</v>
-      </c>
-      <c r="B194" s="1" t="s">
-        <v>307</v>
       </c>
       <c r="C194" s="3">
         <v>2019</v>
@@ -6439,10 +6449,10 @@
     </row>
     <row r="195" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B195" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="B195" s="1" t="s">
-        <v>309</v>
       </c>
       <c r="C195" s="3">
         <v>2022</v>
@@ -6463,10 +6473,10 @@
     </row>
     <row r="196" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B196" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="B196" s="1" t="s">
-        <v>311</v>
       </c>
       <c r="C196" s="3">
         <v>2022</v>
@@ -6492,7 +6502,7 @@
         <v>51</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C197" s="3">
         <v>2024</v>
@@ -6512,16 +6522,24 @@
       <c r="L197" s="2"/>
     </row>
     <row r="198" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A198" s="1"/>
-      <c r="B198" s="1"/>
-      <c r="C198" s="3"/>
+      <c r="A198" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C198" s="3">
+        <v>2020</v>
+      </c>
       <c r="D198" s="2">
         <v>197</v>
       </c>
       <c r="E198" s="2"/>
       <c r="F198" s="2"/>
       <c r="G198" s="2"/>
-      <c r="H198" s="2"/>
+      <c r="H198" s="2">
+        <v>28</v>
+      </c>
       <c r="I198" s="2"/>
       <c r="J198" s="2"/>
       <c r="K198" s="2"/>

</xml_diff>